<commit_message>
trying to add workflow
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -457,8 +457,8 @@
     <col min="2" max="2" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="10" width="19.290714285714284" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="10" width="22.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="26.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="22.14785714285714" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
updated script to dynamically update markdown
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -14,18 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Dataset Name</t>
   </si>
   <si>
+    <t>Link</t>
+  </si>
+  <si>
     <t>Year</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Link</t>
+    <t>Author</t>
   </si>
   <si>
     <t>Documentation</t>
@@ -37,109 +40,22 @@
     <t>Crop Analyses: AI for Telangana Agriculture</t>
   </si>
   <si>
+    <t>https://dataexplorer.ts.adex.org.in/dataset/1da21f2b-87f6-4641-81bd-ed6bcd461303</t>
+  </si>
+  <si>
     <t xml:space="preserve">2022–2024 </t>
   </si>
   <si>
     <t>AI-based crop type map and replication kit</t>
   </si>
   <si>
-    <t>https://dataexplorer.ts.adex.org.in/dataset/1da21f2b-87f6-4641-81bd-ed6bcd461303</t>
+    <t>WRMS</t>
   </si>
   <si>
     <t>datasets-documentation/telangana_crop_data_documentation.md</t>
   </si>
   <si>
     <t>use-case-one-pager/telangana_crop_data_use_case.md</t>
-  </si>
-  <si>
-    <t>Expansion of voice data collection and development of use cases [Mozilla]</t>
-  </si>
-  <si>
-    <t>https://commonvoice.mozilla.org/</t>
-  </si>
-  <si>
-    <t>1st Lacuna Fund Grant: 1st NLP call</t>
-  </si>
-  <si>
-    <t>https://lacunafund.org/datasets/language/</t>
-  </si>
-  <si>
-    <t>Radiant Earth - Geospatial Machine Learning in Africa</t>
-  </si>
-  <si>
-    <t>https://beta.source.coop/repositories/radiantearth/south-africa-crops-competition/description/</t>
-  </si>
-  <si>
-    <t>Training of trainer on open earth observation AI -ML4EO Radiant Earth</t>
-  </si>
-  <si>
-    <t>https://beta.source.coop/radiantearth/south-africa-crops-competition/</t>
-  </si>
-  <si>
-    <t>Digital Green - Local dataset collection for climate-smart agriculture</t>
-  </si>
-  <si>
-    <t>https://github.com/digitalgreenorg/frame-templates</t>
-  </si>
-  <si>
-    <t>EcoVision Lab: High Carbon Stock Mapping in Southeast Asia</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/datasets/HCSA/HCSA_Indonesia_Forest_Plot_Data_2023</t>
-  </si>
-  <si>
-    <t>KNUST Responsible AI Lab (RAIL)</t>
-  </si>
-  <si>
-    <t>https://www.kaggle.com/datasets/responsibleailab/crop-disease-ghana/data</t>
-  </si>
-  <si>
-    <t>Wadhwani AI - Scale Cotton Pest management to Maize (amended)</t>
-  </si>
-  <si>
-    <t>https://github.com/WadhwaniAI/pest-monitoring/tree/main/sample-data</t>
-  </si>
-  <si>
-    <t>100 hours of Text to Speech Dataset for Mundari Language</t>
-  </si>
-  <si>
-    <t>https://github.com/karya-inc/dataset-mundari-tts + https://github.com/karya-inc/dataset-hindi-mundari-translation</t>
-  </si>
-  <si>
-    <t>Speech Data Collection South Africa (10 Languages)</t>
-  </si>
-  <si>
-    <t>https://commonvoice.mozilla.org/de/languages</t>
-  </si>
-  <si>
-    <t>Open AI in Agriculture (Ghana)</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/datasets/KaraAgroAI/CADI-AI/tree/main</t>
-  </si>
-  <si>
-    <t>IISc - Open Voice Data in Indian Languages</t>
-  </si>
-  <si>
-    <t>https://syspin.iisc.ac.in/datasets</t>
-  </si>
-  <si>
-    <t>Text Data Collection for 3 regional languages in Indonesia</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/datasets/prosa-text/nusa-dialogue</t>
-  </si>
-  <si>
-    <t>KAB Platform - Gramvaani Automatic Speech Recognition (ASR)</t>
-  </si>
-  <si>
-    <t>https://gitlab.com/gramvaani/giz_kab_bert_sourcecode</t>
-  </si>
-  <si>
-    <t>Africa Biomass Challenge</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/datasets/data354/Africa_Biomass_dataset</t>
   </si>
 </sst>
 </file>
@@ -147,7 +63,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,12 +89,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -209,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -220,23 +130,20 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,18 +447,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="34.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="22.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="26.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="22.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="34.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="22.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="26.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="22.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25" customFormat="1" s="1">
@@ -573,206 +481,32 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="91.5">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="28.5" customFormat="1" s="1">
-      <c r="A3" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="28.5" customFormat="1" s="1">
-      <c r="A4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="62.25" customFormat="1" s="1">
-      <c r="A5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="51" customFormat="1" s="1">
-      <c r="A6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="39.75" customFormat="1" s="1">
-      <c r="A7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="51" customFormat="1" s="1">
-      <c r="A8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="51" customFormat="1" s="1">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="51" customFormat="1" s="1">
-      <c r="A10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="73.5" customFormat="1" s="1">
-      <c r="A11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="28.5" customFormat="1" s="1">
-      <c r="A12" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="39.75" customFormat="1" s="1">
-      <c r="A13" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="28.5" customFormat="1" s="1">
-      <c r="A14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25" customFormat="1" s="1">
-      <c r="A15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25" customFormat="1" s="1">
-      <c r="A16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25" customFormat="1" s="1">
-      <c r="A17" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
back to old layout
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Dataset Name</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Lacuna Datasets</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t xml:space="preserve">- </t>
@@ -128,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -143,9 +146,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
@@ -468,13 +468,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="34.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="22.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="26.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="22.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="34.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="22.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="26.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="22.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25" customFormat="1" s="1">
@@ -530,20 +530,20 @@
       <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>16</v>
+      <c r="D3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying to add description
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10119"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonas/Library/CloudStorage/GoogleDrive-jonas.nothnagel@gmail.com/My Drive/giz/coding/datasets/docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0006F11C-061F-104A-AAE5-B929DBC3BBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t>Project Title</t>
   </si>
@@ -226,14 +232,19 @@
   </si>
   <si>
     <t>https://huggingface.co/datasets/data354/Africa_Biomass_dataset</t>
+  </si>
+  <si>
+    <t>Description and How to Use it</t>
+  </si>
+  <si>
+    <t>This AI application and replication-kit is about an AI-based crop type map for Telangana. This should be of use to anyone wishing to support sustainable farming practices and evidence-based decision-making for agricultural. Also, this can be used to empower you, as a local business, and NGOs, or a government agency to develop digital agricultural applications. The application focuses on creating localized ground-truth data on several different crop related variables to train AI models tailored to Telangana's diverse agricultural landscape.  This includes an open-access ground-truth dataset, a data challenge with openly available models for yield prediction, a crop classification model using satellite imagery applied to map the whole state of Telangana, and a roadmap for AI implementation in agriculture. Datasets, AI models, and crop maps are all openly available as an open-source replication kit and digital public good.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,7 +267,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF24292e"/>
+      <color rgb="FF24292E"/>
       <name val="Menlo Regular"/>
       <family val="2"/>
     </font>
@@ -286,6 +297,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -314,50 +330,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -368,10 +384,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -409,71 +425,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -501,7 +517,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -524,11 +540,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -537,13 +553,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -553,7 +569,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -562,7 +578,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -571,7 +587,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -579,10 +595,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -647,373 +663,367 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="10" width="45.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="21.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="20.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="20.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="22.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="45.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="26.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="11" width="22.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="45.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="19.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="63" customFormat="1" s="1">
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="184" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="77.25" customFormat="1" s="1">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="77.25" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="31.5" customFormat="1" s="1">
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="31.5" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="42" customFormat="1" s="1">
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="42" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="126" customFormat="1" s="1">
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="126" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="60" customFormat="1" s="1">
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="60" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="131" customFormat="1" s="1">
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="131" customHeight="1">
       <c r="A8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="55" customFormat="1" s="1">
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="55" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="F9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="56" customFormat="1" s="1">
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1" ht="56" customHeight="1">
       <c r="A10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="51" customFormat="1" s="1">
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" ht="51" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="66" customFormat="1" s="1">
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="66" customHeight="1">
       <c r="A12" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="52" customFormat="1" s="1">
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" ht="52" customHeight="1">
       <c r="A13" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="62" customFormat="1" s="1">
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" ht="62" customHeight="1">
       <c r="A14" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="51" customFormat="1" s="1">
+    </row>
+    <row r="15" spans="1:9" s="1" customFormat="1" ht="51" customHeight="1">
       <c r="A15" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="D15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="F15" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="62" customFormat="1" s="1">
+    </row>
+    <row r="16" spans="1:9" s="1" customFormat="1" ht="62" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="B16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="G16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lots and lots of changes2
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -970,10 +970,14 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Soil Health Data</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
+          <t>Open Soil Data for local AI Innovation in Telangana</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Measuring Soil Health for more Sustainable Agriculture in Telangana and beyond</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
@@ -1013,7 +1017,11 @@
           <t>India</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>AI Pest Management: Open Data for Pink Bollworms and American Bollworms</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr">
         <is>
           <t>Cotton Ace: AI-driven Pest Management for Cotton Farmers in India</t>
@@ -1091,17 +1099,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Digital Green - Local dataset collection for climate-smart agriculture</t>
+          <t>Geospatial dataset of wheat and rice farmers in Bihar, India</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Enabling farmers in India to reduce greenhouse gas emissions on their soil</t>
+          <t>Data-driven decision-making for farmers to increase climate resilience</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>GHG estimation for smallholder farmers in Bihar</t>
+          <t>The project developed a scalable data collection model for JEEViKA’s frontline workers, integrating digital tools and geofencing, and empowered farmers with personalized climate-smart advice through Farmer Scorecards.</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1109,7 +1117,11 @@
           <t>https://github.com/digitalgreenorg/frame-templates</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>https://github.com/digitalgreenorg/frame-templates</t>
+        </is>
+      </c>
       <c r="H14" t="inlineStr">
         <is>
           <t>Agriculture, Climate Action</t>
@@ -1152,12 +1164,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Farm Boundaries and Crop Cultivation in Telangana State</t>
+          <t>Open Dataset of Farm Boundaries and Crop Cultivation in Telangana State</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Support farmers in Telangana through AI-powered Crop Identification</t>
+          <t>Support Sustainable Agriculture in Telangana through AI-powered Crop Identification</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1171,11 +1183,7 @@
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Agriculture, Climate Action</t>
-        </is>
-      </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
           <t>Use-Case, Dataset</t>
@@ -1240,15 +1248,27 @@
           <t>India</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Open Air Pollution Data for Patna and Gurugram</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>Combatting Air Pollution and GHG Emissions in India through hyperlocal AI-powered mapping</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://vayu.undp.org.in/</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>https://vayu.undp.org.in/</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
@@ -1276,16 +1296,39 @@
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Forest Forward II: Using AI to map carbon-rich Forests to Combat Climate Change and Protect Livelihoods in India (High Carbon Stock Approach)</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
+          <t>Forest Forward II: Using AI to map carbon in forests using High Carbon Stock Approach and assess fire vulnerability of forests to Combat Climate Change and Protect Livelihoods in India</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Mapping carbon content in forests: This application leverages advanced geospatial technologies, such as remote sensing and AI, to support forest conservation efforts in India. The application will allow stakeholders to better monitor forest health, estimate biomass, and contribute to climate mitigation efforts.
+ Fire Vulnerability Mapping: This application would help develop a fire vulnerability map which could help to identify areas that are prone to fires based on several forest degradation indicators.</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Climate Action</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Pilot, Dataset</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Geospatial</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Michael Anthony &lt;michael@vertify.earth&gt;
+ Aishwarya Salvi &lt;aishwarya.santoshsalvi@giz.de&gt;
+ Jonas Nothnagel &lt;jonas.nothnagel@giz.de&gt;</t>
+        </is>
+      </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
@@ -1306,10 +1349,14 @@
           <t>India</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Open Soil Data for local AI Innovation in Telangana</t>
+        </is>
+      </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Conserving soils in Telangana through GeoAI</t>
+          <t>Measuring Soil Health for more Sustainable Agriculture in Telangana and beyond</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1343,11 +1390,14 @@
           <t>India</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Open-source text-to-speech datasets in 9 Indian languages (Hindi | Bengali | Marathi | Telugu | Bhojpuri | Kannada | Magadhi | Chhattisgarhi | Maithili)</t>
+        </is>
+      </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Building voice-enabled applications in local languages in India 
- Text to Speech models for 9 Indian languages</t>
+          <t>Build inclusive voice technologies in 9 Indian Languages through open language datasets</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1431,8 +1481,16 @@
           <t>India</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Open-source text-to-speech and machine translation datasets in Mundari</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Open-source text-to-speech and machine translation datasets in Mundari</t>
+        </is>
+      </c>
       <c r="E20" t="inlineStr">
         <is>
           <t>100 hours of Text to Speech Dataset for Mundari Language</t>
@@ -1440,7 +1498,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://github.com/karya-inc/dataset-hindi-mundari-translation</t>
+          <t>https://github.com/karya-inc/dataset-hindi-mundari-translation; https://github.com/karya-inc/dataset-mundari-tts</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1497,7 +1555,11 @@
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Natural Language Processing</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
@@ -1529,7 +1591,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Improve Kahi Ankahi Baatein (KAB) platform, m – Fine-tuned Hindi LLM for better user experience</t>
+          <t>Improve Kahi Ankahi Baatein (KAB) platform. Fine-tuned Hindi LLM for better user experience.</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1538,7 +1600,11 @@
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Natural Language Processing</t>
+        </is>
+      </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
@@ -1620,10 +1686,14 @@
           <t>India</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Question-Answer Pairs on Health Related Content in Telugu and Chhatisgarhi</t>
+        </is>
+      </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Digital Audio Content Creation for Women's Empowerment Using Language Technologies</t>
+          <t>Empowering Women Across India with Knowledge in Their Native Languages</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1631,7 +1701,11 @@
           <t>Using TTS models to create health-related audio messages that can be shared with civil society organizations for awareness raising and capacity building</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>https://www.audiopedia.foundation/bharat</t>
+        </is>
+      </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
@@ -1657,10 +1731,14 @@
           <t>India</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Open-source text-to-speech datasets in 9 Indian languages (Hindi | Bengali | Marathi | Telugu | Bhojpuri | Kannada | Magadhi | Chhattisgarhi | Maithili)</t>
+        </is>
+      </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Leveraging voice datasets in 9 Indian languages for climate action &amp; sustainable agriculture (IISc &amp; Bashini)</t>
+          <t>Hack4TTS: Crafting Voice for India’s Low-Resource Languages - Building TTS Systems for Low-Resource Indian Languages with Accent and Style Transfer</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1686,52 +1764,101 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Expand Pest Management App to Apple Value Chain</t>
+          <t>HCSA: High Carbon Stock Mapping in Southeast Asia</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Indonesien</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Forest Forward I: Using AI to map carbon-rich Forests to Combat Climate Change and Protect Livelihoods in Indonesia (High Carbon Stock Approach)</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>This project focuses on creating validated, open-source High Carbon Stock (HCS) forest maps for Indonesia using an AI-driven approach. It adopts the HCS classification system to identify forests suitable for conservation versus sustainable development:
+ • High, Medium, and Low-Density Forests (Conservation Priority): Forests with closed or patchy canopies, rich biodiversity, and carbon storage.
+ • Young Regenerating Forests: Regrowing forests that are transitioning into higher carbon stock potential.
+ • Scrub and Open Land: Areas with minimal carbon stock suitable for sustainable development.
+ The maps integrate field data, satellite imagery, and AI to assist policymakers, NGOs, and businesses in making data-driven decisions for sustainable land-use planning and conservation. Stakeholders can use the outputs for spatial planning, reducing greenhouse gas emissions, and implementing "no deforestation" commitments. The High Carbon Stock Approach (HCSA) project was nominated for the prestigious UN SDG Game Changer award – Category 2: Planet – Innovation for our climate and environment “Artificial Intelligence Meets Jungle/ Forest Forward.</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://huggingface.co/datasets/HCSA/HCSA_Indonesia_Forest_Plot_Data_2023</t>
+        </is>
+      </c>
       <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Climate Action</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Use-Case, Dataset</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Geospatial</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Indonesia’s Ministry of National Development Planning (Bappenas), JKPP https://jkpp.org/, [HCSA](https://highcarbonstock.org/public-consultation/), [EcoVision Lab](https://www.spacehub.uzh.ch/en/research-areas/earth-observation/EcoVision-Lab.html)</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>The finalized HCS dataset and maps are available on Hugging Face HCSA/Forest_Plot_Data_2023, and Global Forest Watch.
+ • License: Open-source (CC BY 4.0) 
+ • Data Type: Geospatial and tabular 
+ • Key Variables: Vegetation classification, carbon stock levels, validation points, and FPIC (Free, Prior and Informed Consent) compliance
+ • Appr. No of observations: Covers ~1.5 million hectares of tropical forests 
+ • Appr. No of dimensions: 60+ attributes, covering vegetation classifications, carbon stock levels, biomass measurements, land-use types, validation points, and FPIC (Free, Prior and Informed Consent) compliance data
+ • Covering 150 field plot high-carbon stock areas across Sumatra, Kalimantan, and West Papua
+ • Format: Geo TIFF, shapefile, CSV
+ The data adheres to FAIR (Findable, Accessible, Interoperable, Reusable) principles and includes anonymization measures to protect sensitive information.</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Processed Data:
+ Field measurements (e.g., biomass and tree species) were combined with Sentinel-2 imagery and NASA GEDI lidar to enhance map accuracy. The resulting geospatial data includes classifications of High Carbon Stock forests and other land-use categories.
+ Model Development:
+ AI models, trained using Convolutional Neural Networks (CNNs) and calibrated with aerial LiDAR and ground-truth data, are hosted on the HCSA GitHub repository: HCS Mapping Code.
+ Application:
+ Validated HCS maps are deployed on Google Earth Engine and Global Forest Watch for conservation planning and policy support, with an ODK-based mobile app under development for offline data collection. The project integrates FPIC (Free, Prior, and Informed Consent) principles throughout, ensuring community involvement and respect for land rights in data collection and mapping.</t>
+        </is>
+      </c>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr">
         <is>
-          <t>ML4EO</t>
+          <t>Computer Vision</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Zindi Crop Classification Data Challenge</t>
+          <t>Text data collection Indonesia</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Indonesien</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Zindi Crop Classification Data Challenge</t>
-        </is>
-      </c>
+      <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Follow-up Activity of Telangana Crop Data Collection</t>
+          <t>Text data collection for 3 regional languages</t>
         </is>
       </c>
       <c r="F27" t="inlineStr"/>
@@ -1745,14 +1872,14 @@
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr">
         <is>
-          <t>ML4EO</t>
+          <t>NLP</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>HCSA: High Carbon Stock Mapping in Southeast Asia</t>
+          <t>Use case development Indonesia</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1763,78 +1890,77 @@
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Forest Forward I: Using AI to map carbon-rich Forests to Combat Climate Change and Protect Livelihoods in Indonesia (High Carbon Stock Approach)</t>
+          <t>Climate Disinformation in Local Indonesian Languages</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>This project focuses on creating validated, open-source High Carbon Stock (HCS) forest maps for Indonesia using an AI-driven approach. It adopts the HCS classification system to identify forests suitable for conservation versus sustainable development:
- • High, Medium, and Low-Density Forests (Conservation Priority): Forests with closed or patchy canopies, rich biodiversity, and carbon storage.
- • Young Regenerating Forests: Regrowing forests that are transitioning into higher carbon stock potential.
- • Scrub and Open Land: Areas with minimal carbon stock suitable for sustainable development.
- The maps integrate field data, satellite imagery, and AI to assist policymakers, NGOs, and businesses in making data-driven decisions for sustainable land-use planning and conservation. Stakeholders can use the outputs for spatial planning, reducing greenhouse gas emissions, and implementing "no deforestation" commitments. The High Carbon Stock Approach (HCSA) project was nominated for the prestigious UN SDG Game Changer award – Category 2: Planet – Innovation for our climate and environment “Artificial Intelligence Meets Jungle/ Forest Forward.</t>
+          <t>This AI application is about developing an AI-based system to tackle climate misinformation in Indonesia, focusing on creating accurate and accessible information tools. The initiative aims to build a multilingual disinformation detection system, covering Bahasa Indonesia and over 10,6 million words and 21 million words translation from Minangkabau, Balinese, and Buginese to classify and verify climate-related content. The application supports stakeholders, including government agencies, NGOs, and communities, in countering false narratives, promoting awareness, and enabling evidence-based decision-making. The AI outcomes include open-access datasets, disinformation, and topic classification models, a user-friendly website, and a chatbot. These tools empower users to identify climate misinformation, enhance public literacy, and foster collaboration for sustainable climate actions. The project emphasizes inclusivity, accessibility, and long-term impact, providing resources for researchers, local businesses, and policy-makers to advance AI applications in combating misinformation. Prosa has developed an AI-powered chatbot to address climate misinformation. The platform's website is available at faktaiklim.prosa.ai, and the chatbot can be accessed via Telegram (Fakta Iklim Bot), with open-source code available on GitHub. User guides are provided in four languages: Indonesian, Minangkabau, Balinese, and Bugis.</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://huggingface.co/datasets/HCSA/HCSA_Indonesia_Forest_Plot_Data_2023</t>
+          <t>https://huggingface.co/prosa-text</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Climate Action</t>
+          <t>Climate Action, Natural Language Processing</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Use-Case, Dataset</t>
+          <t>Dataset, Use-Case</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Geospatial</t>
+          <t>Text</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Indonesia’s Ministry of National Development Planning (Bappenas), JKPP https://jkpp.org/, [HCSA](https://highcarbonstock.org/public-consultation/), [EcoVision Lab](https://www.spacehub.uzh.ch/en/research-areas/earth-observation/EcoVision-Lab.html)</t>
+          <t>Karlina Octaviany (GIZ), Ruth Schmidt (GIZ), Indonesia’s Ministry of National Development Planning (Bappenas), Prosa AI</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>The finalized HCS dataset and maps are available on Hugging Face HCSA/Forest_Plot_Data_2023, and Global Forest Watch.
- • License: Open-source (CC BY 4.0) 
- • Data Type: Geospatial and tabular 
- • Key Variables: Vegetation classification, carbon stock levels, validation points, and FPIC (Free, Prior and Informed Consent) compliance
- • Appr. No of observations: Covers ~1.5 million hectares of tropical forests 
- • Appr. No of dimensions: 60+ attributes, covering vegetation classifications, carbon stock levels, biomass measurements, land-use types, validation points, and FPIC (Free, Prior and Informed Consent) compliance data
- • Covering 150 field plot high-carbon stock areas across Sumatra, Kalimantan, and West Papua
- • Format: Geo TIFF, shapefile, CSV
- The data adheres to FAIR (Findable, Accessible, Interoperable, Reusable) principles and includes anonymization measures to protect sensitive information.</t>
+          <t>The data for this project is fully open-sourced and can be accessed through Hugging Face.
+ ● License: CC BY-SA 4.0
+ ● Data Type: Tabular
+ ● Key Variables: Climate disinformation classification, topic categorization, language distribution (Bahasa Indonesia and regional languages: Minangkabau, Balinese, Buginese)
+ ● Format: CSV
+ ● Data Collection Period: Over 3 months, covering diverse misinformation cases in climate-related domains
+ Data collection involved web crawling and inputs from local communities and experts, using sources like government websites, news articles, and scientific literature. Annotations by trained linguists and marginalized community members followed strict guidelines for consistency. The datasets are formatted for easy integration with AI tools.</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Processed Data:
- Field measurements (e.g., biomass and tree species) were combined with Sentinel-2 imagery and NASA GEDI lidar to enhance map accuracy. The resulting geospatial data includes classifications of High Carbon Stock forests and other land-use categories.
- Model Development:
- AI models, trained using Convolutional Neural Networks (CNNs) and calibrated with aerial LiDAR and ground-truth data, are hosted on the HCSA GitHub repository: HCS Mapping Code.
- Application:
- Validated HCS maps are deployed on Google Earth Engine and Global Forest Watch for conservation planning and policy support, with an ODK-based mobile app under development for offline data collection. The project integrates FPIC (Free, Prior, and Informed Consent) principles throughout, ensuring community involvement and respect for land rights in data collection and mapping.</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr"/>
+          <t>Processed Data and Pretrained Models:
+ Use the multilingual datasets and pre-trained models (IndoBERT, IndoBERTNusa) to detect climate misinformation. The processed dataset can be accessed here: Processed Data
+ Code for AI Models:
+ Access the GitHub repository containing scripts for preprocessing datasets, fine-tuning language models, and training disinformation classifiers. These can be customized for various applications.
+ Application Deployment:
+ The resulting models are integrated into platforms like Kominfo's Anti-Hoax portal and social media crawling APIs. Additionally, a chatbot leveraging these AI models is available to verify climate-related information in real-time. The chatbot and models are publicly accessible via APIs to support further innovation and integration by developers.</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>You can leverage AI models and datasets to develop or enhance applications to address climate misinformation and advance public education. These resources can be adapted to new languages, regions, or even other misinformation topics, such as health or political issues. Combining the datasets with additional sources, like satellite imagery or weather data, could lead to innovative AI applications, including real-time fact-checking tools or misinformation monitoring dashboards. Researchers and developers can also use the models to benchmark against other datasets or refine methodologies, unlocking opportunities for both academic and commercial advancements.
+ These tools can be integrated into platforms like government portals or social media moderation systems to maximize impact. Interactive educational applications, such as gamified platforms or public learning modules, could further engage communities. Collaboration with stakeholders—including government agencies, NGOs, and private companies—can help scale the tools, secure funding, and drive wider adoption. Through partnerships and expanded deployment, this project can contribute to fostering critical awareness and combating misinformation effectively.</t>
+        </is>
+      </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Computer Vision</t>
+          <t>NLP</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Text data collection Indonesia</t>
+          <t>Blue economy for climate mitigation and climate - leveraging AI, community-based approaches and local IoT-measurements</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1843,10 +1969,14 @@
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Blue economy for climate mitigation and climate - leveraging AI, community-based approaches and local IoT-measurements</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Text data collection for 3 regional languages</t>
+          <t>Follow up of HCSA with focus on blue carbon and training of marginalized communities, as well as policy dialogue on climate</t>
         </is>
       </c>
       <c r="F29" t="inlineStr"/>
@@ -1860,173 +1990,55 @@
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr">
         <is>
-          <t>NLP</t>
+          <t>ML4EO</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Use case development Indonesia</t>
+          <t>Early Warning System LDRI</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Indonesien</t>
+          <t>Kenya</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Climate Disinformation in Local Indonesian Languages</t>
+          <t>Early warning system for maize and beans for climate-smart agriculture in Kenya</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>This AI application is about developing an AI-based system to tackle climate misinformation in Indonesia, focusing on creating accurate and accessible information tools. The initiative aims to build a multilingual disinformation detection system, covering Bahasa Indonesia and over 10,6 million words and 21 million words translation from Minangkabau, Balinese, and Buginese to classify and verify climate-related content. The application supports stakeholders, including government agencies, NGOs, and communities, in countering false narratives, promoting awareness, and enabling evidence-based decision-making. The AI outcomes include open-access datasets, disinformation, and topic classification models, a user-friendly website, and a chatbot. These tools empower users to identify climate misinformation, enhance public literacy, and foster collaboration for sustainable climate actions. The project emphasizes inclusivity, accessibility, and long-term impact, providing resources for researchers, local businesses, and policy-makers to advance AI applications in combating misinformation. Prosa has developed an AI-powered chatbot to address climate misinformation. The platform's website is available at faktaiklim.prosa.ai, and the chatbot can be accessed via Telegram (Fakta Iklim Bot), with open-source code available on GitHub. User guides are provided in four languages: Indonesian, Minangkabau, Balinese, and Bugis.</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>https://huggingface.co/prosa-text</t>
-        </is>
-      </c>
+          <t>The Early Warning System (EWS) is an AI-powered platform that monitors farming activities and supports climate-smart precision agriculture for smallholder farms. It uses geo-referenced data collected from farms through mobile phones and high-resolution satellite imagery. The system provides crop monitoring, yield prediction, pest/disease detection, and localized agricultural advisory services in multiple languages. The platform is currently accessed through both WhatsApp by farmers and a self-serve platform/API for institutional users.</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Climate Action, Natural Language Processing</t>
+          <t>Agriculture, Climate Action</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Dataset, Use-Case</t>
+          <t>Use-Case, Dataset</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Text</t>
+          <t>Geospatial, Images</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Karlina Octaviany (GIZ), Ruth Schmidt (GIZ), Indonesia’s Ministry of National Development Planning (Bappenas), Prosa AI</t>
+          <t>University of Western Cape, CSIR, SAICA, GIZ</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
-        <is>
-          <t>The data for this project is fully open-sourced and can be accessed through Hugging Face.
- ● License: CC BY-SA 4.0
- ● Data Type: Tabular
- ● Key Variables: Climate disinformation classification, topic categorization, language distribution (Bahasa Indonesia and regional languages: Minangkabau, Balinese, Buginese)
- ● Format: CSV
- ● Data Collection Period: Over 3 months, covering diverse misinformation cases in climate-related domains
- Data collection involved web crawling and inputs from local communities and experts, using sources like government websites, news articles, and scientific literature. Annotations by trained linguists and marginalized community members followed strict guidelines for consistency. The datasets are formatted for easy integration with AI tools.</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>Processed Data and Pretrained Models:
- Use the multilingual datasets and pre-trained models (IndoBERT, IndoBERTNusa) to detect climate misinformation. The processed dataset can be accessed here: Processed Data
- Code for AI Models:
- Access the GitHub repository containing scripts for preprocessing datasets, fine-tuning language models, and training disinformation classifiers. These can be customized for various applications.
- Application Deployment:
- The resulting models are integrated into platforms like Kominfo's Anti-Hoax portal and social media crawling APIs. Additionally, a chatbot leveraging these AI models is available to verify climate-related information in real-time. The chatbot and models are publicly accessible via APIs to support further innovation and integration by developers.</t>
-        </is>
-      </c>
-      <c r="N30" t="inlineStr">
-        <is>
-          <t>You can leverage AI models and datasets to develop or enhance applications to address climate misinformation and advance public education. These resources can be adapted to new languages, regions, or even other misinformation topics, such as health or political issues. Combining the datasets with additional sources, like satellite imagery or weather data, could lead to innovative AI applications, including real-time fact-checking tools or misinformation monitoring dashboards. Researchers and developers can also use the models to benchmark against other datasets or refine methodologies, unlocking opportunities for both academic and commercial advancements.
- These tools can be integrated into platforms like government portals or social media moderation systems to maximize impact. Interactive educational applications, such as gamified platforms or public learning modules, could further engage communities. Collaboration with stakeholders—including government agencies, NGOs, and private companies—can help scale the tools, secure funding, and drive wider adoption. Through partnerships and expanded deployment, this project can contribute to fostering critical awareness and combating misinformation effectively.</t>
-        </is>
-      </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>NLP</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Blue economy for climate mitigation and climate - leveraging AI, community-based approaches and local IoT-measurements</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Indonesien</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Blue economy for climate mitigation and climate - leveraging AI, community-based approaches and local IoT-measurements</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Follow up of HCSA with focus on blue carbon and training of marginalized communities, as well as policy dialogue on climate</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>ML4EO</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Early Warning System LDRI</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Kenya</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Early warning system for maize and beans for climate-smart agriculture in Kenya</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>The Early Warning System (EWS) is an AI-powered platform that monitors farming activities and supports climate-smart precision agriculture for smallholder farms. It uses geo-referenced data collected from farms through mobile phones and high-resolution satellite imagery. The system provides crop monitoring, yield prediction, pest/disease detection, and localized agricultural advisory services in multiple languages. The platform is currently accessed through both WhatsApp by farmers and a self-serve platform/API for institutional users.</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>Agriculture, Climate Action</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>Use-Case, Dataset</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>Geospatial, Images</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>University of Western Cape, CSIR, SAICA, GIZ</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
         <is>
           <t>Ground truth geo-tagged data from 1,521 farms across 5 regions in Kenya
  Types of data: Crop images, farm boundaries, crop conditions, weekly activity logs
@@ -2036,7 +2048,7 @@
  Collection conducted by LDRI in partnership with champion farmers and agronomists.</t>
         </is>
       </c>
-      <c r="M32" t="inlineStr">
+      <c r="M30" t="inlineStr">
         <is>
           <t>Processed Data and Models:
  1. Uses geo-tagged images collected from farms and annotated for crop types, health status, and specific afflictions (pests/diseases/nutrition deficiency) 
@@ -2054,39 +2066,120 @@
  • Regional agricultural monitoring and planning</t>
         </is>
       </c>
-      <c r="N32" t="inlineStr">
+      <c r="N30" t="inlineStr">
         <is>
           <t>The EWS provides a comprehensive platform that combines AI-powered crop monitoring with localized advisory services. Organizations can access the data and models through :A self-serve platform and API for accessing predictions and analytics; Mobile applications for farmers to receive personalized crop management recommendations in local language; Integration possibilities with existing agricultural extension services and Analytics dashboards for value chain stakeholders and policy institutions. The system can be scaled to new regions and crops through transfer learning and the modular architecture allowing for continuous improvement of individual components. The platform supports both individual farmer-level insights and aggregated regional analytics to optimize crop yields and manage stressors effectively, making it valuable for various stakeholders across the agricultural sector.</t>
         </is>
       </c>
-      <c r="O32" t="inlineStr">
+      <c r="O30" t="inlineStr">
         <is>
           <t>Computer Vision</t>
         </is>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
+    <row r="31">
+      <c r="A31" t="inlineStr">
         <is>
           <t>Office of Data Protection Commission (ODPC) Chatbot Kenya</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B31" t="inlineStr">
         <is>
           <t>Kenya</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr">
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
         <is>
           <t>Providing citizens with information on data protection through the Chatbot of the office of the data protection commissioner in Kenya</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>Placeholder
  Total: 69,820
  Budget: total 40k EUR from FF (29,820k EUR come from DTC Kenya)</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>NLP</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>AIEP MVP Development</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Kenya</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Providing farmers in Kenya and Bihar, India with high-quality, personalized information through AI and developing blueprints for AI-powered Agriculture Information Exchange Platforms</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Developing products that can be replicated through four initiatives: 1. DynAG: 
+ Focused on rice, wheat, and maize, DynAG's platform uses a RAG pipeline powered by LLMs like the GPT suite to provide farmers with advisory services. Accessible via chatbots, Android and Jio-based mobile apps, IVR, and SMS, it ensures wide reach. With machine translation and speech recognition, the platform supports communication in English and Hindi while utilizing CGIAR's data backbone for accurate, data-driven insights. 
+ 2. Digital Green: 
+ Digital Green's platform supports agricultural value chains like dairy, coffee, and wheat in Bihar and Kenya. It integrates a RAG pipeline, using LLMs under evaluation, and offers services through an app, Telegram, and IVR. Features like machine translation, speech technology, image recognition, and weather data enable localized insights. The platform supports multiple languages, including Hindi, Swahili, Gikuyu, and Marathi, ensuring flexibility across regions. 
+ 3. Viamo and Partners: 
+ This platform targets farmers in Kenya and Bihar, focusing on beans and wheat, respectively. Using IVR, SMS, and WhatsApp, the platform is built on a RAG pipeline powered by LLMs, with potential for intent and entity recognition. Machine translation and speech-enabled IVR support English, Hindi, and Swahili, making it accessible across regions. The initiative is part of a broader plan to enhance voice technology for agricultural advisory. 
+ 4. Tech for Her: 
+ Tech for Her empowers women farmers in Bihar and Kenya, focusing on tomatoes and cattle. Accessible via IVR, WhatsApp, and a mobile app, the platform uses LLM-powered intent and entity recognition for personalized chatbot interactions and speech-enabled IVR for voice support. AI-based video generation further enhances engagement. Available in English, Hindi, and Swahili, it caters to the specific needs of women in agriculture.</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>NLP</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Support Mozilla Swahili grantee</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Kenya</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Paza Sauti - chatbot and interactive voice response service in Swahili to raise awareness about the use of collateral (security) to access credit for women in Kenya - see above</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Will see further enhancement of Mozilla grantee work - to actionable data sets and community based engagement feeding back into MCV</t>
         </is>
       </c>
       <c r="F33" t="inlineStr"/>
@@ -2107,7 +2200,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>AIEP MVP Development</t>
+          <t>Building Kenya Language Corpus incl. governance model</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2116,23 +2209,8 @@
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Providing farmers in Kenya and Bihar, India with high-quality, personalized information through AI and developing blueprints for AI-powered Agriculture Information Exchange Platforms</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Developing products that can be replicated through four initiatives: 1. DynAG: 
- Focused on rice, wheat, and maize, DynAG's platform uses a RAG pipeline powered by LLMs like the GPT suite to provide farmers with advisory services. Accessible via chatbots, Android and Jio-based mobile apps, IVR, and SMS, it ensures wide reach. With machine translation and speech recognition, the platform supports communication in English and Hindi while utilizing CGIAR's data backbone for accurate, data-driven insights. 
- 2. Digital Green: 
- Digital Green's platform supports agricultural value chains like dairy, coffee, and wheat in Bihar and Kenya. It integrates a RAG pipeline, using LLMs under evaluation, and offers services through an app, Telegram, and IVR. Features like machine translation, speech technology, image recognition, and weather data enable localized insights. The platform supports multiple languages, including Hindi, Swahili, Gikuyu, and Marathi, ensuring flexibility across regions. 
- 3. Viamo and Partners: 
- This platform targets farmers in Kenya and Bihar, focusing on beans and wheat, respectively. Using IVR, SMS, and WhatsApp, the platform is built on a RAG pipeline powered by LLMs, with potential for intent and entity recognition. Machine translation and speech-enabled IVR support English, Hindi, and Swahili, making it accessible across regions. The initiative is part of a broader plan to enhance voice technology for agricultural advisory. 
- 4. Tech for Her: 
- Tech for Her empowers women farmers in Bihar and Kenya, focusing on tomatoes and cattle. Accessible via IVR, WhatsApp, and a mobile app, the platform uses LLM-powered intent and entity recognition for personalized chatbot interactions and speech-enabled IVR for voice support. AI-based video generation further enhances engagement. Available in English, Hindi, and Swahili, it caters to the specific needs of women in agriculture.</t>
-        </is>
-      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
@@ -2151,7 +2229,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Support Mozilla Swahili grantee</t>
+          <t>AI Conversational Chatbot (with GovStack)</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2162,14 +2240,10 @@
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Paza Sauti - chatbot and interactive voice response service in Swahili to raise awareness about the use of collateral (security) to access credit for women in Kenya - see above</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Will see further enhancement of Mozilla grantee work - to actionable data sets and community based engagement feeding back into MCV</t>
-        </is>
-      </c>
+          <t>Hello, government - better citizen services through "AI Chatbots" as a digital public good</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
@@ -2188,7 +2262,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Building Kenya Language Corpus incl. governance model</t>
+          <t>Early Warning System LDRI – Phase 3</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2197,8 +2271,16 @@
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>SEE ABOVE</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Extension of AI based Food and Nutrition EWS (Phase 3)</t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
@@ -2210,32 +2292,36 @@
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr">
         <is>
-          <t>NLP</t>
+          <t>ML4EO</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>AI Conversational Chatbot (with GovStack)</t>
+          <t>Landslide monitoring use case</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Kenya</t>
+          <t>Rwanda</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Hello, government - better citizen services through "AI Chatbots" as a digital public good</t>
+          <t>Landslide monitoring and early warning system with AI in Rwanda</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Use-Case</t>
+        </is>
+      </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
@@ -2243,30 +2329,30 @@
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr">
         <is>
-          <t>NLP</t>
+          <t>Computer Vision</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Early Warning System LDRI – Phase 3</t>
+          <t>Expansion of voice data collection and development of use cases [Mozilla]</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Kenya</t>
+          <t>Rwanda</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr">
         <is>
-          <t>SEE ABOVE</t>
+          <t>Services to citizens in Swahili: Paza Sauti - chatbot and interactive voice response service in Swahili for better access to credit for women in Kenya and 5 other AI-powered services in Swahili based on Mozillas Common-Voice dataset</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Extension of AI based Food and Nutrition EWS (Phase 3)</t>
+          <t>Activity including local subactivities (Kinyarwanda, Luganda, Kiswahili)</t>
         </is>
       </c>
       <c r="F38" t="inlineStr"/>
@@ -2280,14 +2366,14 @@
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr">
         <is>
-          <t>ML4EO</t>
+          <t>NLP</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Landslide monitoring use case</t>
+          <t>Develop Mbaza AI Chatbot for Covid 19 [with Mozilla]</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2298,18 +2384,18 @@
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Landslide monitoring and early warning system with AI in Rwanda</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr"/>
+          <t>Mbaza Chatbot Rwanda for health related inquiries by citizens</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>PLACEHOLDER - Budget from #SDH</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>Use-Case</t>
-        </is>
-      </c>
+      <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
@@ -2317,14 +2403,14 @@
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Computer Vision</t>
+          <t>NLP</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Expansion of voice data collection and development of use cases [Mozilla]</t>
+          <t>Agriculture chatbot / early warning system for farmers / AI entrepreneurship competition</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2335,14 +2421,10 @@
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Services to citizens in Swahili: Paza Sauti - chatbot and interactive voice response service in Swahili for better access to credit for women in Kenya and 5 other AI-powered services in Swahili based on Mozillas Common-Voice dataset</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>Activity including local subactivities (Kinyarwanda, Luganda, Kiswahili)</t>
-        </is>
-      </c>
+          <t>Better Advise to farmers in Rwanda through Agricultural chatbot (Mbaza Chatbot scaling)</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr"/>
@@ -2361,7 +2443,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Develop Mbaza AI Chatbot for Covid 19 [with Mozilla]</t>
+          <t>Bot of Bots Activity - in collaboration with Govstack for Kenya</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2372,12 +2454,13 @@
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Mbaza Chatbot Rwanda for health related inquiries by citizens</t>
+          <t>Hello, government - better citizen services through "AI Chatbots" as a digital public good</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>PLACEHOLDER - Budget from #SDH</t>
+          <t>Semantic Chatbot(s) &amp; IVR for G2C services in Public Service Delivery and Good Governance 
+ in Collaboration with Konza Technopolis, ICTA</t>
         </is>
       </c>
       <c r="F41" t="inlineStr"/>
@@ -2398,7 +2481,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Agriculture chatbot / early warning system for farmers / AI entrepreneurship competition</t>
+          <t>Kinyarwanda Screen Reader for visually impaired people</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2407,11 +2490,7 @@
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Better Advise to farmers in Rwanda through Agricultural chatbot (Mbaza Chatbot scaling)</t>
-        </is>
-      </c>
+      <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
@@ -2431,7 +2510,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Bot of Bots Activity - in collaboration with Govstack for Kenya</t>
+          <t>ML4EO Crop Mapping Solution Rwanda</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2440,17 +2519,8 @@
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Hello, government - better citizen services through "AI Chatbots" as a digital public good</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Semantic Chatbot(s) &amp; IVR for G2C services in Public Service Delivery and Good Governance 
- in Collaboration with Konza Technopolis, ICTA</t>
-        </is>
-      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr"/>
@@ -2462,14 +2532,14 @@
       <c r="N43" t="inlineStr"/>
       <c r="O43" t="inlineStr">
         <is>
-          <t>NLP</t>
+          <t>ML4EO</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Kinyarwanda Screen Reader for visually impaired people</t>
+          <t>Landslide monitoring model development – data challenge/use case development follow-up</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2478,7 +2548,11 @@
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>SEE ABOVE</t>
+        </is>
+      </c>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
@@ -2491,264 +2565,202 @@
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr">
         <is>
-          <t>NLP</t>
+          <t>ML4EO</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ML4EO Crop Mapping Solution Rwanda</t>
+          <t>South Africa Crop Type Competition</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Rwanda</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>South Africa Crop Type Competition</t>
+        </is>
+      </c>
       <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>https://beta.source.coop/repositories/radiantearth/south-africa-crops-competition/description/</t>
+        </is>
+      </c>
       <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Climate Action, Agriculture</t>
+        </is>
+      </c>
       <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr"/>
-      <c r="K45" t="inlineStr"/>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Tabular</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>[Radiant Earth](https://radiant.earth/)</t>
+        </is>
+      </c>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr"/>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>ML4EO</t>
-        </is>
-      </c>
+      <c r="O45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Landslide monitoring model development – data challenge/use case development follow-up</t>
+          <t>NLP grant Localising Common Voice for South African Languages</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Rwanda</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr">
         <is>
-          <t>SEE ABOVE</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr"/>
+          <t>Making voice data available in all official languages of South Africa as a digital public good - Voices of Mzansi</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Univ of Stellenbosch Grant (Febe de Wet) - Voices of Mzansi project / localise SA local languages on Mozilla CV platform</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>https://commonvoice.mozilla.org/de/languages</t>
+        </is>
+      </c>
       <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
-      <c r="J46" t="inlineStr"/>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Natural Language Processing</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Audio</t>
+        </is>
+      </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr">
         <is>
-          <t>ML4EO</t>
+          <t>NLP</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>South Africa Crop Type Competition</t>
+          <t>ML-based site identification for MiniGrids in Uganda</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Uganda</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t>South Africa Crop Type Competition</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>https://beta.source.coop/repositories/radiantearth/south-africa-crops-competition/description/</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr"/>
+          <t>Electrification Dashboard for Ugandan government - help to find the best energy sources for villages in Uganda</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>This web application is a decision support tool. It is built as a prototype for a large-scale decision support tool for determining electrification strategies for different geographical areas. Currently implemented in Lamwo district electrification.</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>https://lamwo-electrification-demo.vercel.app/</t>
+        </is>
+      </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Climate Action, Agriculture</t>
+          <t>Climate Action</t>
         </is>
       </c>
       <c r="I47" t="inlineStr"/>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>Tabular</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>[Radiant Earth](https://radiant.earth/)</t>
-        </is>
-      </c>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr"/>
       <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr"/>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>Computer Vision</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>NLP grant Localising Common Voice for South African Languages</t>
+          <t>Croppie Coffee Yield Prediction</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Uganda</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Making voice data available in all official languages of South Africa as a digital public good - Voices of Mzansi</t>
+          <t>Croppie- helping smallholder coffee producers to plan sales, get loans, and trace coffee - AI powered coffee yield prediction</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Univ of Stellenbosch Grant (Febe de Wet) - Voices of Mzansi project / localise SA local languages on Mozilla CV platform</t>
+          <t>Croppie is a digital platform that integrates yield estimation functionality with agronomic advice and farm data management. The basic user interface is provided through a mobile application. Croppie’s core functionality is to allow for AI-supported coffee yield estimation. This is done by guiding a selective sampling for a statistical yield estimation service based on branch count and coffee branch picture taking, alongside the integration of additional data provided by the user.</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>https://commonvoice.mozilla.org/de/languages</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr"/>
+          <t>https://huggingface.co/datasets/rgautroncgiar/croppie_coffee_ug</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>https://huggingface.co/rgautroncgiar/croppie_coffee_ug</t>
+        </is>
+      </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Natural Language Processing</t>
+          <t>Agriculture, Climate Action</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Dataset</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>Audio</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr"/>
-      <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>NLP</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>ML-based site identification for MiniGrids in Uganda</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Uganda</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Electrification Dashboard for Ugandan government - help to find the best energy sources for villages in Uganda</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>This web application is a decision support tool. It is built as a prototype for a large-scale decision support tool for determining electrification strategies for different geographical areas. Currently implemented in Lamwo district electrification.</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>https://lamwo-electrification-demo.vercel.app/</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Climate Action</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr"/>
-      <c r="J49" t="inlineStr"/>
-      <c r="K49" t="inlineStr"/>
-      <c r="L49" t="inlineStr"/>
-      <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr"/>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>Computer Vision</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>Croppie Coffee Yield Prediction</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Uganda</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Croppie- helping smallholder coffee producers to plan sales, get loans, and trace coffee - AI powered coffee yield prediction</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>Croppie is a digital platform that integrates yield estimation functionality with agronomic advice and farm data management. The basic user interface is provided through a mobile application. Croppie’s core functionality is to allow for AI-supported coffee yield estimation. This is done by guiding a selective sampling for a statistical yield estimation service based on branch count and coffee branch picture taking, alongside the integration of additional data provided by the user.</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>https://huggingface.co/datasets/rgautroncgiar/croppie_coffee_ug</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>https://huggingface.co/rgautroncgiar/croppie_coffee_ug</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>Agriculture, Climate Action</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
           <t>Use-Case with Business Model</t>
         </is>
       </c>
-      <c r="J50" t="inlineStr"/>
-      <c r="K50" t="inlineStr">
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr">
         <is>
           <t>CIAT, Producers Direct, M-Omolumisa</t>
         </is>
       </c>
-      <c r="L50" t="inlineStr">
+      <c r="L48" t="inlineStr">
         <is>
           <t>The Data is fully open-sourced and can be accessed on Hugging Face
  • License: CC BY SA 4.0
@@ -2759,7 +2771,7 @@
  The data was collected over the span of 1.5 years covering different crop cycles between 2022 and 2024. The Data Collection was conducted by Alliance Bioversity &amp; CIAT and M-Omolumisa via on-the-ground visits of the farms.</t>
         </is>
       </c>
-      <c r="M50" t="inlineStr">
+      <c r="M48" t="inlineStr">
         <is>
           <t>Processed Data:
  The dataset is made of a mix of Arabica and Robusta coffee tree parts (with and without a background isolation element) with individual bounding boxes around all coffee cherries. These RGB pictures were on-farm collected with smartphones with the collaboration of smallholder farmers. 
@@ -2771,11 +2783,101 @@
  The dataset/model can be used for automated cherry count or coffee ripeness assessment.</t>
         </is>
       </c>
-      <c r="N50" t="inlineStr">
+      <c r="N48" t="inlineStr">
         <is>
           <t>Instead of manual cherry counts (the traditional approach to harvest estimation), pictures of the coffee branches are used to automate this task. The coffee harvest on a plot level is estimated by processing pictures through AI-supported image recognition software along with a manual branch count (= tree level estimation) and a tree-per-ha estimation (or recall data) (scaling to plot level). Thus, Croppie serves as a central system for managing yield data at the farmer level. It also provides the option to share this data with external users; with for example cooperatives having the possibility to feed information from the application in an integrated database of their member’s performance and farm characteristics, provided they obtained prior consent to do so. This would then scale the Croppie system to have an aggregated data view of multiple users in a region, e.g. as a cooperative level dashboard.</t>
         </is>
       </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>Computer Vision</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Scaling ML-based site identification for MiniGrids Uganda</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Uganda</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Finding good spots for decentralized green energy grids in Uganda I - AI based site identification for MiniGrids</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Moving towards scaling of the MiniGrid prototype</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>https://github.com/SunbirdAI/lamwo-electrification-project/tree/main</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>https://github.com/SunbirdAI/lamwo-electrification-project/tree/main</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Climate Action</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Use-Case</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Geospatial</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>Computer Vision</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Development of Unbiased AI Models for Solar Irradiance Uganda</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Uganda</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Finding good spots for decentralized green energy grids in Uganda II - Measuring Solar Irradiance wih unbiased AI Models</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
       <c r="O50" t="inlineStr">
         <is>
           <t>Computer Vision</t>
@@ -2785,7 +2887,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Scaling ML-based site identification for MiniGrids Uganda</t>
+          <t>NLP Use Case Strengthening relevance of Auditing reports in Uganda</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2794,14 +2896,10 @@
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Finding good spots for decentralized green energy grids in Uganda I - AI based site identification for MiniGrids</t>
-        </is>
-      </c>
+      <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Moving towards scaling of the MiniGrid prototype</t>
+          <t>This activity is requested by Uganda country office and paid for by them. It is run by the DSC and FF is supporting with technical input. No own funds needed for this.</t>
         </is>
       </c>
       <c r="F51" t="inlineStr"/>
@@ -2815,7 +2913,7 @@
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Computer Vision</t>
+          <t>NLP</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
major update: created python script to download images, changed layout
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -580,7 +580,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>African Biomass Challenge with Open Cocoa Data</t>
+          <t>Ghana Biomass Challenge: Ghana Crop Disease Detection Challenge</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -591,28 +591,28 @@
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Leveraging ML to predict above-ground biomass in cocoa plantations in Cote d'Ivoire</t>
+          <t>Leveraging ML for crop disease detection</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>the challenge was organized to predict biomass in shaded regions (cocoa plantations) in Cote d’Ivoire based on GEDI, Sentinel-2 and ground truth biomass data. Remote monitoring of the increase of biomass will help measure the impact of reforestation efforts in Cote d’Ivoire as well as detect degradation of forests due to cocoa, without requiring expensive and labor-intensive biomass estimates on the ground.</t>
+          <t>The Ghana Crop Disease Detection Challenge is an online data science challenge that seeks to leverage the power of Machine Learning and Artificial Intelligence to detect diseases that attack crops and offer immediate remedies.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://huggingface.co/datasets/data354/Africa_Biomass_dataset</t>
+          <t>https://www.kaggle.com/datasets/responsibleailab/crop-disease-ghana</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Climate Action</t>
+          <t>Agriculture</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Pilot</t>
+          <t>Dataset</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -622,7 +622,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>[Data354](https://data354.com/en/)</t>
+          <t>RAIL - KNUST (https://rail.knust.edu.gh/)</t>
         </is>
       </c>
       <c r="L3" t="inlineStr"/>
@@ -638,7 +638,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ghana Biomass Challenge: Ghana Crop Disease Detection Challenge</t>
+          <t>African Biomass Challenge with Open Cocoa Data</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -649,28 +649,28 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Leveraging ML for crop disease detection</t>
+          <t>Leveraging ML to predict above-ground biomass in cocoa plantations in Cote d'Ivoire</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>The Ghana Crop Disease Detection Challenge is an online data science challenge that seeks to leverage the power of Machine Learning and Artificial Intelligence to detect diseases that attack crops and offer immediate remedies.</t>
+          <t>the challenge was organized to predict biomass in shaded regions (cocoa plantations) in Cote d’Ivoire based on GEDI, Sentinel-2 and ground truth biomass data. Remote monitoring of the increase of biomass will help measure the impact of reforestation efforts in Cote d’Ivoire as well as detect degradation of forests due to cocoa, without requiring expensive and labor-intensive biomass estimates on the ground.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.kaggle.com/datasets/responsibleailab/crop-disease-ghana</t>
+          <t>https://huggingface.co/datasets/data354/Africa_Biomass_dataset</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Agriculture</t>
+          <t>Climate Action</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Dataset</t>
+          <t>Pilot</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -680,7 +680,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>RAIL - KNUST (https://rail.knust.edu.gh/)</t>
+          <t>Data354 (https://data354.com/en/)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr"/>
@@ -975,7 +975,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Soil Data Collection in Telangana</t>
+          <t>Digital Audio Content Creation for Women's Empowerment Using Language Technologies</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -985,39 +985,35 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Open Soil Data for local AI Innovation in Telangana</t>
+          <t>Question-Answer Pairs on Health Related Content in Telugu and Chhatisgarhi</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Measuring Soil Health for more Sustainable Agriculture in Telangana and beyond</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+          <t>Empowering Women Across India with Knowledge in Their Native Languages</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Using TTS models to create health-related audio messages that can be shared with civil society organizations for awareness raising and capacity building</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://www.audiopedia.foundation/bharat</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Agriculture, Climate Action</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Dataset</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Geospatial</t>
-        </is>
-      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Computer Vision</t>
+          <t>NLP</t>
         </is>
       </c>
       <c r="P12" t="inlineStr"/>
@@ -1025,7 +1021,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Wadhwani AI - Open AI for Cotton Pest Control with smallholder farmers - National Entrepreneurship Network (NEN)</t>
+          <t>Hyperlocal Mapping of Air Pollution and GHG Emissions in India with UNDP</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1035,66 +1031,31 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>AI Pest Management: Open Data for Pink Bollworms and American Bollworms</t>
+          <t>Open Air Pollution Data for Patna and Gurugram</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Cotton Ace: AI-driven Pest Management for Cotton Farmers in India</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Wadhwani AI has developed a mobile app to support cotton farmers combat pest infestations, a major threat to cotton productivity. For this, they have collaborated with FAIR Forward – AI for All, a project of German Development Cooperation. The app allows farmers to take photos of pheromone traps, which capture male bollworms, and uses an AI model to count the pests in the images. Based on the AI-generated counts, the app provides recommendations to farmers on how to respond. This technology empowers small-scale farmers to make informed decisions, reduce uncertainty in yield, and improve their livelihoods.
- As the codebase, dataset and research are openly available it can be used to build on, test and research similar applications in other contexts. This would esp. apply to problems of identification and counting of agricultural pests.</t>
-        </is>
-      </c>
+          <t>Combatting Air Pollution and GHG Emissions in India through hyperlocal AI-powered mapping</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://source.coop/repositories/wadhwani-ai/wiai-pm-open-data/description; https://github.com/WadhwaniAI/pest-management-opendata?tab=readme-ov-file; https://huggingface.co/datasets/wadhwani-ai/pest-management-opendata</t>
+          <t>https://vayu.undp.org.in/</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://github.com/WadhwaniAI/pest-monitoring, https://dl.acm.org/doi/10.1145/3394486.3403363</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Agriculture</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Use-Case, Dataset</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Images</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Wadhwani AI (agri-ai@wadhwaniai.org, https://github.com/WadhwaniAI/pest-monitoring)</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>Wadhwani AI with support from German Development Cooperation provided training data consisting of ca. 13,000 images:
- (a) These images were captured by farmers and farm extension workers since 2018
- (b) The dataset contains two types of images: those with pests and bounding boxes labelling either pink bollworm (PBW) or American bollworm (ABW), and those without pests, representing real-world user behavior.
- (c) License: Apache 2.0</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>Wadhwani AI with support from German Development cooperation provided the codebase of the pest identification model:
- (a) At its core, this repository packages an object detection implementation. 
- (b) While there are several object detection implementations, and even implementation aggregations, there are none that completely solve for the challenges faced here (e.g., highly diverse image quality, model size restrictions)
- (c) License: Apache 2.0</t>
-        </is>
-      </c>
+          <t>https://vayu.undp.org.in/</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr">
         <is>
@@ -1106,7 +1067,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Digital Green - Local dataset collection for climate-smart agriculture</t>
+          <t>IISc - Open Voice Data in Indian Languages</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1116,350 +1077,48 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Geospatial dataset of wheat and rice farmers in Bihar, India</t>
+          <t>Open-source text-to-speech datasets in 9 Indian languages (Hindi | Bengali | Marathi | Telugu | Bhojpuri | Kannada | Magadhi | Chhattisgarhi | Maithili)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Data-driven decision-making for farmers to increase climate resilience</t>
+          <t>Build inclusive voice technologies in 9 Indian Languages through open language datasets</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
-        <is>
-          <t>The project developed a scalable data collection model for JEEViKA’s frontline workers, integrating digital tools and geofencing, and empowered farmers with personalized climate-smart advice through Farmer Scorecards.</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>https://github.com/digitalgreenorg/frame-templates</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>https://github.com/digitalgreenorg/frame-templates</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Agriculture, Climate Action</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Pilot, Dataset</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Tabular</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>[Digital Green](https://digitalgreen.org/ourwork/india/)</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>Computer Vision</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>ML4EO Telangana: Crop Identification</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Open Dataset of Farm Boundaries and Crop Cultivation in Telangana State</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Support Sustainable Agriculture in Telangana through AI-powered Crop Identification</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>This AI application and replication-kit is about an AI-based crop type map for Telangana. This should be of use to anyone wishing to support sustainable farming practices and evidence-based decision-making for agricultural. Also, this can be used to empower you, as a local business, and NGOs, or a government agency to develop digital agricultural applications. The application focuses on creating localized ground-truth data on several different crop related variables to train AI models tailored to Telangana's diverse agricultural landscape. This includes an open-access ground-truth dataset, a data challenge with openly available models for yield prediction, a crop classification model using satellite imagery applied to map the whole state of Telangana, and a roadmap for AI implementation in agriculture. Datasets, AI models, and crop maps are all openly available as an open-source replication kit and digital public good.</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>https://dataexplorer.ts.adex.org.in/dataset/583e8f01-160e-4f51-bde5-31dc7f2a5887</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Agriculture, Climate Action</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Use-Case, Dataset</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Geospatial</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>[WRMS](https://wrmsglobal.com/)</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>The Data is fully open-sourced and can be accessed at the Telangana Data Exchange Platform: ADEX
- • License: CC BY 4.0
- • Data Type: Tabular
- • Key Variables: Crop type (6), Crop Health, Crop Yield, Irrigation Methods.
- • Appr. No of observations: &gt; 12000 
- • Appr. No of dimensions: 45 
- • Covering 6 Mandals in Telangana
- • Format: dbf, csv
- The data was collected over the span of 1.5 years covering different crop cycles between 2022 and 2024. The Data Collection was conducted by WRMS via on-the-ground visits of the fields and by surveying farmers in Telangana State.</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>Processed Data:
- The ground truth data was combined with open-source Sentinel-2 data to create a geospatial dataset with crop type as labels.
- The processed dataset can be accessed here: Processed Data
- Code for Crop Classification Model:
- Code to create the training data and for training the models for crop mapping can be accessed here: Code
- Application:
- The resulting shapefiles that predict crop type for the state of Telangana are deployed on DICRA – a digital public good ran by the Indian Development Bank NABARD and UNDP: DICRA
- Based on the collected data, GIZ organised a data challenged together with Zindi to build state-of-the-art crop mapping models. The outcomes of the challenge can be accessed here: Zindi</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>You can make use of the existing models on yield prediction and crop type mapping to infer other similar datapoints – for example neighbouring states of Telangana. Additionally, you can try to combine the dataset with other existing open-source datasets from the ADEX platform and conduct research/commercial scoping on these. 
- The present dataset is quite unique in the fact that it includes observations such as irrigation methods, crop health and expected yield. You may combine these with other data sources, i.e. satellite/remote sensing data (open-source or commercial) to build high-quality crop monitoring/recommendation systems to support various agricultural entities, farmers and decision makers in India. This could also inform commercial products. 
- As crop mapping is a prominent use-case, the data can be used for benchmarking different available crop datasets and models or inform foundational geospatial models as well as constitute to a region-wide crop mapping. Potential partners on the ground for collaboration, commercial involvement or funding are the Telangana Government, specifically the IT and Agricultural department and Nabard Dicra.</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>Computer Vision</t>
-        </is>
-      </c>
-      <c r="P15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Hyperlocal Mapping of Air Pollution and GHG Emissions in India with UNDP</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Open Air Pollution Data for Patna and Gurugram</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Combatting Air Pollution and GHG Emissions in India through hyperlocal AI-powered mapping</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>https://vayu.undp.org.in/</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>https://vayu.undp.org.in/</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>Computer Vision</t>
-        </is>
-      </c>
-      <c r="P16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Forest Forward</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Forest Forward II: Using AI to map carbon in forests using High Carbon Stock Approach and assess fire vulnerability of forests to Combat Climate Change and Protect Livelihoods in India</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Mapping carbon content in forests: This application leverages advanced geospatial technologies, such as remote sensing and AI, to support forest conservation efforts in India. The application will allow stakeholders to better monitor forest health, estimate biomass, and contribute to climate mitigation efforts.
- Fire Vulnerability Mapping: This application would help develop a fire vulnerability map which could help to identify areas that are prone to fires based on several forest degradation indicators.</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Climate Action</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Pilot, Dataset</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Geospatial</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>Michael Anthony &lt;michael@vertify.earth&gt;
- Aishwarya Salvi &lt;aishwarya.santoshsalvi@giz.de&gt;
- Jonas Nothnagel &lt;jonas.nothnagel@giz.de&gt;</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>Computer Vision</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>GeoAI for Soil Conservation: Innovations for Telangana</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Open Soil Data for local AI Innovation in Telangana</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Measuring Soil Health for more Sustainable Agriculture in Telangana and beyond</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Merged from 2 service contract: (1) implement CC recommendations nationla (110k) and (2) implement CC recommendations state (20k)</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>Computer Vision</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>IISc - Open Voice Data in Indian Languages</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Open-source text-to-speech datasets in 9 Indian languages (Hindi | Bengali | Marathi | Telugu | Bhojpuri | Kannada | Magadhi | Chhattisgarhi | Maithili)</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Build inclusive voice technologies in 9 Indian Languages through open language datasets</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
         <is>
           <t>This dataset is part of the initiative SYSPIN (SYnthesizing SPeech in INdian languages), that develops large open-source Text-to-Speech (TTS) corpora, i.e., speech training datasets and AI models in 9 Indian languages, namely – Bengali, Bhojpuri, Chhattisgarhi, Hindi, Kannada, Magahi, Maithili, Marathi, and Telugu. This data is useful for those wishing to build voice-enabled, user-friendly applications in Indian languages. Through voice-based solutions, these AI models can be used to empower communities that do not have access to digital services in their own native language. They can be used by private companies, researchers, NGOs or government departments to develop digital applications. 
  The datasets and TTS models are available to the AI community and anyone wishing to build voice-enabled applications in Indian languages.</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>https://syspin.iisc.ac.in/datasets</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr">
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
         <is>
           <t>Natural Language Processing</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>Pilot, Dataset</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>Audio</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>Dr Prasanta Ghosh, prasantag@iisc.ac.in 
- Dr Philipp Olbrich, philipp.olbrich@giz.de</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Dr Prasanta Ghosh (prasantag@iisc.ac.in), 
+ Dr Philipp Olbrich (philipp.olbrich@giz.de)</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
         <is>
           <t>The Data is fully open-sourced and can be accessed at:
  • Hugging face: &lt;Link To be added&gt;
@@ -1476,7 +1135,7 @@
  • Data was collected and created over 3 years from 2021-2024</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>Processed Data:
  The validated sentences were recording in a recording room (size 10'3" x 5'9") by voice artists using a Neumann TLM-103 studio microphone and Audio Interface UAD Apollo Twin X. 
@@ -1485,14 +1144,373 @@
  Audio files of Audiopedia Foundation’s content created in the low-resource language Chhattisgarhi using IISc TTS Chhattisgarhi model can be found here.</t>
         </is>
       </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>The TTS models can be used to develop innovative solutions and voice-based services for Indians in their native language. This would be especially beneficial for those who cannot read/write or have speech and visual disabilities but can access digital services through audio/voice-based mediums. The data and models are a crucial stepping stone for developing such assistive technologies. Including low-resource languages, some of which do not even have enough print/digital literature, would benefit vulnerable communities for whom language barriers make access to technological solutions even more difficult. The 720 hours of open-source TTS data also present immense opportunities for academic and industrial research.</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>NLP</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Wadhwani AI - Open AI for Cotton Pest Control with smallholder farmers - National Entrepreneurship Network (NEN)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>AI Pest Management: Open Data for Pink Bollworms and American Bollworms</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Cotton Ace: AI-driven Pest Management for Cotton Farmers in India</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Wadhwani AI has developed a mobile app to support cotton farmers combat pest infestations, a major threat to cotton productivity. For this, they have collaborated with FAIR Forward – AI for All, a project of German Development Cooperation. The app allows farmers to take photos of pheromone traps, which capture male bollworms, and uses an AI model to count the pests in the images. Based on the AI-generated counts, the app provides recommendations to farmers on how to respond. This technology empowers small-scale farmers to make informed decisions, reduce uncertainty in yield, and improve their livelihoods.
+ As the codebase, dataset and research are openly available it can be used to build on, test and research similar applications in other contexts. This would esp. apply to problems of identification and counting of agricultural pests.</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://source.coop/repositories/wadhwani-ai/wiai-pm-open-data/description; https://github.com/WadhwaniAI/pest-management-opendata?tab=readme-ov-file; https://huggingface.co/datasets/wadhwani-ai/pest-management-opendata</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>https://github.com/WadhwaniAI/pest-monitoring, https://dl.acm.org/doi/10.1145/3394486.3403363</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Agriculture</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Use-Case, Dataset</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Images</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Wadhwani AI (agri-ai@wadhwaniai.org), Github (https://github.com/WadhwaniAI/pest-monitoring)</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Wadhwani AI with support from German Development Cooperation provided training data consisting of ca. 13,000 images:
+ (a) These images were captured by farmers and farm extension workers since 2018
+ (b) The dataset contains two types of images: those with pests and bounding boxes labelling either pink bollworm (PBW) or American bollworm (ABW), and those without pests, representing real-world user behavior.
+ (c) License: Apache 2.0</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Wadhwani AI with support from German Development cooperation provided the codebase of the pest identification model:
+ (a) At its core, this repository packages an object detection implementation. 
+ (b) While there are several object detection implementations, and even implementation aggregations, there are none that completely solve for the challenges faced here (e.g., highly diverse image quality, model size restrictions)
+ (c) License: Apache 2.0</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Computer Vision</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Developing a concept with MFIN on voice-based chatbot</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>MicroFinance Industry Network India use of voice technology (Gramvaani)</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Contract name: Automation of components of the MFIN-CGRM CRM solution 
+ Follow-up project from former MFIN engagement to move from prototype to production and implement the remaining use-cases.</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://gitlab.com/gramvaani/giz_kab_bert_sourcecode</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Natural Language Processing</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Dataset, Pilot</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>GramVaani (https://gramvaani.org/)</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>NLP</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>100 hours of Text to Speech Dataset for Mundari Language</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Open-source text-to-speech and machine translation datasets in Mundari</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Open-source text-to-speech and machine translation datasets in Mundari</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>100 hours of Text to Speech Dataset for Mundari Language</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://github.com/karya-inc/dataset-hindi-mundari-translation; https://github.com/karya-inc/dataset-mundari-tts</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Natural Language Processing</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Karya (https://karya.in/)</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>NLP</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Digital Green - Local dataset collection for climate-smart agriculture</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Geospatial dataset of wheat and rice farmers in Bihar, India</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Data-driven decision-making for farmers to increase climate resilience</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>The project developed a scalable data collection model for JEEViKA’s frontline workers, integrating digital tools and geofencing, and empowered farmers with personalized climate-smart advice through Farmer Scorecards.</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://github.com/digitalgreenorg/frame-templates</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>https://github.com/digitalgreenorg/frame-templates</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Agriculture, Climate Action</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Pilot, Dataset</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Tabular</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Digital Green (https://digitalgreen.org/ourwork/india/)</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Computer Vision</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ML4EO Telangana: Crop Identification</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Open Dataset of Farm Boundaries and Crop Cultivation in Telangana State</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Support Sustainable Agriculture in Telangana through AI-powered Crop Identification</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>This AI application and replication-kit is about an AI-based crop type map for Telangana. This should be of use to anyone wishing to support sustainable farming practices and evidence-based decision-making for agricultural. Also, this can be used to empower you, as a local business, and NGOs, or a government agency to develop digital agricultural applications. The application focuses on creating localized ground-truth data on several different crop related variables to train AI models tailored to Telangana's diverse agricultural landscape. This includes an open-access ground-truth dataset, a data challenge with openly available models for yield prediction, a crop classification model using satellite imagery applied to map the whole state of Telangana, and a roadmap for AI implementation in agriculture. Datasets, AI models, and crop maps are all openly available as an open-source replication kit and digital public good.</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://dataexplorer.ts.adex.org.in/dataset/583e8f01-160e-4f51-bde5-31dc7f2a5887</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Agriculture, Climate Action</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Use-Case, Dataset</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Geospatial</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>WRMS (https://wrmsglobal.com/)</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>The Data is fully open-sourced and can be accessed at the Telangana Data Exchange Platform: ADEX
+ • License: CC BY 4.0
+ • Data Type: Tabular
+ • Key Variables: Crop type (6), Crop Health, Crop Yield, Irrigation Methods.
+ • Appr. No of observations: &gt; 12000 
+ • Appr. No of dimensions: 45 
+ • Covering 6 Mandals in Telangana
+ • Format: dbf, csv
+ The data was collected over the span of 1.5 years covering different crop cycles between 2022 and 2024. The Data Collection was conducted by WRMS via on-the-ground visits of the fields and by surveying farmers in Telangana State.</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Processed Data:
+ The ground truth data was combined with open-source Sentinel-2 data to create a geospatial dataset with crop type as labels.
+ The processed dataset can be accessed here: Processed Data
+ Code for Crop Classification Model:
+ Code to create the training data and for training the models for crop mapping can be accessed here: Code
+ Application:
+ The resulting shapefiles that predict crop type for the state of Telangana are deployed on DICRA – a digital public good ran by the Indian Development Bank NABARD and UNDP: DICRA
+ Based on the collected data, GIZ organised a data challenged together with Zindi to build state-of-the-art crop mapping models. The outcomes of the challenge can be accessed here: Zindi</t>
+        </is>
+      </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>The TTS models can be used to develop innovative solutions and voice-based services for Indians in their native language. This would be especially beneficial for those who cannot read/write or have speech and visual disabilities but can access digital services through audio/voice-based mediums. The data and models are a crucial stepping stone for developing such assistive technologies. Including low-resource languages, some of which do not even have enough print/digital literature, would benefit vulnerable communities for whom language barriers make access to technological solutions even more difficult. The 720 hours of open-source TTS data also present immense opportunities for academic and industrial research.</t>
+          <t>You can make use of the existing models on yield prediction and crop type mapping to infer other similar datapoints – for example neighbouring states of Telangana. Additionally, you can try to combine the dataset with other existing open-source datasets from the ADEX platform and conduct research/commercial scoping on these. 
+ The present dataset is quite unique in the fact that it includes observations such as irrigation methods, crop health and expected yield. You may combine these with other data sources, i.e. satellite/remote sensing data (open-source or commercial) to build high-quality crop monitoring/recommendation systems to support various agricultural entities, farmers and decision makers in India. This could also inform commercial products. 
+ As crop mapping is a prominent use-case, the data can be used for benchmarking different available crop datasets and models or inform foundational geospatial models as well as constitute to a region-wide crop mapping. Potential partners on the ground for collaboration, commercial involvement or funding are the Telangana Government, specifically the IT and Agricultural department and Nabard Dicra.</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>NLP</t>
+          <t>Computer Vision</t>
         </is>
       </c>
       <c r="P19" t="inlineStr"/>
@@ -1500,7 +1518,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>100 hours of Text to Speech Dataset for Mundari Language</t>
+          <t>Gramvaani Automatic Speech Recognition (ASR)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1508,47 +1526,27 @@
           <t>India</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Open-source text-to-speech and machine translation datasets in Mundari</t>
-        </is>
-      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Open-source text-to-speech and machine translation datasets in Mundari</t>
+          <t>Providing better information on sexual and reproductive health and rights (SRHR) of young people through the Kahi Ankahi Baatein infloline (Hindi LLM finetuning)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>100 hours of Text to Speech Dataset for Mundari Language</t>
+          <t>Improve Kahi Ankahi Baatein (KAB) platform, m – Fine-tuned Hindi LLM for better user experience</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://github.com/karya-inc/dataset-hindi-mundari-translation; https://github.com/karya-inc/dataset-mundari-tts</t>
+          <t>[GramVaani](https://gramvaani.org/)</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Natural Language Processing</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>Dataset</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>[Karya](https://karya.in/)</t>
-        </is>
-      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
@@ -1562,7 +1560,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Two Al-based dialogue systems (e.g. voice-based chatbot) in Indian Languages - consultancy for design implementation etc</t>
+          <t>Soil Data Collection in Telangana</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1570,29 +1568,41 @@
           <t>India</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Open Soil Data for local AI Innovation in Telangana</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Voice-based advisory for farmers (female kitchen gardeners) with NiceSSM / Use Case Gramvaani</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Creation of voice based chatbots</t>
-        </is>
-      </c>
+          <t>Measuring Soil Health for more Sustainable Agriculture in Telangana and beyond</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Agriculture, Climate Action</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Geospatial</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr">
         <is>
-          <t>NLP</t>
+          <t>Computer Vision</t>
         </is>
       </c>
       <c r="P21" t="inlineStr"/>
@@ -1600,7 +1610,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Gramvaani Automatic Speech Recognition (ASR)</t>
+          <t>Forest Forward</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1611,30 +1621,45 @@
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Providing better information on sexual and reproductive health and rights (SRHR) of young people through the Kahi Ankahi Baatein infloline (Hindi LLM finetuning)</t>
+          <t>Forest Forward II: Using AI to map carbon in forests using High Carbon Stock Approach and assess fire vulnerability of forests to Combat Climate Change and Protect Livelihoods in India</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Improve Kahi Ankahi Baatein (KAB) platform, m – Fine-tuned Hindi LLM for better user experience</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>[GramVaani](https://gramvaani.org/)</t>
-        </is>
-      </c>
+          <t>Mapping carbon content in forests: This application leverages advanced geospatial technologies, such as remote sensing and AI, to support forest conservation efforts in India. The application will allow stakeholders to better monitor forest health, estimate biomass, and contribute to climate mitigation efforts.
+ Fire Vulnerability Mapping: This application would help develop a fire vulnerability map which could help to identify areas that are prone to fires based on several forest degradation indicators.</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Climate Action</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Pilot, Dataset</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Geospatial</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Michael Anthony &lt;michael@vertify.earth&gt;
+ Aishwarya Salvi &lt;aishwarya.santoshsalvi@giz.de&gt;
+ Jonas Nothnagel &lt;jonas.nothnagel@giz.de&gt;</t>
+        </is>
+      </c>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr">
         <is>
-          <t>NLP</t>
+          <t>Computer Vision</t>
         </is>
       </c>
       <c r="P22" t="inlineStr"/>
@@ -1642,7 +1667,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Developing a concept with MFIN on voice-based chatbot</t>
+          <t>GeoAI for Soil Conservation: Innovations for Telangana</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1650,50 +1675,33 @@
           <t>India</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Open Soil Data for local AI Innovation in Telangana</t>
+        </is>
+      </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>MicroFinance Industry Network India use of voice technology (Gramvaani)</t>
+          <t>Measuring Soil Health for more Sustainable Agriculture in Telangana and beyond</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Contract name: Automation of components of the MFIN-CGRM CRM solution 
- Follow-up project from former MFIN engagement to move from prototype to production and implement the remaining use-cases.</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>https://gitlab.com/gramvaani/giz_kab_bert_sourcecode</t>
-        </is>
-      </c>
+          <t>Merged from 2 service contract: (1) implement CC recommendations nationla (110k) and (2) implement CC recommendations state (20k)</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Natural Language Processing</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>Dataset, Pilot</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>[GramVaani](https://gramvaani.org/)</t>
-        </is>
-      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr">
         <is>
-          <t>NLP</t>
+          <t>Computer Vision</t>
         </is>
       </c>
       <c r="P23" t="inlineStr"/>
@@ -1701,7 +1709,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Digital Audio Content Creation for Women's Empowerment Using Language Technologies</t>
+          <t>Two Al-based dialogue systems (e.g. voice-based chatbot) in Indian Languages - consultancy for design implementation etc</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1709,26 +1717,18 @@
           <t>India</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Question-Answer Pairs on Health Related Content in Telugu and Chhatisgarhi</t>
-        </is>
-      </c>
+      <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Empowering Women Across India with Knowledge in Their Native Languages</t>
+          <t>Voice-based advisory for farmers (female kitchen gardeners) with NiceSSM / Use Case Gramvaani</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Using TTS models to create health-related audio messages that can be shared with civil society organizations for awareness raising and capacity building</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>https://www.audiopedia.foundation/bharat</t>
-        </is>
-      </c>
+          <t>Creation of voice based chatbots</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
@@ -1789,7 +1789,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>HCSA: High Carbon Stock Mapping in Southeast Asia</t>
+          <t>Use case development Indonesia</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1800,10 +1800,92 @@
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
+          <t>Climate Disinformation in Local Indonesian Languages</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>This AI application is about developing an AI-based system to tackle climate misinformation in Indonesia, focusing on creating accurate and accessible information tools. The initiative aims to build a multilingual disinformation detection system, covering Bahasa Indonesia and over 10,6 million words and 21 million words translation from Minangkabau, Balinese, and Buginese to classify and verify climate-related content. The application supports stakeholders, including government agencies, NGOs, and communities, in countering false narratives, promoting awareness, and enabling evidence-based decision-making. The AI outcomes include open-access datasets, disinformation, and topic classification models, a user-friendly website, and a chatbot. These tools empower users to identify climate misinformation, enhance public literacy, and foster collaboration for sustainable climate actions. The project emphasizes inclusivity, accessibility, and long-term impact, providing resources for researchers, local businesses, and policy-makers to advance AI applications in combating misinformation. Prosa has developed an AI-powered chatbot to address climate misinformation. The platform's website is available at faktaiklim.prosa.ai, and the chatbot can be accessed via Telegram (Fakta Iklim Bot), with open-source code available on GitHub. User guides are provided in four languages: Indonesian, Minangkabau, Balinese, and Bugis.</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://huggingface.co/prosa-text</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Climate Action, Natural Language Processing</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Dataset, Use-Case</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Bappenas (https://www.bappenas.go.id/), Prosa AI (https://prosa.ai/)</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>The data for this project is fully open-sourced and can be accessed through Hugging Face.
+ ● License: CC BY-SA 4.0
+ ● Data Type: Tabular
+ ● Key Variables: Climate disinformation classification, topic categorization, language distribution (Bahasa Indonesia and regional languages: Minangkabau, Balinese, Buginese)
+ ● Format: CSV
+ ● Data Collection Period: Over 3 months, covering diverse misinformation cases in climate-related domains
+ Data collection involved web crawling and inputs from local communities and experts, using sources like government websites, news articles, and scientific literature. Annotations by trained linguists and marginalized community members followed strict guidelines for consistency. The datasets are formatted for easy integration with AI tools.</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Processed Data and Pretrained Models:
+ Use the multilingual datasets and pre-trained models (IndoBERT, IndoBERTNusa) to detect climate misinformation. The processed dataset can be accessed here: Processed Data
+ Code for AI Models:
+ Access the GitHub repository containing scripts for preprocessing datasets, fine-tuning language models, and training disinformation classifiers. These can be customized for various applications.
+ Application Deployment:
+ The resulting models are integrated into platforms like Kominfo's Anti-Hoax portal and social media crawling APIs. Additionally, a chatbot leveraging these AI models is available to verify climate-related information in real-time. The chatbot and models are publicly accessible via APIs to support further innovation and integration by developers.</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>You can leverage AI models and datasets to develop or enhance applications to address climate misinformation and advance public education. These resources can be adapted to new languages, regions, or even other misinformation topics, such as health or political issues. Combining the datasets with additional sources, like satellite imagery or weather data, could lead to innovative AI applications, including real-time fact-checking tools or misinformation monitoring dashboards. Researchers and developers can also use the models to benchmark against other datasets or refine methodologies, unlocking opportunities for both academic and commercial advancements.
+ These tools can be integrated into platforms like government portals or social media moderation systems to maximize impact. Interactive educational applications, such as gamified platforms or public learning modules, could further engage communities. Collaboration with stakeholders—including government agencies, NGOs, and private companies—can help scale the tools, secure funding, and drive wider adoption. Through partnerships and expanded deployment, this project can contribute to fostering critical awareness and combating misinformation effectively.</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>NLP</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>HCSA: High Carbon Stock Mapping in Southeast Asia</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Indonesien</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
           <t>Forest Forward I: Using AI to map carbon-rich Forests to Combat Climate Change and Protect Livelihoods in Indonesia (High Carbon Stock Approach)</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>This project focuses on creating validated, open-source High Carbon Stock (HCS) forest maps for Indonesia using an AI-driven approach. It adopts the HCS classification system to identify forests suitable for conservation versus sustainable development:
  • High, Medium, and Low-Density Forests (Conservation Priority): Forests with closed or patchy canopies, rich biodiversity, and carbon storage.
@@ -1812,33 +1894,33 @@
  The maps integrate field data, satellite imagery, and AI to assist policymakers, NGOs, and businesses in making data-driven decisions for sustainable land-use planning and conservation. Stakeholders can use the outputs for spatial planning, reducing greenhouse gas emissions, and implementing "no deforestation" commitments. The High Carbon Stock Approach (HCSA) project was nominated for the prestigious UN SDG Game Changer award – Category 2: Planet – Innovation for our climate and environment “Artificial Intelligence Meets Jungle/ Forest Forward.</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>https://huggingface.co/datasets/HCSA/HCSA_Indonesia_Forest_Plot_Data_2023</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr">
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr">
         <is>
           <t>Climate Action</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="I27" t="inlineStr">
         <is>
           <t>Use-Case, Dataset</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
+      <c r="J27" t="inlineStr">
         <is>
           <t>Geospatial</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>Indonesia’s Ministry of National Development Planning (Bappenas), JKPP https://jkpp.org/, [HCSA](https://highcarbonstock.org/public-consultation/), [EcoVision Lab](https://www.spacehub.uzh.ch/en/research-areas/earth-observation/EcoVision-Lab.html)</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Bappenas (https://www.bappenas.go.id/), JKPP (https://jkpp.org/), HCSA (https://highcarbonstock.org/public-consultation/), EcoVision Lab (https://www.spacehub.uzh.ch/en/research-areas/earth-observation/EcoVision-Lab.html)</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
         <is>
           <t>The finalized HCS dataset and maps are available on Hugging Face HCSA/Forest_Plot_Data_2023, and Global Forest Watch.
  • License: Open-source (CC BY 4.0) 
@@ -1851,7 +1933,7 @@
  The data adheres to FAIR (Findable, Accessible, Interoperable, Reusable) principles and includes anonymization measures to protect sensitive information.</t>
         </is>
       </c>
-      <c r="M26" t="inlineStr">
+      <c r="M27" t="inlineStr">
         <is>
           <t>Processed Data:
  Field measurements (e.g., biomass and tree species) were combined with Sentinel-2 imagery and NASA GEDI lidar to enhance map accuracy. The resulting geospatial data includes classifications of High Carbon Stock forests and other land-use categories.
@@ -1861,44 +1943,10 @@
  Validated HCS maps are deployed on Google Earth Engine and Global Forest Watch for conservation planning and policy support, with an ODK-based mobile app under development for offline data collection. The project integrates FPIC (Free, Prior, and Informed Consent) principles throughout, ensuring community involvement and respect for land rights in data collection and mapping.</t>
         </is>
       </c>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>Computer Vision</t>
-        </is>
-      </c>
-      <c r="P26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Text data collection Indonesia</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Indonesien</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Text data collection for 3 regional languages</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr">
         <is>
-          <t>NLP</t>
+          <t>Computer Vision</t>
         </is>
       </c>
       <c r="P27" t="inlineStr"/>
@@ -1906,7 +1954,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Use case development Indonesia</t>
+          <t>Text data collection Indonesia</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1915,69 +1963,21 @@
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Climate Disinformation in Local Indonesian Languages</t>
-        </is>
-      </c>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>This AI application is about developing an AI-based system to tackle climate misinformation in Indonesia, focusing on creating accurate and accessible information tools. The initiative aims to build a multilingual disinformation detection system, covering Bahasa Indonesia and over 10,6 million words and 21 million words translation from Minangkabau, Balinese, and Buginese to classify and verify climate-related content. The application supports stakeholders, including government agencies, NGOs, and communities, in countering false narratives, promoting awareness, and enabling evidence-based decision-making. The AI outcomes include open-access datasets, disinformation, and topic classification models, a user-friendly website, and a chatbot. These tools empower users to identify climate misinformation, enhance public literacy, and foster collaboration for sustainable climate actions. The project emphasizes inclusivity, accessibility, and long-term impact, providing resources for researchers, local businesses, and policy-makers to advance AI applications in combating misinformation. Prosa has developed an AI-powered chatbot to address climate misinformation. The platform's website is available at faktaiklim.prosa.ai, and the chatbot can be accessed via Telegram (Fakta Iklim Bot), with open-source code available on GitHub. User guides are provided in four languages: Indonesian, Minangkabau, Balinese, and Bugis.</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>https://huggingface.co/prosa-text</t>
-        </is>
-      </c>
+          <t>Text data collection for 3 regional languages</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Climate Action, Natural Language Processing</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>Dataset, Use-Case</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>Karlina Octaviany (GIZ), Ruth Schmidt (GIZ), Indonesia’s Ministry of National Development Planning (Bappenas), Prosa AI</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>The data for this project is fully open-sourced and can be accessed through Hugging Face.
- ● License: CC BY-SA 4.0
- ● Data Type: Tabular
- ● Key Variables: Climate disinformation classification, topic categorization, language distribution (Bahasa Indonesia and regional languages: Minangkabau, Balinese, Buginese)
- ● Format: CSV
- ● Data Collection Period: Over 3 months, covering diverse misinformation cases in climate-related domains
- Data collection involved web crawling and inputs from local communities and experts, using sources like government websites, news articles, and scientific literature. Annotations by trained linguists and marginalized community members followed strict guidelines for consistency. The datasets are formatted for easy integration with AI tools.</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>Processed Data and Pretrained Models:
- Use the multilingual datasets and pre-trained models (IndoBERT, IndoBERTNusa) to detect climate misinformation. The processed dataset can be accessed here: Processed Data
- Code for AI Models:
- Access the GitHub repository containing scripts for preprocessing datasets, fine-tuning language models, and training disinformation classifiers. These can be customized for various applications.
- Application Deployment:
- The resulting models are integrated into platforms like Kominfo's Anti-Hoax portal and social media crawling APIs. Additionally, a chatbot leveraging these AI models is available to verify climate-related information in real-time. The chatbot and models are publicly accessible via APIs to support further innovation and integration by developers.</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>You can leverage AI models and datasets to develop or enhance applications to address climate misinformation and advance public education. These resources can be adapted to new languages, regions, or even other misinformation topics, such as health or political issues. Combining the datasets with additional sources, like satellite imagery or weather data, could lead to innovative AI applications, including real-time fact-checking tools or misinformation monitoring dashboards. Researchers and developers can also use the models to benchmark against other datasets or refine methodologies, unlocking opportunities for both academic and commercial advancements.
- These tools can be integrated into platforms like government portals or social media moderation systems to maximize impact. Interactive educational applications, such as gamified platforms or public learning modules, could further engage communities. Collaboration with stakeholders—including government agencies, NGOs, and private companies—can help scale the tools, secure funding, and drive wider adoption. Through partnerships and expanded deployment, this project can contribute to fostering critical awareness and combating misinformation effectively.</t>
-        </is>
-      </c>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr">
         <is>
           <t>NLP</t>
@@ -2616,7 +2616,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>South Africa Crop Type Competition</t>
+          <t>ML4EO for Precision Agriculture</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2627,32 +2627,24 @@
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
         <is>
-          <t>South Africa Crop Type Competition</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr"/>
+          <t>Enabling geo-scientists to use Machine Learning for Precision Agriculture of geospatial data</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Field data collected on agricultural farm land (crops) with raw datasets + applied use cases of classification of land use cover using ML (based on individual projects presented)</t>
+        </is>
+      </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>https://beta.source.coop/repositories/radiantearth/south-africa-crops-competition/description/</t>
+          <t>TBC Jonas N</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>Climate Action, Agriculture</t>
-        </is>
-      </c>
+      <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>Tabular</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>[Radiant Earth](https://radiant.earth/)</t>
-        </is>
-      </c>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr"/>
@@ -2662,7 +2654,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ML4EO for Precision Agriculture</t>
+          <t>NLP grant Localising Common Voice for South African Languages</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2673,34 +2665,54 @@
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Enabling geo-scientists to use Machine Learning for Precision Agriculture of geospatial data</t>
+          <t>Making voice data available in all official languages of South Africa as a digital public good - Voices of Mzansi</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Field data collected on agricultural farm land (crops) with raw datasets + applied use cases of classification of land use cover using ML (based on individual projects presented)</t>
+          <t>Univ of Stellenbosch Grant (Febe de Wet) - Voices of Mzansi project / localise SA local languages on Mozilla CV platform</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>TBC Jonas N</t>
+          <t>https://commonvoice.mozilla.org/de/languages</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
-      <c r="J46" t="inlineStr"/>
-      <c r="K46" t="inlineStr"/>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Natural Language Processing</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Prof Febe de Wet</t>
+        </is>
+      </c>
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr"/>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>NLP</t>
+        </is>
+      </c>
       <c r="P46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>NLP grant Localising Common Voice for South African Languages</t>
+          <t>South Africa Crop Type Competition</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2711,54 +2723,42 @@
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Making voice data available in all official languages of South Africa as a digital public good - Voices of Mzansi</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>Univ of Stellenbosch Grant (Febe de Wet) - Voices of Mzansi project / localise SA local languages on Mozilla CV platform</t>
-        </is>
-      </c>
+          <t>South Africa Crop Type Competition</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>https://commonvoice.mozilla.org/de/languages</t>
+          <t>https://beta.source.coop/repositories/radiantearth/south-africa-crops-competition/description/</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Natural Language Processing</t>
-        </is>
-      </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>Dataset</t>
-        </is>
-      </c>
+          <t>Climate Action, Agriculture</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Text</t>
+          <t>Tabular</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Prof Febe de Wet</t>
+          <t>Radiant Earth (https://radiant.earth/)</t>
         </is>
       </c>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr"/>
       <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>NLP</t>
-        </is>
-      </c>
+      <c r="O47" t="inlineStr"/>
       <c r="P47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ML-based site identification for MiniGrids in Uganda</t>
+          <t>Croppie Coffee Yield Prediction</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2769,87 +2769,41 @@
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Electrification Dashboard for Ugandan government - help to find the best energy sources for villages in Uganda</t>
+          <t>Croppie- helping smallholder coffee producers to plan sales, get loans, and trace coffee - AI powered coffee yield prediction</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>This web application is a decision support tool. It is built as a prototype for a large-scale decision support tool for determining electrification strategies for different geographical areas. Currently implemented in Lamwo district electrification.</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr"/>
+          <t>Croppie is a digital platform that integrates yield estimation functionality with agronomic advice and farm data management. The basic user interface is provided through a mobile application. Croppie’s core functionality is to allow for AI-supported coffee yield estimation. This is done by guiding a selective sampling for a statistical yield estimation service based on branch count and coffee branch picture taking, alongside the integration of additional data provided by the user.</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>https://huggingface.co/datasets/rgautroncgiar/croppie_coffee_ug</t>
+        </is>
+      </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://lamwo-electrification-demo.vercel.app/</t>
+          <t>https://huggingface.co/rgautroncgiar/croppie_coffee_ug</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Climate Action</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr"/>
+          <t>Agriculture, Climate Action</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Use-Case with Business Model</t>
+        </is>
+      </c>
       <c r="J48" t="inlineStr"/>
-      <c r="K48" t="inlineStr"/>
-      <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>Computer Vision</t>
-        </is>
-      </c>
-      <c r="P48" t="inlineStr"/>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>Croppie Coffee Yield Prediction</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Uganda</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Croppie- helping smallholder coffee producers to plan sales, get loans, and trace coffee - AI powered coffee yield prediction</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>Croppie is a digital platform that integrates yield estimation functionality with agronomic advice and farm data management. The basic user interface is provided through a mobile application. Croppie’s core functionality is to allow for AI-supported coffee yield estimation. This is done by guiding a selective sampling for a statistical yield estimation service based on branch count and coffee branch picture taking, alongside the integration of additional data provided by the user.</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>https://huggingface.co/datasets/rgautroncgiar/croppie_coffee_ug</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>https://huggingface.co/rgautroncgiar/croppie_coffee_ug</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Agriculture, Climate Action</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>Use-Case with Business Model</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr"/>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>CIAT, Producers Direct, M-Omolumisa</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr">
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Croppie (https://croppie.org/#contact), Producers Direct (https://producersdirect.org/), M-Omolumisa, CIAT</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
         <is>
           <t>The Data is fully open-sourced and can be accessed on Hugging Face
  • License: CC BY SA 4.0
@@ -2860,7 +2814,7 @@
  The data was collected over the span of 1.5 years covering different crop cycles between 2022 and 2024. The Data Collection was conducted by Alliance Bioversity &amp; CIAT and M-Omolumisa via on-the-ground visits of the farms.</t>
         </is>
       </c>
-      <c r="M49" t="inlineStr">
+      <c r="M48" t="inlineStr">
         <is>
           <t>Processed Data:
  The dataset is made of a mix of Arabica and Robusta coffee tree parts (with and without a background isolation element) with individual bounding boxes around all coffee cherries. These RGB pictures were on-farm collected with smartphones with the collaboration of smallholder farmers. 
@@ -2872,11 +2826,69 @@
  The dataset/model can be used for automated cherry count or coffee ripeness assessment.</t>
         </is>
       </c>
-      <c r="N49" t="inlineStr">
+      <c r="N48" t="inlineStr">
         <is>
           <t>Instead of manual cherry counts (the traditional approach to harvest estimation), pictures of the coffee branches are used to automate this task. The coffee harvest on a plot level is estimated by processing pictures through AI-supported image recognition software along with a manual branch count (= tree level estimation) and a tree-per-ha estimation (or recall data) (scaling to plot level). Thus, Croppie serves as a central system for managing yield data at the farmer level. It also provides the option to share this data with external users; with for example cooperatives having the possibility to feed information from the application in an integrated database of their member’s performance and farm characteristics, provided they obtained prior consent to do so. This would then scale the Croppie system to have an aggregated data view of multiple users in a region, e.g. as a cooperative level dashboard.</t>
         </is>
       </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>Computer Vision</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Scaling ML-based site identification for MiniGrids Uganda</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Uganda</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Finding good spots for decentralized green energy grids in Uganda I - AI based site identification for MiniGrids</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Moving towards scaling of the MiniGrid prototype</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>https://github.com/SunbirdAI/lamwo-electrification-project/tree/main</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>https://github.com/SunbirdAI/lamwo-electrification-project/tree/main</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Climate Action</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Use-Case</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Geospatial</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
       <c r="O49" t="inlineStr">
         <is>
           <t>Computer Vision</t>
@@ -2887,7 +2899,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Scaling ML-based site identification for MiniGrids Uganda</t>
+          <t>ML-based site identification for MiniGrids in Uganda</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2898,22 +2910,18 @@
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Finding good spots for decentralized green energy grids in Uganda I - AI based site identification for MiniGrids</t>
+          <t>Electrification Dashboard for Ugandan government - help to find the best energy sources for villages in Uganda</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Moving towards scaling of the MiniGrid prototype</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>https://github.com/SunbirdAI/lamwo-electrification-project/tree/main</t>
-        </is>
-      </c>
+          <t>This web application is a decision support tool. It is built as a prototype for a large-scale decision support tool for determining electrification strategies for different geographical areas. Currently implemented in Lamwo district electrification.</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://github.com/SunbirdAI/lamwo-electrification-project/tree/main</t>
+          <t>https://lamwo-electrification-demo.vercel.app/</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2921,16 +2929,8 @@
           <t>Climate Action</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>Use-Case</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>Geospatial</t>
-        </is>
-      </c>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr"/>
@@ -2956,7 +2956,7 @@
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Predicting and Correcting Solar Irradiance wih unbiased AI Models in East Africa</t>
+          <t>Finding good spots for decentralized green energy grids in Uganda II - Measuring Solar Irradiance wih unbiased AI Models</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>

</xml_diff>

<commit_message>
Revert "new data fetch"
This reverts commit 83831f894976ea80bd15d9c3db6ced989fead04a.
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X101"/>
+  <dimension ref="A1:X91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1362,11 +1362,7 @@
           <t>Masakhane Grant (Local Subsidy)</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Maybe catchy project title?</t>
-        </is>
-      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
           <t>Supporting Pan-African research Networks on natural language processing (Masakhane)</t>
@@ -1374,15 +1370,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Supporting the Masakhane network to develop an NLP data catalogue, handbook, datasheets, and governance models for management of catalogue, see https://www.masakhane.io/
-1.  Development of an African NLP Data Collection Handbook
-This handbook will compile learnings and recommendations from the language data collection experiences of those amongst our ranks and others within our network who have undertaken this work. 
-2. Management and Maintenance of an AfricaNLP data catalogue 
-Lanfrica is a platform that catalogues and links African language resources to make localised African content accessible and discoverable with a centralised African NLP catalogue.
-3. Case Studies on IP, Copyright and Fair Use in Africa
-Researchers often approach 'access to data' requests, for research purposes, with a western mindset, which assumes fair use. However the Masakhane approach requires engaging data owners, sharing intentions and asking for permission, a process for which some templates exist. The case study explores partnership models that would enable us to access data and these can also be documented. Here, a minimum of 5 case studies detail how our Masakhane approach have unfolded with several data owners in Africa.
-4. Tooling for Data Statements
-Datasheets for datasets is a tool for documenting the datasets used for training and evaluating machine learning models. Datasheets intend to increase dataset transparency and facilitate better communication between dataset creators and dataset consumers (e.g., those using datasets to train machine learning models). </t>
+          <t>Supporting the Masakhane network to develop an NLP data catalogue, handbook, datasheets, and governance models for management of catalogue, see https://www.masakhane.io/</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
@@ -1430,20 +1418,15 @@
           <t>Mozilla Community Licence Project</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>TBC</t>
-        </is>
-      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Our language, our data: Co-creating equitable governance models with African language communities - language dataset creatd: Dhuluo</t>
+          <t>Our language, our data: Co-creating equitable governance models with African language communities</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Mozilla Foundation seeks to select and support a community (group of language speakers who would like to collectively create or enhance a text and audio dataset for their  language), to experiment with a governance structure for this dataset that suits their particular needs. 
-This project will enable language communities to leverage governance tools (such as licenses) that center their needs and context, and have them be more accessible and widely used. Over the period of the project, the goal is to have a particular language community, or small group of them, piloting a novel, community-centered license on the Common Voice platform, as a proof of concept that can then be replicated and adapted</t>
+          <t>Our language, our data: Co-creating equitable governance models with African language communities</t>
         </is>
       </c>
       <c r="F13" t="inlineStr"/>
@@ -4485,13 +4468,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Enabling geo-scientists to use Machine Learning for Precision Agriculture of geospatial data 
-Some new options:
-From Maps to Meals: ML for Precision Ag"
-Geo-Intelligence for Greener Fields
-Geo-science Meets Smart Farming
-Tilling the Datafields
-Earth to Algorithm</t>
+          <t>Enabling geo-scientists to use Machine Learning for Precision Agriculture of geospatial data</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4501,19 +4478,18 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Development and implementation of a training program to enable practitioners in the field of Earth Observation in South Africa to use machine learning. 
-Field data collected on small holder agricultural farm land (crops) with raw datasets + applied use cases of classification of land use cover using ML (based on individual projects presented)</t>
+          <t>Field data collected on small holder agricultural farm land (crops) with raw datasets + applied use cases of classification of land use cover using ML (based on individual projects presented)</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1P_bW8Is1Qa1HJIznVbq_vsQwH3ejKUa5?usp=drive_link</t>
+          <t>https://drive.google.com/drive/folders/1X0u_BkiGGOn5ZRjrX9DIr6XT9yueoD3K?usp=drive_link</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Agriculture, Climate Action, Disaster Risk Reduction Management</t>
+          <t>Agriculture, Climate Action</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
@@ -4523,12 +4499,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>1. Satellite-Based Data: Sentinel-1 (SAR),  
-Sentinel-2 (optical), Sentinel-2 (Vis),  Sentinel-2 (imagery)
-2. Drone-Based Data: Drone imagery, multispectral
-3. Ground-Based / In-situ Data
-4. Spectral Data Types: Hyperspectral, Thermal IR
-Data Formats: Images, Tabular</t>
+          <t>Images, Tabular</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4541,26 +4512,14 @@
           <t>South Africa</t>
         </is>
       </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>Field-level reflectance, chlorophyll-related vegetation indices (VIs), Spectral response to stress; Sentinel-2, NIR bands, Low-res images, spectral variability for phosphorus deficiency &amp; MSV, Spatial mapping of weeds vs. crops, Red-edge based chlorophyll estimates, Red-edge bands, REIP indices, Thermal + multispectral image fusion, Temporal NDVI, vegetation change monitoring, Crop separability via bands 7, 8, 8A, 11, Correlation of VIs to LAI</t>
-        </is>
-      </c>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>see sub-projects</t>
-        </is>
-      </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>see sub-projects</t>
-        </is>
-      </c>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr">
         <is>
           <t xml:space="preserve">Powered by:  Move Beyond Consulting
-Implementing partners: MBC, WITS, CSIR, ARC
+Implementing partners: WITS, CSIR, ARC
 Catalyzed by: FAIR Forward - AI for All
 Financed by: BMZ </t>
         </is>
@@ -4575,16 +4534,8 @@
           <t>ML4EO</t>
         </is>
       </c>
-      <c r="T52" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1JMDhPAwVfS80qSFerU7f7jRhuKG05OFi?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="U52" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1R7iawHmEnTRJu_kmoR1iz26aii15ELIT?usp=drive_link</t>
-        </is>
-      </c>
+      <c r="T52" t="inlineStr"/>
+      <c r="U52" t="inlineStr"/>
       <c r="V52" t="inlineStr"/>
       <c r="W52" t="inlineStr"/>
       <c r="X52" t="inlineStr"/>
@@ -4592,35 +4543,34 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>ui_52_1</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr"/>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Tomato Crushers</t>
-        </is>
-      </c>
+          <t>ui_53</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>NLP grant Localising Common Voice for South African Languages</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Detecting and Assessing Tomato Stress using ASD Measurements and Drone Data: The Case of Project Munei Holding Investments, Ha-Mphaila, Makhado Local Municipality</t>
+          <t>Making voice data available in all official languages of South Africa as a digital public good - Voices of Mzansi</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Investigates methods for detecting and assessing stress in tomato plants using ASD measurements and drone data, focusing on Project Munei Holding Investment in Ha-Mphaila, Limpopo
-</t>
+          <t>Univ of Stellenbosch Grant (Febe de Wet) - Voices of Mzansi project / localise SA local languages on Mozilla CV platform</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1P_bW8Is1Qa1HJIznVbq_vsQwH3ejKUa5?usp=drive_link</t>
+          <t>https://commonvoice.mozilla.org/de/languages</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Agriculture, Disaster Risk Reduction Management / SDG 2 (Zero Hunger)</t>
+          <t>Natural Language Processing</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -4630,12 +4580,12 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Hyperspectral, UAV imagery, SPAD, Images, Tabular</t>
+          <t>Text</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Dr Meena Lysko</t>
+          <t>Prof Febe de Wet</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4643,50 +4593,25 @@
           <t>South Africa</t>
         </is>
       </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>Field-level reflectance, chlorophyll-related vegetation indices (VIs)</t>
-        </is>
-      </c>
-      <c r="N53" t="inlineStr">
-        <is>
-          <t>Random Forest; used for stress classification; Software/Application: Random Forest + UAV analytics</t>
-        </is>
-      </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>Train RF using spectral indices; cost includes UAV flights, ASD rentals; open-source RF models or GEE usable</t>
-        </is>
-      </c>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Powered by:  Move Beyond Consulting
-Implementing partners: MBC, WITS, CSIR, ARC
-Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ </t>
-        </is>
-      </c>
-      <c r="R53" t="inlineStr">
-        <is>
-          <t>Gladness Khoza and Chuma Majova</t>
-        </is>
-      </c>
+          <t>Powered by:  University of Stellenbosch 
+Catalyzed by: South African Digital Language Resources (SADILAR), FAIR Forward - AI for All, Mozilla Foundation, UNESCO decade of indigenous languages
+Financed by: BMZ</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr"/>
       <c r="S53" t="inlineStr">
         <is>
-          <t>ML4EO</t>
-        </is>
-      </c>
-      <c r="T53" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1XAzVlTGTc1TuXb10h67WDmuU91k2c2BP/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="U53" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1t3KiZiEQFprZMb8AYI01HrbSsSrfUwlb/view?usp=drive_link</t>
-        </is>
-      </c>
+          <t>NLP</t>
+        </is>
+      </c>
+      <c r="T53" t="inlineStr"/>
+      <c r="U53" t="inlineStr"/>
       <c r="V53" t="inlineStr"/>
       <c r="W53" t="inlineStr"/>
       <c r="X53" t="inlineStr"/>
@@ -4694,49 +4619,57 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>ui_52_2</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr"/>
+          <t>ui_54</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>South Africa Crop Type Competition</t>
+        </is>
+      </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Artificial Intelligence for Maize (AIM)</t>
+          <t>Crop Type Identification from Satellite Imagery in Western Cape, South Africa</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Characterizing Maize Stress Using UAV Remote Sensing: A Machine Learning Approach</t>
+          <t>Crop Type Identification from Satellite Imagery in Western Cape, South Africa</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Investigates the use of remote sensing and machine learning to characterize maize stress in the Limpopo Province, South Africa. The study concludes that integrating field spectra and remotely sensed reflectance provides valuable information for maize stress investigation, supporting the development of mitigation and prevention strategies to ensure food security.</t>
+          <t>This dataset and AI model was produced as part of the Radiant Earth Spot the Crop Challenge (https://zindi.africa/hackathons/radiant-earth-spot-the-crop-hackathon). The objective of the competition was to create a machine learning model to classify fields by crop type from images collected during the growing season by the Sentinel-2 and Sentinel-1 satellites.</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1P_bW8Is1Qa1HJIznVbq_vsQwH3ejKUa5?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr"/>
+          <t>https://beta.source.coop/repositories/radiantearth/south-africa-crops-competition/description/</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>https://github.com/radiantearth/spot-the-crop-challenge</t>
+        </is>
+      </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Agriculture, Disaster Risk Reduction Management/ SDG 2 (Zero Hunger)</t>
+          <t>Climate Action, Agriculture</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>Dataset</t>
+          <t>Dataset --&gt; Pilot</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Satellite + field spectroscopy,  Images, Tabular</t>
+          <t>Tabular</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Dr Meena Lysko</t>
+          <t>Radiant Earth (ml@radiant.earth), Western Cape Department of Agriculture</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -4746,46 +4679,46 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>Spectral response to stress; Sentinel-2, NIR bands</t>
+          <t>The dataset contains a time-series of satellite imagery and labels for crop type that have been collected through aerial and ground survey. Labels are derived from the survey conducted by the Western Cape Department of Agriculture. Satellite data including multispectral Sentinel-2 are then matched with corresponding labels.</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>Random Forest, SVM; Software/Application: Sentinel-2 + field spectral data</t>
+          <t xml:space="preserve">This repository contains the winning models from the Zindi data competition "Spot the Crop" in which participants used time series of Sentinel-2 multispectral imagery as input for crop type classification.
+</t>
         </is>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Access Sentinel-2 (free); field spectrometer needed for calibration</t>
-        </is>
-      </c>
-      <c r="P54" t="inlineStr"/>
+          <t>The agricultural sector makes a substantial contribution to GDP and livelihoods across the developing world. However, regular and reliable agricultural data remains difficult and expensive to collect on the ground. As a result, policy-makers usually don’t have access to updated data for implementing policies or supporting farmers. Earth observation satellites provide a wealth of multispectral image data that can be used for developing agricultural monitoring tools. These tools support farmers and policy-makers across Africa and the developing world. With this dataset and AI model you can use time-series of Sentinel-2 multi-spectral data to classify crops in the Western Cape of South Africa.</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>CC-BY 4.0</t>
+        </is>
+      </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Powered by:  Move Beyond Consulting
-Implementing partners: MBC, WITS, CSIR, ARC
+          <t>Powered by: Radiant Earth, Western Cape Department of Agriculture
 Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ </t>
+Financed by: BMZ</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
         <is>
-          <t>Gerhardt Botha and Mikka Parag</t>
+          <t>Philipp Olbrich</t>
         </is>
       </c>
       <c r="S54" t="inlineStr">
         <is>
-          <t>ML4EO</t>
-        </is>
-      </c>
-      <c r="T54" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1XkSwcY0fmPmleRxfekkoOcBvF7kuAHFX/view?usp=drive_link</t>
-        </is>
-      </c>
+          <t>Computer Vision</t>
+        </is>
+      </c>
+      <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1cMBiijRJUyz8MVAuudrDnK2kkxbnoT6J/view?usp=drive_link</t>
+          <t>https://zindi.africa/competitions/radiant-earth-spot-the-crop-challenge</t>
         </is>
       </c>
       <c r="V54" t="inlineStr"/>
@@ -4795,1074 +4728,65 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>ui_52_3</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr"/>
+          <t>ui_55</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Croppie Coffee Yield Prediction</t>
+        </is>
+      </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Stress Detectors</t>
+          <t>Precision Farming Simplified: Croppie’s AI-Powered Agronomic Advisor</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Monitoring Zea Mays Disease Stress using Drone data and Machine Learning Techniques, and Advising on Possible Causes and Solutions</t>
+          <t>Croppie- helping smallholder coffee producers to plan sales, get loans, and trace coffee - AI powered coffee yield prediction</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Assesses the capabilities of Earth observation and machine learning algorithms, specifically Random Forest and Support Vector Machines, in detecting maize disease stress using drone data. The study was conducted on a small-scale farm in Limpopo, South Africa, focusing on healthy maize, maize with streak virus, and maize with phosphorus deficiency. </t>
+          <t>Unpredictable weather conditions and price fluctuations pose major challenges for coffee farmers in Uganda. The platform and app 'Croppie' supports them with targeted cultivation recommendations and precise crop forecasts—using AI-supported image recognition of coffee plants. As a digital public good based on open-source technology, it can be adapted and further developed locally. The basic user interface is provided through a mobile application. Croppie’s core functionality is to allow for AI-supported coffee yield estimation. This is done by guiding a selective sampling for a statistical yield estimation service based on branch count and coffee branch picture taking, alongside the integration of additional data provided by the user.</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1P_bW8Is1Qa1HJIznVbq_vsQwH3ejKUa5?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr"/>
+          <t>https://huggingface.co/datasets/rgautroncgiar/croppie_coffee_ug</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>https://huggingface.co/rgautroncgiar/croppie_coffee_ug</t>
+        </is>
+      </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Agriculture, Disaster Risk Reduction Management / SDG 2 (Zero Hunger)</t>
+          <t>Agriculture, Climate Action</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>Dataset</t>
+          <t>Dataset --&gt; Pilot --&gt; Use-Case --&gt; Use-Case with Business Model</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Drone imagery, hyperspectral, Images, Tabular</t>
+          <t>Tabular</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Dr Meena Lysko</t>
+          <t>Croppie (https://croppie.org/#contact), Producers Direct (https://producersdirect.org/), M-Omolumisa, CIAT</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Uganda</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
-        <is>
-          <t>Low-res images, spectral variability for phosphorus deficiency &amp; MSV</t>
-        </is>
-      </c>
-      <c r="N55" t="inlineStr">
-        <is>
-          <t>Random Forest, SVM; &lt;80% accuracy; Software/Application: Drone + ML (RF, SVM)</t>
-        </is>
-      </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>Requires high-quality imagery, better spectral resolution; GEE and drone access recommended</t>
-        </is>
-      </c>
-      <c r="P55" t="inlineStr"/>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Powered by:  Move Beyond Consulting
-Implementing partners: MBC, WITS, CSIR, ARC
-Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ </t>
-        </is>
-      </c>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>Khanyisa Mpisane and Kanya Xongo</t>
-        </is>
-      </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>ML4EO</t>
-        </is>
-      </c>
-      <c r="T55" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1CV_nkCyPYt9ecxWyEcmEguYpLh9DFb2V/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="U55" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/13tu-8UnI1FYk7DLkI_Z1qmprWW3EWlfp/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="V55" t="inlineStr"/>
-      <c r="W55" t="inlineStr"/>
-      <c r="X55" t="inlineStr"/>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>ui_52_4</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr"/>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Weeties</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Precision weed mapping and management in tomato fields using drone data in support of small-holder farming</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>Drone high-resolution images were used with a semi-automated random forest (RF) classifier algorithm in Google Earth Engine to classify bare soil, weeds, and tomatoes. The findings can serve as a reference for agricultural researchers and advise farmers on crop management, potentially reducing costs and herbicide use.</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1P_bW8Is1Qa1HJIznVbq_vsQwH3ejKUa5?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>Agriculture, Disaster Risk Reduction Management / SDG 2 (Zero Hunger), SDG 12 (Responsible Consumption)</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>Dataset</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>Drone data, RGB/multispectral, Images, Tabular</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>Dr Meena Lysko</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>South Africa</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>Spatial mapping of weeds vs. crops</t>
-        </is>
-      </c>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t>Random Forest; high training accuracy (89%); Software/Application: GEE + Random Forest</t>
-        </is>
-      </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>Drone + GEE for processing; reduce herbicide usage</t>
-        </is>
-      </c>
-      <c r="P56" t="inlineStr"/>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Powered by:  Move Beyond Consulting
-Implementing partners: MBC, WITS, CSIR, ARC
-Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ </t>
-        </is>
-      </c>
-      <c r="R56" t="inlineStr">
-        <is>
-          <t>Martin Chari and Makgabo Mashala</t>
-        </is>
-      </c>
-      <c r="S56" t="inlineStr">
-        <is>
-          <t>ML4EO</t>
-        </is>
-      </c>
-      <c r="T56" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1hyiQSbdMyB0O5BYR8fl31BfyvRzRIlP8/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="U56" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1uFKAZ9CCniykTKRSsh2-nxKW2f3Wkpbb/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="V56" t="inlineStr"/>
-      <c r="W56" t="inlineStr"/>
-      <c r="X56" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>ui_52_5</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr"/>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Chlorophyll-Busters</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Estimation of chlorophyll contents of crops (maize and tomato) using Sentinel-2 and drone data by applying Random Forest machine learning algorithm: A case study of the Ha-Mphaila farming area of South Africa</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>Explores using the Random Forest Regression (RFR) machine learning algorithm with Sentinel-2 and drone imagery to estimate relative chlorophyll values in tomato and maize crops within South Africa's Ha-Mphaila farming area. The research concludes that both Sentinel-2 imagery (10m and 20m spatial resolution) and high-resolution drone images are valuable for rapidly assessing crop chlorophyll content across significant areas, offering useful insights for precision agriculture.</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1P_bW8Is1Qa1HJIznVbq_vsQwH3ejKUa5?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>Agriculture, Disaster Risk Reduction Management / SDG 2 (Zero Hunger)</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>Dataset</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>Drone + Sentinel-2, Vis,  Images, Tabular</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>Dr Meena Lysko</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>South Africa</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>Red-edge based chlorophyll estimates</t>
-        </is>
-      </c>
-      <c r="N57" t="inlineStr">
-        <is>
-          <t>Random Forest Regression; Software/Application: Sentinel-2 + drone + RF</t>
-        </is>
-      </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>Sentinel free; drone + SPAD sensor may be costly unless shared</t>
-        </is>
-      </c>
-      <c r="P57" t="inlineStr"/>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Powered by:  Move Beyond Consulting
-Implementing partners: MBC, WITS, CSIR, ARC
-Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ </t>
-        </is>
-      </c>
-      <c r="R57" t="inlineStr">
-        <is>
-          <t>Cindy Viviers and Dr. Abraham Thomas</t>
-        </is>
-      </c>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>ML4EO</t>
-        </is>
-      </c>
-      <c r="T57" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1KVUM-JLYg6CY-B3WmVj4-puKacJvg8_x/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="U57" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1dfgcycIgFy7SKUHJcZ2qFERbQTbehxVh/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="V57" t="inlineStr"/>
-      <c r="W57" t="inlineStr"/>
-      <c r="X57" t="inlineStr"/>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>ui_52_6</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr"/>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>The Agro-Innovators</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Evaluating the Performance of Machine Learning Algorithms for Estimating Chlorophyll Content of Tomatoes with Unmanned Aerial Vehicle (UAV)-Based Data.</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Evaluates the performance of machine learning algorithms for estimating chlorophyll content in tomatoes using Sentinel-2 satellite data. </t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1P_bW8Is1Qa1HJIznVbq_vsQwH3ejKUa5?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr"/>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>Agriculture, Disaster Risk Reduction Management / SDG 2 (Zero Hunger)</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>Dataset</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>Sentinel-2 imagery, SPAD chlorophyll,  Images, Tabular</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>Dr Meena Lysko</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>South Africa</t>
-        </is>
-      </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>Red-edge bands, REIP indices</t>
-        </is>
-      </c>
-      <c r="N58" t="inlineStr">
-        <is>
-          <t>Bagging, Boosting, ANN, SVR; Software/Application: Chlorophyll estimation ML</t>
-        </is>
-      </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>Train model on SPAD + satellite indices; uses open-source ML tools</t>
-        </is>
-      </c>
-      <c r="P58" t="inlineStr"/>
-      <c r="Q58" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Powered by:  Move Beyond Consulting
-Implementing partners: MBC, WITS, CSIR, ARC
-Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ </t>
-        </is>
-      </c>
-      <c r="R58" t="inlineStr">
-        <is>
-          <t>Sisipho Ngebe and Afika Singano</t>
-        </is>
-      </c>
-      <c r="S58" t="inlineStr">
-        <is>
-          <t>ML4EO</t>
-        </is>
-      </c>
-      <c r="T58" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1kugMpKasnb5_7XJkRj3jnAQw8retlV4W/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="U58" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1QYB5PBhQVaDQ1J-YP0ZfOAsLXznla_Kr/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="V58" t="inlineStr"/>
-      <c r="W58" t="inlineStr"/>
-      <c r="X58" t="inlineStr"/>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>ui_52_7</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Agro-thermography</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Integration of ground-based vegetation parameters, thermal infrared and UAV multispectral data for mapping of crop canopy temperature</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>Explores the integration of ground-based vegetation parameters, thermal infrared data from handheld cameras, and UAV multispectral data to map crop canopy temperature at high resolution. The research, conducted at the Ha-Mphaila irrigation scheme in Limpopo, South Africa, focused on tomato crops.</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1P_bW8Is1Qa1HJIznVbq_vsQwH3ejKUa5?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr"/>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>Agriculture, Disaster Risk Reduction Management / SDG 13 (Climate Action), SDG 2 (Zero Hunger)</t>
-        </is>
-      </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>Dataset</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>Thermal IR + Multispectral UAV + field data,  Images, Tabular</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>Dr Meena Lysko</t>
-        </is>
-      </c>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>South Africa</t>
-        </is>
-      </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>Thermal + multispectral image fusion</t>
-        </is>
-      </c>
-      <c r="N59" t="inlineStr">
-        <is>
-          <t>Regression model; canopy temperature estimation; Software/Application: Thermal camera + UAV + regression models</t>
-        </is>
-      </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>Needs UAV &amp; thermal cam; costly setup unless shared or borrowed</t>
-        </is>
-      </c>
-      <c r="P59" t="inlineStr"/>
-      <c r="Q59" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Powered by:  Move Beyond Consulting
-Implementing partners: MBC, WITS, CSIR, ARC
-Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ </t>
-        </is>
-      </c>
-      <c r="R59" t="inlineStr">
-        <is>
-          <t>Dr. Mohamed Ahmed and Phumlani Zwane</t>
-        </is>
-      </c>
-      <c r="S59" t="inlineStr">
-        <is>
-          <t>ML4EO</t>
-        </is>
-      </c>
-      <c r="T59" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1MOSiW0BIzqwK2YMEp1dCcIzItgLm8wR8/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="U59" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1GMpDiMlY-wYXTB6T5woikRpFbgQ21hhp/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="V59" t="inlineStr"/>
-      <c r="W59" t="inlineStr"/>
-      <c r="X59" t="inlineStr"/>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>ui_52_8</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr"/>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Discovering Agriculture Insurance</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Remote Sensing and Machine Learning Applications in Agriculture Index Insurance (AII)</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>Investigates how remote sensing and machine learning can be used to improve Agricultural Index Insurance (AII) for smallholder farmers in South Africa, who often lack access to affordable insurance.  Key recommendations include supporting further research and development in these areas and implementing educational campaigns to build farmer trust and awareness of index insurance benefits.</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1P_bW8Is1Qa1HJIznVbq_vsQwH3ejKUa5?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr"/>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>Insurance &amp; Agriculture / SDG 13 (Climate action), SDG 2 (Zero Hunger)</t>
-        </is>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>Dataset</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>Drone, Sentinel imagery, chlorophyll &amp; NDVI indices,  Images, Tabular</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>Dr Meena Lysko</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>South Africa</t>
-        </is>
-      </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>Temporal NDVI, vegetation change monitoring</t>
-        </is>
-      </c>
-      <c r="N60" t="inlineStr">
-        <is>
-          <t>ML for index-insurance mapping; Software/Application: Dynamic World + ML</t>
-        </is>
-      </c>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>Integrate indices into insurance design; Sentinel-2 free; ML libraries (e.g., Scikit-learn)</t>
-        </is>
-      </c>
-      <c r="P60" t="inlineStr"/>
-      <c r="Q60" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Powered by:  Move Beyond Consulting
-Implementing partners: MBC, WITS, CSIR, ARC
-Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ </t>
-        </is>
-      </c>
-      <c r="R60" t="inlineStr">
-        <is>
-          <t>Shereen Francis and Yashoda Maharaj</t>
-        </is>
-      </c>
-      <c r="S60" t="inlineStr">
-        <is>
-          <t>ML4EO</t>
-        </is>
-      </c>
-      <c r="T60" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1LHAaaDSYSNbBAaeVdmBFlpecX_ntVEKf/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="U60" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1rGoapVNyVsVwMxDfBrRfdVoyRCpjwnIy/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="V60" t="inlineStr"/>
-      <c r="W60" t="inlineStr"/>
-      <c r="X60" t="inlineStr"/>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>ui_52_9</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr"/>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>SAR Busters</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Crop type mapping in Mphaila irrigation scheme in Vhembe District in Limpopo Province</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Explores the use of Sentinel-1 and Sentinel-2 satellite data for crop type mapping in smallholder farming areas. The study focuses on improving classification accuracy by identifying optimal spectral bands and evaluating machine learning algorithms like decision tree and random forest classifiers
-</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1P_bW8Is1Qa1HJIznVbq_vsQwH3ejKUa5?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr"/>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>Agriculture/ SDG 2 (Zero Hunger)</t>
-        </is>
-      </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>Dataset</t>
-        </is>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>Sentinel-1 (SAR), Sentinel-2 (optical),  Images, Tabular</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>Dr Meena Lysko</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>South Africa</t>
-        </is>
-      </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>Crop separability via bands 7, 8, 8A, 11</t>
-        </is>
-      </c>
-      <c r="N61" t="inlineStr">
-        <is>
-          <t>Decision Tree, Random Forest; Software/Application: Crop mapping using ML</t>
-        </is>
-      </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>Sentinel data free; GEE platform usable</t>
-        </is>
-      </c>
-      <c r="P61" t="inlineStr"/>
-      <c r="Q61" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Powered by:  Move Beyond Consulting
-Implementing partners: MBC, WITS, CSIR, ARC
-Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ </t>
-        </is>
-      </c>
-      <c r="R61" t="inlineStr">
-        <is>
-          <t>Dleme Tswai and Dr. Theunis Morgenthal</t>
-        </is>
-      </c>
-      <c r="S61" t="inlineStr">
-        <is>
-          <t>ML4EO</t>
-        </is>
-      </c>
-      <c r="T61" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1mjjI5knaWJqjOQURj7OKfKxMbMDEmvEH/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="U61" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1c54f9Lh5IV8T_XLrlf_8ItAitrBEjTVZ/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="V61" t="inlineStr"/>
-      <c r="W61" t="inlineStr"/>
-      <c r="X61" t="inlineStr"/>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>ui_52_10</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr"/>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>The internet of Crops (IOC)</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Leaf Area Index Estimation of Tomato Crops in Sub-Humid Regions Based On Sentinel 2 Imagery and Random Forest Regression Ensemble</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>Investigates the use of Sentinel-2 satellite imagery and a random forest (RF) machine learning algorithm to estimate the Leaf Area Index (LAI) of tomato crops in the Ha-Mphaila irrigation scheme, Limpopo Province, South Africa. The research aimed to determine key wavebands and vegetation indices for LAI estimation, compare the performance of RF models with stepwise multiple linear regression (SMLR) models, and map the spatial distribution of LAI.</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1P_bW8Is1Qa1HJIznVbq_vsQwH3ejKUa5?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr"/>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>Agriculture/ SDG 2 (Zero Hunger)</t>
-        </is>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>Dataset</t>
-        </is>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>Sentinel-2 + LAI ground truth,  Images, Tabular</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>Dr Meena Lysko</t>
-        </is>
-      </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>South Africa</t>
-        </is>
-      </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>Correlation of VIs to LAI</t>
-        </is>
-      </c>
-      <c r="N62" t="inlineStr">
-        <is>
-          <t>Random Forest Regression; Software/Application: Sentinel-2 + RF</t>
-        </is>
-      </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>Free Sentinel-2 + fieldwork required; ML code free (e.g., Python)</t>
-        </is>
-      </c>
-      <c r="P62" t="inlineStr"/>
-      <c r="Q62" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Powered by:  Move Beyond Consulting
-Implementing partners: MBC, WITS, CSIR, ARC
-Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ </t>
-        </is>
-      </c>
-      <c r="R62" t="inlineStr">
-        <is>
-          <t>Frederick Mashao and Dr. Olufemi Olayiwola</t>
-        </is>
-      </c>
-      <c r="S62" t="inlineStr">
-        <is>
-          <t>ML4EO</t>
-        </is>
-      </c>
-      <c r="T62" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1ZmDPVVb2SLxrWDE7LnCIl87_Wse4f8oK/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="U62" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1rqnCZTZ2b4MSp9C0nkFhU3A1Xhk4CwIe/view?usp=drive_link</t>
-        </is>
-      </c>
-      <c r="V62" t="inlineStr"/>
-      <c r="W62" t="inlineStr"/>
-      <c r="X62" t="inlineStr"/>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>ui_53</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>NLP grant Localising Common Voice for South African Languages</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Speaking Data, Speaking Home 
-Mzansi Speaks
-Our voices, our code
-Voices of Mzansi (project title)</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Making voice data available in all official languages of South Africa as a digital public good - Voices of Mzansi</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>Univ of Stellenbosch Grant (Febe de Wet) - Voices of Mzansi project aimed to get South Africa's languages launched on the Mozilla Common Voice platform1. To achieve this aim the Common Voice website had to be translated from English into the other official languages and at least 5 000 sentences had to be collected for each language. The collected sentences have to be available in the open domain under CC-0 licensing. Once a languages is launched, the sentences are used as prompts for speech data collection through the Common Voice platform.</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>https://commonvoice.mozilla.org/de/languages</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr"/>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>Natural Language Processing</t>
-        </is>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>Dataset</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>Prof Febe de Wet</t>
-        </is>
-      </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>South Africa</t>
-        </is>
-      </c>
-      <c r="M63" t="inlineStr"/>
-      <c r="N63" t="inlineStr"/>
-      <c r="O63" t="inlineStr"/>
-      <c r="P63" t="inlineStr">
-        <is>
-          <t>CC-O</t>
-        </is>
-      </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>Powered by:  University of Stellenbosch 
-Catalyzed by: South African Digital Language Resources (SADILAR), FAIR Forward - AI for All, Mozilla Foundation, UNESCO decade of indigenous languages
-Financed by: BMZ</t>
-        </is>
-      </c>
-      <c r="R63" t="inlineStr"/>
-      <c r="S63" t="inlineStr">
-        <is>
-          <t>NLP</t>
-        </is>
-      </c>
-      <c r="T63" t="inlineStr"/>
-      <c r="U63" t="inlineStr">
-        <is>
-          <t>Mozilla CVP</t>
-        </is>
-      </c>
-      <c r="V63" t="inlineStr"/>
-      <c r="W63" t="inlineStr"/>
-      <c r="X63" t="inlineStr"/>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>ui_54</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>South Africa Crop Type Competition</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Spot the Crop</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Crop Type Identification from Satellite Imagery in Western Cape, South Africa</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>This dataset and AI model was produced as part of the Radiant Earth Spot the Crop Challenge (https://zindi.africa/hackathons/radiant-earth-spot-the-crop-hackathon). The objective of the competition was to create a machine learning model to classify fields by crop type from images collected during the growing season by the Sentinel-2 and Sentinel-1 satellites.</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>https://beta.source.coop/repositories/radiantearth/south-africa-crops-competition/description/</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>https://github.com/radiantearth/spot-the-crop-challenge</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>Climate Action, Agriculture</t>
-        </is>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>Dataset --&gt; Pilot</t>
-        </is>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>Tabular</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>Radiant Earth (ml@radiant.earth), Western Cape Department of Agriculture</t>
-        </is>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>South Africa</t>
-        </is>
-      </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>The dataset contains a time-series of satellite imagery and labels for crop type that have been collected through aerial and ground survey. Labels are derived from the survey conducted by the Western Cape Department of Agriculture. Satellite data including multispectral Sentinel-2 are then matched with corresponding labels.</t>
-        </is>
-      </c>
-      <c r="N64" t="inlineStr">
-        <is>
-          <t xml:space="preserve">This repository contains the winning models from the Zindi data competition "Spot the Crop" in which participants used time series of Sentinel-2 multispectral imagery as input for crop type classification.
-</t>
-        </is>
-      </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>The agricultural sector makes a substantial contribution to GDP and livelihoods across the developing world. However, regular and reliable agricultural data remains difficult and expensive to collect on the ground. As a result, policy-makers usually don’t have access to updated data for implementing policies or supporting farmers. Earth observation satellites provide a wealth of multispectral image data that can be used for developing agricultural monitoring tools. These tools support farmers and policy-makers across Africa and the developing world. With this dataset and AI model you can use time-series of Sentinel-2 multi-spectral data to classify crops in the Western Cape of South Africa.</t>
-        </is>
-      </c>
-      <c r="P64" t="inlineStr">
-        <is>
-          <t>CC-BY 4.0</t>
-        </is>
-      </c>
-      <c r="Q64" t="inlineStr">
-        <is>
-          <t>Powered by: Radiant Earth, Western Cape Department of Agriculture
-Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ</t>
-        </is>
-      </c>
-      <c r="R64" t="inlineStr">
-        <is>
-          <t>Philipp Olbrich</t>
-        </is>
-      </c>
-      <c r="S64" t="inlineStr">
-        <is>
-          <t>Computer Vision</t>
-        </is>
-      </c>
-      <c r="T64" t="inlineStr"/>
-      <c r="U64" t="inlineStr">
-        <is>
-          <t>https://zindi.africa/competitions/radiant-earth-spot-the-crop-challenge</t>
-        </is>
-      </c>
-      <c r="V64" t="inlineStr"/>
-      <c r="W64" t="inlineStr"/>
-      <c r="X64" t="inlineStr"/>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>ui_55</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Croppie Coffee Yield Prediction</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Precision Farming Simplified: Croppie’s AI-Powered Agronomic Advisor</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Croppie- helping smallholder coffee producers to plan sales, get loans, and trace coffee - AI powered coffee yield prediction</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>Unpredictable weather conditions and price fluctuations pose major challenges for coffee farmers in Uganda. The platform and app 'Croppie' supports them with targeted cultivation recommendations and precise crop forecasts—using AI-supported image recognition of coffee plants. As a digital public good based on open-source technology, it can be adapted and further developed locally. The basic user interface is provided through a mobile application. Croppie’s core functionality is to allow for AI-supported coffee yield estimation. This is done by guiding a selective sampling for a statistical yield estimation service based on branch count and coffee branch picture taking, alongside the integration of additional data provided by the user.</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>https://huggingface.co/datasets/rgautroncgiar/croppie_coffee_ug</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>https://huggingface.co/rgautroncgiar/croppie_coffee_ug</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>Agriculture, Climate Action</t>
-        </is>
-      </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>Dataset --&gt; Pilot --&gt; Use-Case --&gt; Use-Case with Business Model</t>
-        </is>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>Tabular</t>
-        </is>
-      </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>Croppie (https://croppie.org/#contact), Producers Direct (https://producersdirect.org/), M-Omolumisa, CIAT</t>
-        </is>
-      </c>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>Uganda</t>
-        </is>
-      </c>
-      <c r="M65" t="inlineStr">
         <is>
           <t>The Data is fully open-sourced and can be accessed on Hugging Face
  • License: CC BY SA 4.0
@@ -5873,7 +4797,7 @@
  The data was collected over the span of 1.5 years covering different crop cycles between 2022 and 2024. The Data Collection was conducted by Alliance Bioversity &amp; CIAT and M-Omolumisa via on-the-ground visits of the farms.</t>
         </is>
       </c>
-      <c r="N65" t="inlineStr">
+      <c r="N55" t="inlineStr">
         <is>
           <t>Processed Data:
  The dataset is made of a mix of Arabica and Robusta coffee tree parts (with and without a background isolation element) with individual bounding boxes around all coffee cherries. These RGB pictures were on-farm collected with smartphones with the collaboration of smallholder farmers. 
@@ -5885,25 +4809,589 @@
  The dataset/model can be used for automated cherry count or coffee ripeness assessment.</t>
         </is>
       </c>
-      <c r="O65" t="inlineStr">
+      <c r="O55" t="inlineStr">
         <is>
           <t>Instead of manual cherry counts (the traditional approach to harvest estimation), pictures of the coffee branches are used to automate this task. The coffee harvest on a plot level is estimated by processing pictures through AI-supported image recognition software along with a manual branch count (= tree level estimation) and a tree-per-ha estimation (or recall data) (scaling to plot level). Thus, Croppie serves as a central system for managing yield data at the farmer level. It also provides the option to share this data with external users; with for example cooperatives having the possibility to feed information from the application in an integrated database of their member’s performance and farm characteristics, provided they obtained prior consent to do so. This would then scale the Croppie system to have an aggregated data view of multiple users in a region, e.g. as a cooperative level dashboard.</t>
         </is>
       </c>
-      <c r="P65" t="inlineStr"/>
-      <c r="Q65" t="inlineStr">
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr">
         <is>
           <t>Powered by:  
 Catalyzed by: FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
       </c>
+      <c r="R55" t="inlineStr"/>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>Computer Vision</t>
+        </is>
+      </c>
+      <c r="T55" t="inlineStr"/>
+      <c r="U55" t="inlineStr"/>
+      <c r="V55" t="inlineStr"/>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>ui_56</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Scaling ML-based site identification for MiniGrids Uganda</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Bridging the Energy Gap: Machine Learning Applications in Uganda's Rural Electrification</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Finding good spots for decentralized green energy grids in Uganda I - AI based site identification for MiniGrids</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>The Site Identification tool is an AI-driven tool to enhance renewable energy planning. This tool utilizes machine learning and satellite imagery to identify optimal sites for renewable energy deployment, particularly in remote regions. A successful pilot in Lamwo District demonstrated its potential to improve energy access by recommending suitable electrification strategies for villages. This initiative aligns with Uganda’s National Electrification Strategy, which seeks to connect 10 million households to the most optimal energy source by 2030.</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>https://github.com/SunbirdAI/lamwo-electrification-project/tree/main</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>https://lamwo-electrification-demo-47qi01med-evie-8s-projects.vercel.app/</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Climate Action</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Dataset --&gt; Pilot --&gt; Use-Case</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Geospatial</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Sunbird.ai
+Ernest Mwebaze &lt;emwebaze@sunbird.ai&gt;</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Uganda</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-• Data Type: Geospatial and tabular 
+• Key Variables: Solar Irradiance,Biomass Resources,Wind Speed and Consistency,Biomass Resources,Hydropower Potential,
+Population Density,Proximity to Existing Grids,Road Networks,Land Availability,Protected Areas,Cost of Energy Delivery
+• The data adheres to FAIR (Findable, Accessible, Interoperable, Reusable) principles and includes anonymization measures to protect sensitive information.
+</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This web application is a decision support tool. It is built as a prototype for a large-scale decision support tool for determining electrification strategies for different geographical areas. Currently implemented in Lamwo district electrification. </t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>This web application is a prototype decision support tool designed to guide electrification strategies across various geographic areas. It offers an initial village-level assessment through a color-coded map, with the legend explaining each category. Users can explore detailed analyses at the village level—the smallest unit for assessing electrification needs. The tool evaluates both demand and supply factors and suggests the most suitable energy solutions, including biomass, wind, solar home systems, mini-grids, or grid extension. It is intended to support government officials, energy sector stakeholders, and development partners in making informed renewable energy decisions.</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>Powered by:  
+Catalyzed by: FAIR Forward - AI for All
+Financed by: BMZ</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr"/>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>Computer Vision</t>
+        </is>
+      </c>
+      <c r="T56" t="inlineStr"/>
+      <c r="U56" t="inlineStr"/>
+      <c r="V56" t="inlineStr"/>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>ui_57</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>ML-based site identification for MiniGrids in Uganda</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Electrification Dashboard for Ugandan government - help to find the best energy sources for villages in Uganda</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>COVERED WITH ENTRY ABOVE. This web application is a decision support tool. It is built as a prototype for a large-scale decision support tool for determining electrification strategies for different geographical areas. Currently implemented in Lamwo district electrification.</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Climate Action</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Uganda</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>Powered by:  
+Catalyzed by: FAIR Forward - AI for All
+Financed by: BMZ</t>
+        </is>
+      </c>
+      <c r="R57" t="inlineStr"/>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>Computer Vision</t>
+        </is>
+      </c>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="inlineStr"/>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>ui_58</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Development of Unbiased AI Models for Solar Irradiance Uganda</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Finding good spots for decentralized green energy grids in Uganda II - Measuring Solar Irradiance with unbiased AI Models</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Machine Learning models to predict unbiased solar irradiance for a given location in sub-saharan Africa</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>https://irradianceportal.me/; https://github.com/Marconi-Lab/Solar_irradiation; https://github.com/Marconi-Lab/Irradiation_Portal</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Climate Action</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Numerical meteorolgical data</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Uganda</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>Key variable: Solar Irradiation</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>Powered by:  
+Catalyzed by: FAIR Forward - AI for All
+Financed by: BMZ</t>
+        </is>
+      </c>
+      <c r="R58" t="inlineStr"/>
+      <c r="S58" t="inlineStr"/>
+      <c r="T58" t="inlineStr"/>
+      <c r="U58" t="inlineStr"/>
+      <c r="V58" t="inlineStr"/>
+      <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>ui_59</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>NLP Use Case Strengthening relevance of Auditing reports in Uganda</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>NLP Use Case Strengthening relevance of Auditing reports in Uganda</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>This activity is requested by Uganda country office and paid for by them. It is run by the DSC and FF is supporting with technical input. No own funds needed for this.</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Climate Action</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Uganda</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr"/>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>Powered by:  
+Catalyzed by: FAIR Forward - AI for All
+Financed by: BMZ</t>
+        </is>
+      </c>
+      <c r="R59" t="inlineStr"/>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>NLP</t>
+        </is>
+      </c>
+      <c r="T59" t="inlineStr"/>
+      <c r="U59" t="inlineStr"/>
+      <c r="V59" t="inlineStr"/>
+      <c r="W59" t="inlineStr"/>
+      <c r="X59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>ui_60</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Datasets marking Personal Identifiable Information (PII) and Gender Bias</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Datasets marking Personal Identifiable Information (PII) and Gender Bias</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>This dataset contains annotated sentences with personally identifiable information (PII) in Luganda, Lumasaba, Hausa, and Kanuri. These four languages span Central and Eastern Uganda, Nigeria, Ghana, and Northern Cameroon. The team collected 3,000 sentences for both Kanuri and Hausa, 5,000 for Lumasaba, and 4,000 for Luganda. Potential use cases for these datasets include named entity recognition (NER), text classification, privacy-preserving data analysis and research, language modeling, machine translation, and linguistic research.
+ The team aimed to curate a dataset that is gender inclusive, and their work highlighted the need for standardized guidelines for annotating low-resourced languages. Having these guidelines would help to avoid common pitfalls and errors when labeling text data in these low-resource languages.</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>https://dataverse.harvard.edu/citation?persistentId=doi:10.7910/DVN/CGHWZE</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Climate Action, Natural Language Processing</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Andrew Katumba - Makerere University (katumba@mak.ac.ug)</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Uganda,Kenya,Nigeria</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr"/>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>Powered by:  
+Catalyzed by: Lacuna-Fund / Meridian &amp;  FAIR Forward - AI for All
+Financed by: BMZ</t>
+        </is>
+      </c>
+      <c r="R60" t="inlineStr"/>
+      <c r="S60" t="inlineStr"/>
+      <c r="T60" t="inlineStr"/>
+      <c r="U60" t="inlineStr"/>
+      <c r="V60" t="inlineStr"/>
+      <c r="W60" t="inlineStr"/>
+      <c r="X60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>ui_61</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Ecuadorian Dataset on Access, Demand, &amp; Availability of Electricity Supply</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>ESPOL University</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Ecuador</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr"/>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
+      <c r="Q61" t="inlineStr"/>
+      <c r="R61" t="inlineStr"/>
+      <c r="S61" t="inlineStr"/>
+      <c r="T61" t="inlineStr"/>
+      <c r="U61" t="inlineStr"/>
+      <c r="V61" t="inlineStr"/>
+      <c r="W61" t="inlineStr"/>
+      <c r="X61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>ui_62</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Artificial Intelligence for Energy Access (AI4EA)</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Reiner Lemoine Institut gGmbH (RLI)</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Benin,Ghana,Niger,Togo</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr"/>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr"/>
+      <c r="R62" t="inlineStr"/>
+      <c r="S62" t="inlineStr"/>
+      <c r="T62" t="inlineStr"/>
+      <c r="U62" t="inlineStr"/>
+      <c r="V62" t="inlineStr"/>
+      <c r="W62" t="inlineStr"/>
+      <c r="X62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>ui_63</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Residential Energy and Weather Dataset (REWD) of Pakistan</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Lahore University of Management Sciences (LUMS)</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Pakistan</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr"/>
+      <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
+      <c r="Q63" t="inlineStr"/>
+      <c r="R63" t="inlineStr"/>
+      <c r="S63" t="inlineStr"/>
+      <c r="T63" t="inlineStr"/>
+      <c r="U63" t="inlineStr"/>
+      <c r="V63" t="inlineStr"/>
+      <c r="W63" t="inlineStr"/>
+      <c r="X63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>ui_64</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Datasets for transportation impact evaluation</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Fundación Despacio,World Resources Institute,Fundación Despacio</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Colombia</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="inlineStr"/>
+      <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
+      <c r="Q64" t="inlineStr"/>
+      <c r="R64" t="inlineStr"/>
+      <c r="S64" t="inlineStr"/>
+      <c r="T64" t="inlineStr"/>
+      <c r="U64" t="inlineStr"/>
+      <c r="V64" t="inlineStr"/>
+      <c r="W64" t="inlineStr"/>
+      <c r="X64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>ui_65</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Machine learning training data for continental Ecuador and Galapagos</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Fundacion Ecociencia</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Ecuador</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr"/>
+      <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
       <c r="R65" t="inlineStr"/>
-      <c r="S65" t="inlineStr">
-        <is>
-          <t>Computer Vision</t>
-        </is>
-      </c>
+      <c r="S65" t="inlineStr"/>
       <c r="T65" t="inlineStr"/>
       <c r="U65" t="inlineStr"/>
       <c r="V65" t="inlineStr"/>
@@ -5913,98 +5401,39 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>ui_56</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Scaling ML-based site identification for MiniGrids Uganda</t>
-        </is>
-      </c>
+          <t>ui_66</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Bridging the Energy Gap: Machine Learning Applications in Uganda's Rural Electrification</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Finding good spots for decentralized green energy grids in Uganda I - AI based site identification for MiniGrids</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>The Site Identification tool is an AI-driven tool to enhance renewable energy planning. This tool utilizes machine learning and satellite imagery to identify optimal sites for renewable energy deployment, particularly in remote regions. A successful pilot in Lamwo District demonstrated its potential to improve energy access by recommending suitable electrification strategies for villages. This initiative aligns with Uganda’s National Electrification Strategy, which seeks to connect 10 million households to the most optimal energy source by 2030.</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>https://github.com/SunbirdAI/lamwo-electrification-project/tree/main</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>https://lamwo-electrification-demo-47qi01med-evie-8s-projects.vercel.app/</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>Climate Action</t>
-        </is>
-      </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>Dataset --&gt; Pilot --&gt; Use-Case</t>
-        </is>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>Geospatial</t>
-        </is>
-      </c>
+          <t>Forest carbon sequestration in the Congo Basin</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
       <c r="K66" t="inlineStr">
         <is>
-          <t>Sunbird.ai
-Ernest Mwebaze &lt;emwebaze@sunbird.ai&gt;</t>
+          <t>World Resources Institute</t>
         </is>
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Uganda</t>
-        </is>
-      </c>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t xml:space="preserve">-• Data Type: Geospatial and tabular 
-• Key Variables: Solar Irradiance,Biomass Resources,Wind Speed and Consistency,Biomass Resources,Hydropower Potential,
-Population Density,Proximity to Existing Grids,Road Networks,Land Availability,Protected Areas,Cost of Energy Delivery
-• The data adheres to FAIR (Findable, Accessible, Interoperable, Reusable) principles and includes anonymization measures to protect sensitive information.
-</t>
-        </is>
-      </c>
-      <c r="N66" t="inlineStr">
-        <is>
-          <t xml:space="preserve">This web application is a decision support tool. It is built as a prototype for a large-scale decision support tool for determining electrification strategies for different geographical areas. Currently implemented in Lamwo district electrification. </t>
-        </is>
-      </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>This web application is a prototype decision support tool designed to guide electrification strategies across various geographic areas. It offers an initial village-level assessment through a color-coded map, with the legend explaining each category. Users can explore detailed analyses at the village level—the smallest unit for assessing electrification needs. The tool evaluates both demand and supply factors and suggests the most suitable energy solutions, including biomass, wind, solar home systems, mini-grids, or grid extension. It is intended to support government officials, energy sector stakeholders, and development partners in making informed renewable energy decisions.</t>
-        </is>
-      </c>
+          <t>Cameroon,DRC</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr"/>
       <c r="P66" t="inlineStr"/>
-      <c r="Q66" t="inlineStr">
-        <is>
-          <t>Powered by:  
-Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ</t>
-        </is>
-      </c>
+      <c r="Q66" t="inlineStr"/>
       <c r="R66" t="inlineStr"/>
-      <c r="S66" t="inlineStr">
-        <is>
-          <t>Computer Vision</t>
-        </is>
-      </c>
+      <c r="S66" t="inlineStr"/>
       <c r="T66" t="inlineStr"/>
       <c r="U66" t="inlineStr"/>
       <c r="V66" t="inlineStr"/>
@@ -6014,57 +5443,39 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>ui_57</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>ML-based site identification for MiniGrids in Uganda</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>Electrification Dashboard for Ugandan government - help to find the best energy sources for villages in Uganda</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>COVERED WITH ENTRY ABOVE. This web application is a decision support tool. It is built as a prototype for a large-scale decision support tool for determining electrification strategies for different geographical areas. Currently implemented in Lamwo district electrification.</t>
-        </is>
-      </c>
+          <t>ui_67</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>GEO Indigenous Alliance</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>Climate Action</t>
-        </is>
-      </c>
+      <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr"/>
-      <c r="K67" t="inlineStr"/>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>GEO Indigenous Alliance</t>
+        </is>
+      </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Uganda</t>
+          <t>Ecuador,Kenya</t>
         </is>
       </c>
       <c r="M67" t="inlineStr"/>
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="inlineStr"/>
       <c r="P67" t="inlineStr"/>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>Powered by:  
-Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ</t>
-        </is>
-      </c>
+      <c r="Q67" t="inlineStr"/>
       <c r="R67" t="inlineStr"/>
-      <c r="S67" t="inlineStr">
-        <is>
-          <t>Computer Vision</t>
-        </is>
-      </c>
+      <c r="S67" t="inlineStr"/>
       <c r="T67" t="inlineStr"/>
       <c r="U67" t="inlineStr"/>
       <c r="V67" t="inlineStr"/>
@@ -6074,63 +5485,37 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>ui_58</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Development of Unbiased AI Models for Solar Irradiance Uganda</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>Finding good spots for decentralized green energy grids in Uganda II - Measuring Solar Irradiance with unbiased AI Models</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>Machine Learning models to predict unbiased solar irradiance for a given location in sub-saharan Africa</t>
-        </is>
-      </c>
+          <t>ui_68</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Ivorian mangroves and carbon stock</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>https://irradianceportal.me/; https://github.com/Marconi-Lab/Solar_irradiation; https://github.com/Marconi-Lab/Irradiation_Portal</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>Climate Action</t>
-        </is>
-      </c>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr"/>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>Numerical meteorolgical data</t>
-        </is>
-      </c>
-      <c r="K68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>data354</t>
+        </is>
+      </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Uganda</t>
-        </is>
-      </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>Key variable: Solar Irradiation</t>
-        </is>
-      </c>
+          <t>Cote d'Ivoire</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr"/>
       <c r="N68" t="inlineStr"/>
       <c r="O68" t="inlineStr"/>
       <c r="P68" t="inlineStr"/>
-      <c r="Q68" t="inlineStr">
-        <is>
-          <t>Powered by:  
-Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ</t>
-        </is>
-      </c>
+      <c r="Q68" t="inlineStr"/>
       <c r="R68" t="inlineStr"/>
       <c r="S68" t="inlineStr"/>
       <c r="T68" t="inlineStr"/>
@@ -6142,57 +5527,39 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>ui_59</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>NLP Use Case Strengthening relevance of Auditing reports in Uganda</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>NLP Use Case Strengthening relevance of Auditing reports in Uganda</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>This activity is requested by Uganda country office and paid for by them. It is run by the DSC and FF is supporting with technical input. No own funds needed for this.</t>
-        </is>
-      </c>
+          <t>ui_69</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Reference Data Collection for Improving Land Use Change Mapping in Ghana</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>Climate Action</t>
-        </is>
-      </c>
+      <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr"/>
-      <c r="K69" t="inlineStr"/>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>Center for Remote Sensing and Geographic Information Services</t>
+        </is>
+      </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Uganda</t>
+          <t>Ghana</t>
         </is>
       </c>
       <c r="M69" t="inlineStr"/>
       <c r="N69" t="inlineStr"/>
       <c r="O69" t="inlineStr"/>
       <c r="P69" t="inlineStr"/>
-      <c r="Q69" t="inlineStr">
-        <is>
-          <t>Powered by:  
-Catalyzed by: FAIR Forward - AI for All
-Financed by: BMZ</t>
-        </is>
-      </c>
+      <c r="Q69" t="inlineStr"/>
       <c r="R69" t="inlineStr"/>
-      <c r="S69" t="inlineStr">
-        <is>
-          <t>NLP</t>
-        </is>
-      </c>
+      <c r="S69" t="inlineStr"/>
       <c r="T69" t="inlineStr"/>
       <c r="U69" t="inlineStr"/>
       <c r="V69" t="inlineStr"/>
@@ -6202,78 +5569,59 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>ui_60</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Datasets marking Personal Identifiable Information (PII) and Gender Bias</t>
-        </is>
-      </c>
+          <t>ui_70</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Datasets marking Personal Identifiable Information (PII) and Gender Bias</t>
+          <t>Remote sensing and weather dataset for improved reforestation monitoring</t>
         </is>
       </c>
       <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>This dataset contains annotated sentences with personally identifiable information (PII) in Luganda, Lumasaba, Hausa, and Kanuri. These four languages span Central and Eastern Uganda, Nigeria, Ghana, and Northern Cameroon. The team collected 3,000 sentences for both Kanuri and Hausa, 5,000 for Lumasaba, and 4,000 for Luganda. Potential use cases for these datasets include named entity recognition (NER), text classification, privacy-preserving data analysis and research, language modeling, machine translation, and linguistic research.
- The team aimed to curate a dataset that is gender inclusive, and their work highlighted the need for standardized guidelines for annotating low-resourced languages. Having these guidelines would help to avoid common pitfalls and errors when labeling text data in these low-resource languages.</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>https://dataverse.harvard.edu/citation?persistentId=doi:10.7910/DVN/CGHWZE</t>
-        </is>
-      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr"/>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>Climate Action, Natural Language Processing</t>
-        </is>
-      </c>
+      <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Andrew Katumba - Makerere University (katumba@mak.ac.ug)</t>
+          <t>Dedan Kimathi University of Technology,Data Science Africa</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Uganda,Kenya,Nigeria</t>
+          <t>Kenya</t>
         </is>
       </c>
       <c r="M70" t="inlineStr"/>
       <c r="N70" t="inlineStr"/>
       <c r="O70" t="inlineStr"/>
       <c r="P70" t="inlineStr"/>
-      <c r="Q70" t="inlineStr">
-        <is>
-          <t>Powered by:  
-Catalyzed by: Lacuna-Fund / Meridian &amp;  FAIR Forward - AI for All
-Financed by: BMZ</t>
-        </is>
-      </c>
+      <c r="Q70" t="inlineStr"/>
       <c r="R70" t="inlineStr"/>
       <c r="S70" t="inlineStr"/>
       <c r="T70" t="inlineStr"/>
       <c r="U70" t="inlineStr"/>
       <c r="V70" t="inlineStr"/>
       <c r="W70" t="inlineStr"/>
-      <c r="X70" t="inlineStr"/>
+      <c r="X70" t="inlineStr">
+        <is>
+          <t>Is this from Lacuna? (DB)</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>ui_61</t>
+          <t>ui_71</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Ecuadorian Dataset on Access, Demand, &amp; Availability of Electricity Supply</t>
+          <t>DATASETS FOR PREDICTION OF LAND USE/COVER CHANGES IN UGANDA</t>
         </is>
       </c>
       <c r="D71" t="inlineStr"/>
@@ -6285,12 +5633,12 @@
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr">
         <is>
-          <t>ESPOL University</t>
+          <t>Makerere University</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Uganda</t>
         </is>
       </c>
       <c r="M71" t="inlineStr"/>
@@ -6309,13 +5657,13 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>ui_62</t>
+          <t>ui_72</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Artificial Intelligence for Energy Access (AI4EA)</t>
+          <t>African Trees for Climate Resilience: A Comprehensive Database</t>
         </is>
       </c>
       <c r="D72" t="inlineStr"/>
@@ -6327,12 +5675,12 @@
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Reiner Lemoine Institut gGmbH (RLI)</t>
+          <t>University of Stellenbosch</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Benin,Ghana,Niger,Togo</t>
+          <t>Angola,DRC,Germany,Kenya,Mozambique,Nigeria,South Africa,Tanzania,United Kingdom,Zambia</t>
         </is>
       </c>
       <c r="M72" t="inlineStr"/>
@@ -6351,13 +5699,13 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>ui_63</t>
+          <t>ui_73</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Residential Energy and Weather Dataset (REWD) of Pakistan</t>
+          <t>Datasets to understand mangroves health in relationship to climate change</t>
         </is>
       </c>
       <c r="D73" t="inlineStr"/>
@@ -6369,12 +5717,12 @@
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Lahore University of Management Sciences (LUMS)</t>
+          <t>"Laboratory of Biomathematics and Forest Estimations, University of Abomey-Calavi"</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>Benin</t>
         </is>
       </c>
       <c r="M73" t="inlineStr"/>
@@ -6393,13 +5741,13 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>ui_64</t>
+          <t>ui_74</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Datasets for transportation impact evaluation</t>
+          <t>Advancing oil palm mapping with social forestry and machine learning</t>
         </is>
       </c>
       <c r="D74" t="inlineStr"/>
@@ -6411,12 +5759,12 @@
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Fundación Despacio,World Resources Institute,Fundación Despacio</t>
+          <t>RECOFTC</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="M74" t="inlineStr"/>
@@ -6435,13 +5783,13 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>ui_65</t>
+          <t>ui_75</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Machine learning training data for continental Ecuador and Galapagos</t>
+          <t>Inclusive MRV for India's Eastern Himalayas</t>
         </is>
       </c>
       <c r="D75" t="inlineStr"/>
@@ -6453,12 +5801,12 @@
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Fundacion Ecociencia</t>
+          <t>Balipara Foundation</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>India</t>
         </is>
       </c>
       <c r="M75" t="inlineStr"/>
@@ -6477,13 +5825,13 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ui_66</t>
+          <t>ui_76</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Forest carbon sequestration in the Congo Basin</t>
+          <t>Data-enabled climate shock absorbance through agroforestry (Agrof4resilience)</t>
         </is>
       </c>
       <c r="D76" t="inlineStr"/>
@@ -6495,12 +5843,12 @@
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr">
         <is>
-          <t>World Resources Institute</t>
+          <t>International Center of Insect Physiology and Ecology (ICIPE)</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Cameroon,DRC</t>
+          <t>Kenya</t>
         </is>
       </c>
       <c r="M76" t="inlineStr"/>
@@ -6519,13 +5867,13 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>ui_67</t>
+          <t>ui_77</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr">
         <is>
-          <t>GEO Indigenous Alliance</t>
+          <t>QUANTIFYING COLOMBIAN MANGROVES ABOVEGROUND BIOMASS AND CARBON CONTENT</t>
         </is>
       </c>
       <c r="D77" t="inlineStr"/>
@@ -6537,12 +5885,12 @@
       <c r="J77" t="inlineStr"/>
       <c r="K77" t="inlineStr">
         <is>
-          <t>GEO Indigenous Alliance</t>
+          <t>Centre Tecnològic de Telecomunicacions de Catalunya (CTTC)</t>
         </is>
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Ecuador,Kenya</t>
+          <t>Columbia</t>
         </is>
       </c>
       <c r="M77" t="inlineStr"/>
@@ -6561,13 +5909,13 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>ui_68</t>
+          <t>ui_78</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Ivorian mangroves and carbon stock</t>
+          <t>Phenological Dataset for Ecological Forecasting (PheDEF Project)</t>
         </is>
       </c>
       <c r="D78" t="inlineStr"/>
@@ -6579,12 +5927,12 @@
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr">
         <is>
-          <t>data354</t>
+          <t>"Department of Biological Science, School of Science, University of Energy and Natural Resources, Sunyani, Ghana"</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Cote d'Ivoire</t>
+          <t>Ghana,Netherlands</t>
         </is>
       </c>
       <c r="M78" t="inlineStr"/>
@@ -6603,41 +5951,101 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>ui_69</t>
+          <t>ui_79</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Reference Data Collection for Improving Land Use Change Mapping in Ghana</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr"/>
-      <c r="F79" t="inlineStr"/>
-      <c r="G79" t="inlineStr"/>
-      <c r="H79" t="inlineStr"/>
-      <c r="I79" t="inlineStr"/>
-      <c r="J79" t="inlineStr"/>
+          <t>Machine Translation - for Moodle LMS</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Parallel Text for machine translation in Eng-Kin; Domain-specific for Education (digital literacy)</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enabling language translation capabilities on the Moodle LMS platform, through a collaboration with Atingi; the use case explores 3 modes of translation. The first mode is navigation based, simply translating static messages such as buttons and notifications, secondly it explores full content translation, lastly, in-line translation. The project uses the NLLB-200 model for translation, other models could be experimented to explore feasibility of additional features such as QA or summarization, leveraging the plugin built by the team. </t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://huggingface.co/datasets/DigitalUmuganda/kinyarwanda-english-machine-translation-dataset;  https://huggingface.co/datasets/mbazaNLP/Kinyarwanda_English_parallel_dataset; https://huggingface.co/datasets/mbazaNLP/NMT_Education_parallel_data_en_kin; https://huggingface.co/datasets/DigitalUmuganda/kinyarwanda-english-machine-translation-dataset </t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://huggingface.co/mbazaNLP/Quantized_Nllb_Finetuned_Edu_En_Kin_8bit; https://huggingface.co/mbazaNLP/Nllb_finetuned_general_en_kin; https://huggingface.co/DigitalUmuganda/Finetuned-NLLB </t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Inclusive Education</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Center for Remote Sensing and Geographic Information Services</t>
+          <t xml:space="preserve">FAIR Forward Rwanda / Digital Umuganda </t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Ghana</t>
-        </is>
-      </c>
-      <c r="M79" t="inlineStr"/>
-      <c r="N79" t="inlineStr"/>
-      <c r="O79" t="inlineStr"/>
-      <c r="P79" t="inlineStr"/>
-      <c r="Q79" t="inlineStr"/>
-      <c r="R79" t="inlineStr"/>
-      <c r="S79" t="inlineStr"/>
+          <t>Rwanda</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>Parallel datasets can be used to finetune LLMs to specific languages or domains; the example is for English-Kinyarwanda, to improve NLLB translation performance</t>
+        </is>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Open source model NLLB-200, some variations quantized to minimize compute resource usage </t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Integrate preferred machine translation model with Moodle plugin: https://github.com/Digital-Umuganda/moodle-translate_courses . Need to update for compatibility with newer Moodle updates, this was implemented during Moodle version 3.0 </t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>Permissive</t>
+        </is>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>Atingi, Digital Umuganda, Clear Global</t>
+        </is>
+      </c>
+      <c r="R79" t="inlineStr">
+        <is>
+          <t>Isaac</t>
+        </is>
+      </c>
+      <c r="S79" t="inlineStr">
+        <is>
+          <t>NLP</t>
+        </is>
+      </c>
       <c r="T79" t="inlineStr"/>
-      <c r="U79" t="inlineStr"/>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- https://moodlemoot.org/2024/timetable/event/246/ / https://aiopeneducation.pubpub.org/pub/7npwm2su/release/5?readingCollection=06969c6d </t>
+        </is>
+      </c>
       <c r="V79" t="inlineStr"/>
       <c r="W79" t="inlineStr"/>
       <c r="X79" t="inlineStr"/>
@@ -6645,15 +6053,11 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>ui_70</t>
+          <t>ui_80</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Remote sensing and weather dataset for improved reforestation monitoring</t>
-        </is>
-      </c>
+      <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr"/>
@@ -6661,16 +6065,8 @@
       <c r="H80" t="inlineStr"/>
       <c r="I80" t="inlineStr"/>
       <c r="J80" t="inlineStr"/>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>Dedan Kimathi University of Technology,Data Science Africa</t>
-        </is>
-      </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>Kenya</t>
-        </is>
-      </c>
+      <c r="K80" t="inlineStr"/>
+      <c r="L80" t="inlineStr"/>
       <c r="M80" t="inlineStr"/>
       <c r="N80" t="inlineStr"/>
       <c r="O80" t="inlineStr"/>
@@ -6682,24 +6078,16 @@
       <c r="U80" t="inlineStr"/>
       <c r="V80" t="inlineStr"/>
       <c r="W80" t="inlineStr"/>
-      <c r="X80" t="inlineStr">
-        <is>
-          <t>Is this from Lacuna? (DB)</t>
-        </is>
-      </c>
+      <c r="X80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>ui_71</t>
+          <t>ui_81</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>DATASETS FOR PREDICTION OF LAND USE/COVER CHANGES IN UGANDA</t>
-        </is>
-      </c>
+      <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr"/>
@@ -6707,16 +6095,8 @@
       <c r="H81" t="inlineStr"/>
       <c r="I81" t="inlineStr"/>
       <c r="J81" t="inlineStr"/>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>Makerere University</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>Uganda</t>
-        </is>
-      </c>
+      <c r="K81" t="inlineStr"/>
+      <c r="L81" t="inlineStr"/>
       <c r="M81" t="inlineStr"/>
       <c r="N81" t="inlineStr"/>
       <c r="O81" t="inlineStr"/>
@@ -6733,15 +6113,11 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>ui_72</t>
+          <t>ui_82</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>African Trees for Climate Resilience: A Comprehensive Database</t>
-        </is>
-      </c>
+      <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr"/>
@@ -6749,16 +6125,8 @@
       <c r="H82" t="inlineStr"/>
       <c r="I82" t="inlineStr"/>
       <c r="J82" t="inlineStr"/>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>University of Stellenbosch</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>Angola,DRC,Germany,Kenya,Mozambique,Nigeria,South Africa,Tanzania,United Kingdom,Zambia</t>
-        </is>
-      </c>
+      <c r="K82" t="inlineStr"/>
+      <c r="L82" t="inlineStr"/>
       <c r="M82" t="inlineStr"/>
       <c r="N82" t="inlineStr"/>
       <c r="O82" t="inlineStr"/>
@@ -6775,15 +6143,11 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>ui_73</t>
+          <t>ui_83</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>Datasets to understand mangroves health in relationship to climate change</t>
-        </is>
-      </c>
+      <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr"/>
@@ -6791,16 +6155,8 @@
       <c r="H83" t="inlineStr"/>
       <c r="I83" t="inlineStr"/>
       <c r="J83" t="inlineStr"/>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>"Laboratory of Biomathematics and Forest Estimations, University of Abomey-Calavi"</t>
-        </is>
-      </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>Benin</t>
-        </is>
-      </c>
+      <c r="K83" t="inlineStr"/>
+      <c r="L83" t="inlineStr"/>
       <c r="M83" t="inlineStr"/>
       <c r="N83" t="inlineStr"/>
       <c r="O83" t="inlineStr"/>
@@ -6817,15 +6173,11 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>ui_74</t>
+          <t>ui_84</t>
         </is>
       </c>
       <c r="B84" t="inlineStr"/>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Advancing oil palm mapping with social forestry and machine learning</t>
-        </is>
-      </c>
+      <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr"/>
@@ -6833,16 +6185,8 @@
       <c r="H84" t="inlineStr"/>
       <c r="I84" t="inlineStr"/>
       <c r="J84" t="inlineStr"/>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>RECOFTC</t>
-        </is>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>Indonesia</t>
-        </is>
-      </c>
+      <c r="K84" t="inlineStr"/>
+      <c r="L84" t="inlineStr"/>
       <c r="M84" t="inlineStr"/>
       <c r="N84" t="inlineStr"/>
       <c r="O84" t="inlineStr"/>
@@ -6859,15 +6203,11 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>ui_75</t>
+          <t>ui_85</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Inclusive MRV for India's Eastern Himalayas</t>
-        </is>
-      </c>
+      <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr"/>
@@ -6875,16 +6215,8 @@
       <c r="H85" t="inlineStr"/>
       <c r="I85" t="inlineStr"/>
       <c r="J85" t="inlineStr"/>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>Balipara Foundation</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
+      <c r="K85" t="inlineStr"/>
+      <c r="L85" t="inlineStr"/>
       <c r="M85" t="inlineStr"/>
       <c r="N85" t="inlineStr"/>
       <c r="O85" t="inlineStr"/>
@@ -6901,15 +6233,11 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>ui_76</t>
+          <t>ui_86</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>Data-enabled climate shock absorbance through agroforestry (Agrof4resilience)</t>
-        </is>
-      </c>
+      <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
@@ -6917,16 +6245,8 @@
       <c r="H86" t="inlineStr"/>
       <c r="I86" t="inlineStr"/>
       <c r="J86" t="inlineStr"/>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>International Center of Insect Physiology and Ecology (ICIPE)</t>
-        </is>
-      </c>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>Kenya</t>
-        </is>
-      </c>
+      <c r="K86" t="inlineStr"/>
+      <c r="L86" t="inlineStr"/>
       <c r="M86" t="inlineStr"/>
       <c r="N86" t="inlineStr"/>
       <c r="O86" t="inlineStr"/>
@@ -6943,15 +6263,11 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>ui_77</t>
+          <t>ui_87</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>QUANTIFYING COLOMBIAN MANGROVES ABOVEGROUND BIOMASS AND CARBON CONTENT</t>
-        </is>
-      </c>
+      <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr"/>
@@ -6959,16 +6275,8 @@
       <c r="H87" t="inlineStr"/>
       <c r="I87" t="inlineStr"/>
       <c r="J87" t="inlineStr"/>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>Centre Tecnològic de Telecomunicacions de Catalunya (CTTC)</t>
-        </is>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>Columbia</t>
-        </is>
-      </c>
+      <c r="K87" t="inlineStr"/>
+      <c r="L87" t="inlineStr"/>
       <c r="M87" t="inlineStr"/>
       <c r="N87" t="inlineStr"/>
       <c r="O87" t="inlineStr"/>
@@ -6985,15 +6293,11 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>ui_78</t>
+          <t>ui_88</t>
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>Phenological Dataset for Ecological Forecasting (PheDEF Project)</t>
-        </is>
-      </c>
+      <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
@@ -7001,16 +6305,8 @@
       <c r="H88" t="inlineStr"/>
       <c r="I88" t="inlineStr"/>
       <c r="J88" t="inlineStr"/>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>"Department of Biological Science, School of Science, University of Energy and Natural Resources, Sunyani, Ghana"</t>
-        </is>
-      </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>Ghana,Netherlands</t>
-        </is>
-      </c>
+      <c r="K88" t="inlineStr"/>
+      <c r="L88" t="inlineStr"/>
       <c r="M88" t="inlineStr"/>
       <c r="N88" t="inlineStr"/>
       <c r="O88" t="inlineStr"/>
@@ -7027,101 +6323,29 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>ui_79</t>
+          <t>ui_89</t>
         </is>
       </c>
       <c r="B89" t="inlineStr"/>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>Machine Translation - for Moodle LMS</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>Parallel Text for machine translation in Eng-Kin; Domain-specific for Education (digital literacy)</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Enabling language translation capabilities on the Moodle LMS platform, through a collaboration with Atingi; the use case explores 3 modes of translation. The first mode is navigation based, simply translating static messages such as buttons and notifications, secondly it explores full content translation, lastly, in-line translation. The project uses the NLLB-200 model for translation, other models could be experimented to explore feasibility of additional features such as QA or summarization, leveraging the plugin built by the team. </t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://huggingface.co/datasets/DigitalUmuganda/kinyarwanda-english-machine-translation-dataset;  https://huggingface.co/datasets/mbazaNLP/Kinyarwanda_English_parallel_dataset; https://huggingface.co/datasets/mbazaNLP/NMT_Education_parallel_data_en_kin; https://huggingface.co/datasets/DigitalUmuganda/kinyarwanda-english-machine-translation-dataset </t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://huggingface.co/mbazaNLP/Quantized_Nllb_Finetuned_Edu_En_Kin_8bit; https://huggingface.co/mbazaNLP/Nllb_finetuned_general_en_kin; https://huggingface.co/DigitalUmuganda/Finetuned-NLLB </t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Inclusive Education</t>
-        </is>
-      </c>
-      <c r="I89" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t xml:space="preserve">FAIR Forward Rwanda / Digital Umuganda </t>
-        </is>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>Rwanda</t>
-        </is>
-      </c>
-      <c r="M89" t="inlineStr">
-        <is>
-          <t>Parallel datasets can be used to finetune LLMs to specific languages or domains; the example is for English-Kinyarwanda, to improve NLLB translation performance</t>
-        </is>
-      </c>
-      <c r="N89" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Open source model NLLB-200, some variations quantized to minimize compute resource usage </t>
-        </is>
-      </c>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Integrate preferred machine translation model with Moodle plugin: https://github.com/Digital-Umuganda/moodle-translate_courses . Need to update for compatibility with newer Moodle updates, this was implemented during Moodle version 3.0 </t>
-        </is>
-      </c>
-      <c r="P89" t="inlineStr">
-        <is>
-          <t>Permissive</t>
-        </is>
-      </c>
-      <c r="Q89" t="inlineStr">
-        <is>
-          <t>Atingi, Digital Umuganda, Clear Global</t>
-        </is>
-      </c>
-      <c r="R89" t="inlineStr">
-        <is>
-          <t>Isaac</t>
-        </is>
-      </c>
-      <c r="S89" t="inlineStr">
-        <is>
-          <t>NLP</t>
-        </is>
-      </c>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
+      <c r="K89" t="inlineStr"/>
+      <c r="L89" t="inlineStr"/>
+      <c r="M89" t="inlineStr"/>
+      <c r="N89" t="inlineStr"/>
+      <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
+      <c r="Q89" t="inlineStr"/>
+      <c r="R89" t="inlineStr"/>
+      <c r="S89" t="inlineStr"/>
       <c r="T89" t="inlineStr"/>
-      <c r="U89" t="inlineStr">
-        <is>
-          <t xml:space="preserve">- https://moodlemoot.org/2024/timetable/event/246/ / https://aiopeneducation.pubpub.org/pub/7npwm2su/release/5?readingCollection=06969c6d </t>
-        </is>
-      </c>
+      <c r="U89" t="inlineStr"/>
       <c r="V89" t="inlineStr"/>
       <c r="W89" t="inlineStr"/>
       <c r="X89" t="inlineStr"/>
@@ -7129,7 +6353,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>ui_80</t>
+          <t>ui_90</t>
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
@@ -7159,7 +6383,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>ui_81</t>
+          <t>ui_91</t>
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
@@ -7186,306 +6410,6 @@
       <c r="W91" t="inlineStr"/>
       <c r="X91" t="inlineStr"/>
     </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>ui_82</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr"/>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr"/>
-      <c r="F92" t="inlineStr"/>
-      <c r="G92" t="inlineStr"/>
-      <c r="H92" t="inlineStr"/>
-      <c r="I92" t="inlineStr"/>
-      <c r="J92" t="inlineStr"/>
-      <c r="K92" t="inlineStr"/>
-      <c r="L92" t="inlineStr"/>
-      <c r="M92" t="inlineStr"/>
-      <c r="N92" t="inlineStr"/>
-      <c r="O92" t="inlineStr"/>
-      <c r="P92" t="inlineStr"/>
-      <c r="Q92" t="inlineStr"/>
-      <c r="R92" t="inlineStr"/>
-      <c r="S92" t="inlineStr"/>
-      <c r="T92" t="inlineStr"/>
-      <c r="U92" t="inlineStr"/>
-      <c r="V92" t="inlineStr"/>
-      <c r="W92" t="inlineStr"/>
-      <c r="X92" t="inlineStr"/>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>ui_83</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr"/>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr"/>
-      <c r="F93" t="inlineStr"/>
-      <c r="G93" t="inlineStr"/>
-      <c r="H93" t="inlineStr"/>
-      <c r="I93" t="inlineStr"/>
-      <c r="J93" t="inlineStr"/>
-      <c r="K93" t="inlineStr"/>
-      <c r="L93" t="inlineStr"/>
-      <c r="M93" t="inlineStr"/>
-      <c r="N93" t="inlineStr"/>
-      <c r="O93" t="inlineStr"/>
-      <c r="P93" t="inlineStr"/>
-      <c r="Q93" t="inlineStr"/>
-      <c r="R93" t="inlineStr"/>
-      <c r="S93" t="inlineStr"/>
-      <c r="T93" t="inlineStr"/>
-      <c r="U93" t="inlineStr"/>
-      <c r="V93" t="inlineStr"/>
-      <c r="W93" t="inlineStr"/>
-      <c r="X93" t="inlineStr"/>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>ui_84</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr"/>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr"/>
-      <c r="F94" t="inlineStr"/>
-      <c r="G94" t="inlineStr"/>
-      <c r="H94" t="inlineStr"/>
-      <c r="I94" t="inlineStr"/>
-      <c r="J94" t="inlineStr"/>
-      <c r="K94" t="inlineStr"/>
-      <c r="L94" t="inlineStr"/>
-      <c r="M94" t="inlineStr"/>
-      <c r="N94" t="inlineStr"/>
-      <c r="O94" t="inlineStr"/>
-      <c r="P94" t="inlineStr"/>
-      <c r="Q94" t="inlineStr"/>
-      <c r="R94" t="inlineStr"/>
-      <c r="S94" t="inlineStr"/>
-      <c r="T94" t="inlineStr"/>
-      <c r="U94" t="inlineStr"/>
-      <c r="V94" t="inlineStr"/>
-      <c r="W94" t="inlineStr"/>
-      <c r="X94" t="inlineStr"/>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>ui_85</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr"/>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
-      <c r="E95" t="inlineStr"/>
-      <c r="F95" t="inlineStr"/>
-      <c r="G95" t="inlineStr"/>
-      <c r="H95" t="inlineStr"/>
-      <c r="I95" t="inlineStr"/>
-      <c r="J95" t="inlineStr"/>
-      <c r="K95" t="inlineStr"/>
-      <c r="L95" t="inlineStr"/>
-      <c r="M95" t="inlineStr"/>
-      <c r="N95" t="inlineStr"/>
-      <c r="O95" t="inlineStr"/>
-      <c r="P95" t="inlineStr"/>
-      <c r="Q95" t="inlineStr"/>
-      <c r="R95" t="inlineStr"/>
-      <c r="S95" t="inlineStr"/>
-      <c r="T95" t="inlineStr"/>
-      <c r="U95" t="inlineStr"/>
-      <c r="V95" t="inlineStr"/>
-      <c r="W95" t="inlineStr"/>
-      <c r="X95" t="inlineStr"/>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>ui_86</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr"/>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr"/>
-      <c r="E96" t="inlineStr"/>
-      <c r="F96" t="inlineStr"/>
-      <c r="G96" t="inlineStr"/>
-      <c r="H96" t="inlineStr"/>
-      <c r="I96" t="inlineStr"/>
-      <c r="J96" t="inlineStr"/>
-      <c r="K96" t="inlineStr"/>
-      <c r="L96" t="inlineStr"/>
-      <c r="M96" t="inlineStr"/>
-      <c r="N96" t="inlineStr"/>
-      <c r="O96" t="inlineStr"/>
-      <c r="P96" t="inlineStr"/>
-      <c r="Q96" t="inlineStr"/>
-      <c r="R96" t="inlineStr"/>
-      <c r="S96" t="inlineStr"/>
-      <c r="T96" t="inlineStr"/>
-      <c r="U96" t="inlineStr"/>
-      <c r="V96" t="inlineStr"/>
-      <c r="W96" t="inlineStr"/>
-      <c r="X96" t="inlineStr"/>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>ui_87</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr"/>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr"/>
-      <c r="E97" t="inlineStr"/>
-      <c r="F97" t="inlineStr"/>
-      <c r="G97" t="inlineStr"/>
-      <c r="H97" t="inlineStr"/>
-      <c r="I97" t="inlineStr"/>
-      <c r="J97" t="inlineStr"/>
-      <c r="K97" t="inlineStr"/>
-      <c r="L97" t="inlineStr"/>
-      <c r="M97" t="inlineStr"/>
-      <c r="N97" t="inlineStr"/>
-      <c r="O97" t="inlineStr"/>
-      <c r="P97" t="inlineStr"/>
-      <c r="Q97" t="inlineStr"/>
-      <c r="R97" t="inlineStr"/>
-      <c r="S97" t="inlineStr"/>
-      <c r="T97" t="inlineStr"/>
-      <c r="U97" t="inlineStr"/>
-      <c r="V97" t="inlineStr"/>
-      <c r="W97" t="inlineStr"/>
-      <c r="X97" t="inlineStr"/>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>ui_88</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr"/>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="inlineStr"/>
-      <c r="F98" t="inlineStr"/>
-      <c r="G98" t="inlineStr"/>
-      <c r="H98" t="inlineStr"/>
-      <c r="I98" t="inlineStr"/>
-      <c r="J98" t="inlineStr"/>
-      <c r="K98" t="inlineStr"/>
-      <c r="L98" t="inlineStr"/>
-      <c r="M98" t="inlineStr"/>
-      <c r="N98" t="inlineStr"/>
-      <c r="O98" t="inlineStr"/>
-      <c r="P98" t="inlineStr"/>
-      <c r="Q98" t="inlineStr"/>
-      <c r="R98" t="inlineStr"/>
-      <c r="S98" t="inlineStr"/>
-      <c r="T98" t="inlineStr"/>
-      <c r="U98" t="inlineStr"/>
-      <c r="V98" t="inlineStr"/>
-      <c r="W98" t="inlineStr"/>
-      <c r="X98" t="inlineStr"/>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>ui_89</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr"/>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr"/>
-      <c r="E99" t="inlineStr"/>
-      <c r="F99" t="inlineStr"/>
-      <c r="G99" t="inlineStr"/>
-      <c r="H99" t="inlineStr"/>
-      <c r="I99" t="inlineStr"/>
-      <c r="J99" t="inlineStr"/>
-      <c r="K99" t="inlineStr"/>
-      <c r="L99" t="inlineStr"/>
-      <c r="M99" t="inlineStr"/>
-      <c r="N99" t="inlineStr"/>
-      <c r="O99" t="inlineStr"/>
-      <c r="P99" t="inlineStr"/>
-      <c r="Q99" t="inlineStr"/>
-      <c r="R99" t="inlineStr"/>
-      <c r="S99" t="inlineStr"/>
-      <c r="T99" t="inlineStr"/>
-      <c r="U99" t="inlineStr"/>
-      <c r="V99" t="inlineStr"/>
-      <c r="W99" t="inlineStr"/>
-      <c r="X99" t="inlineStr"/>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>ui_90</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr"/>
-      <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr"/>
-      <c r="E100" t="inlineStr"/>
-      <c r="F100" t="inlineStr"/>
-      <c r="G100" t="inlineStr"/>
-      <c r="H100" t="inlineStr"/>
-      <c r="I100" t="inlineStr"/>
-      <c r="J100" t="inlineStr"/>
-      <c r="K100" t="inlineStr"/>
-      <c r="L100" t="inlineStr"/>
-      <c r="M100" t="inlineStr"/>
-      <c r="N100" t="inlineStr"/>
-      <c r="O100" t="inlineStr"/>
-      <c r="P100" t="inlineStr"/>
-      <c r="Q100" t="inlineStr"/>
-      <c r="R100" t="inlineStr"/>
-      <c r="S100" t="inlineStr"/>
-      <c r="T100" t="inlineStr"/>
-      <c r="U100" t="inlineStr"/>
-      <c r="V100" t="inlineStr"/>
-      <c r="W100" t="inlineStr"/>
-      <c r="X100" t="inlineStr"/>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>ui_91</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr"/>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
-      <c r="E101" t="inlineStr"/>
-      <c r="F101" t="inlineStr"/>
-      <c r="G101" t="inlineStr"/>
-      <c r="H101" t="inlineStr"/>
-      <c r="I101" t="inlineStr"/>
-      <c r="J101" t="inlineStr"/>
-      <c r="K101" t="inlineStr"/>
-      <c r="L101" t="inlineStr"/>
-      <c r="M101" t="inlineStr"/>
-      <c r="N101" t="inlineStr"/>
-      <c r="O101" t="inlineStr"/>
-      <c r="P101" t="inlineStr"/>
-      <c r="Q101" t="inlineStr"/>
-      <c r="R101" t="inlineStr"/>
-      <c r="S101" t="inlineStr"/>
-      <c r="T101" t="inlineStr"/>
-      <c r="U101" t="inlineStr"/>
-      <c r="V101" t="inlineStr"/>
-      <c r="W101" t="inlineStr"/>
-      <c r="X101" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed data type filter error
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -3980,7 +3980,7 @@
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Climate Action, Disaster Risk Reduction Management</t>
+          <t>Climate Action, Disaster Risk Management</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -5332,7 +5332,7 @@
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Agriculture, Climate action, SDG 2 </t>
+          <t xml:space="preserve">Agriculture, Climate Action, SDG 2 </t>
         </is>
       </c>
       <c r="I60" t="inlineStr">

</xml_diff>

<commit_message>
shortened SDG 10 tag
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -589,7 +589,7 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Climate Action, Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>Climate Action, SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -2385,7 +2385,7 @@
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2657,7 +2657,7 @@
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2733,7 +2733,7 @@
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
@@ -2798,7 +2798,7 @@
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2988,7 +2988,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -3225,7 +3225,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -3331,7 +3331,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -3659,7 +3659,7 @@
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -3911,7 +3911,7 @@
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -3975,7 +3975,7 @@
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -4055,7 +4055,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Climate Action, Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -4269,7 +4269,7 @@
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -4419,7 +4419,7 @@
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Agriculture, Climate Action, Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -4621,7 +4621,7 @@
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -4722,7 +4722,7 @@
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Agriculture, Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -4798,7 +4798,7 @@
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -4878,7 +4878,7 @@
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
@@ -4950,7 +4950,7 @@
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
@@ -5106,7 +5106,7 @@
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -5170,7 +5170,7 @@
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Health, Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -5234,7 +5234,7 @@
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I63" t="inlineStr"/>
@@ -5299,7 +5299,7 @@
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -5363,7 +5363,7 @@
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
@@ -6737,7 +6737,7 @@
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
@@ -7346,7 +7346,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Inclusive Education, Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>Inclusive Education, SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
@@ -7436,7 +7436,7 @@
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Agriculture, Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>Agriculture, SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I88" t="inlineStr"/>
@@ -7504,7 +7504,7 @@
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Agriculture, Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>Agriculture, SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
@@ -7576,7 +7576,7 @@
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Agriculture, Reduced inequality through access to info in local languages/NLP  (SDG 10)</t>
+          <t>Agriculture, SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">

</xml_diff>

<commit_message>
data pull and fixed backup
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X99"/>
+  <dimension ref="A1:X96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,17 +568,13 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Making access to financial applications possible in native Ghanaian languages in informal settings: Akan (Akuapem Twi, Asante Twi, Fante) and Ga</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Build AI-powered solutions to improve financial inclusion within the informal sector of Ghana's economy</t>
-        </is>
-      </c>
+          <t>Facilitating access to financial applications in informal settings in four Ghanaian dialects: Akuapem Twi, Ashante Twi, Fante and Ga.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>This speech dataset for the Ghanian languages Akan (Akuapem Twi, Asante Twi, Fante) and Ga includes 104,000 utterances (speech) across the four dialects/languages with approximately 200 speakers per dialect/language. This amounts to about 148 hours of speech in total. The dataset was developed to support the development of financial applications in native Ghanaian languages to allow illiterate and semi-literate people to fully benefit from digital financial services. Secondly, it aims to answer research questions related to domain-specific vs. general-purpose dataset development, dialects, as well as NLP system development in low resource settings.</t>
+          <t xml:space="preserve">This speech dataset for the Ghanian languages Akan (Akuapem Twi, Asante Twi, Fante) and Ga includes 104,000 utterances (speech) across the four dialects/languages with approximately 200 speakers per dialect/language. This amounts to about 148 hours of speech in total. The dataset was developed to support the development of financial applications in native Ghanaian languages to allow illiterate and semi-literate people to fully benefit from digital financial services. Secondly, it aims to answer research questions related to domain-specific vs. general-purpose dataset development, dialects, as well as NLP system development in low resource settings.  Overall, a total of 83,829 audios were recorded from which the datasets were published and made publicly accessible.  </t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -589,7 +585,7 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Climate Action, SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>Reduced inequality through access to info in local languages/NLP (SDG 10), Promote inclusive economic growth through financial inclusion (SDG 8)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -607,9 +603,22 @@
           <t>Ghana</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>The data is freely available for use based on the provided open source license and courtesy the funding from Lacuna Fund. We performed a stratified random sampling (5%) of the data for each language and reviewed it to get the following quality assessments.
+0.1% of the Ga audios were of low quality
+1.3% of the Fanti audios were of low qaulity.
+1.6% of the Asanti Twi audios were of low quality.
+2.8% of the Akuapem Twi audios were of low quality.
+Low quality means that what the user recorded did not match the given prompt either because there was a truncation or the recording was totally different from the prompt.</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>The dataset might be used to devise more inclusive banking platforms that better understand users in  in four Ghanaian dialects: Akuapem Twi, Ashante Twi, Fante and Ga. It can thereby help to achive more financial inclusion.</t>
+        </is>
+      </c>
       <c r="O2" t="inlineStr">
         <is>
           <t>https://creativecommons.org/licenses/by/4.0/</t>
@@ -617,14 +626,14 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Powered by:  
+          <t>Powered by:  Ashesi University, Nokwary Technologies
 Catalyzed by: Lacuna-Fund / Meridian &amp; FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Elikplim Sabblah </t>
+          <t xml:space="preserve">Elikplim Sabblah, Balthas Seibold </t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -660,7 +669,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Drone-based Agricultural Dataset for Crop Yield Estimation in Ghana and Uganda (Cashew, Cocoa and Coffee) </t>
+          <t>Enable Cashew, Cocoa and Coffee farmers to make good business decisions - Drone-based Agricultural Dataset for Crop Yield Estimation in Ghana and Uganda</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -678,7 +687,7 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Climate Action, Agriculture</t>
+          <t>Climate Action, End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -749,13 +758,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Building parallel corpora for Kenya’s Indigenous Languages and Swahili</t>
+          <t>Enabling machine translation from Kiswahili into the indigenous Kenyan languages Kidaw'ida, Kalenjin, and Dholuo, preserving these languages &amp; supporting crowd-sourced voice recognition via Mozilla Common Voice for these languages</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>There is a significant opportunity to make digitized government services in Kenya more easily discoverable and, by extension, enhance their accessibility and use by citizens through chatbot technology. Based on NLP technology, chatbots can help citizens access information on Kenya’s eGovernment services through text and voice inputs in Kiswahili and English. This project foresees the development of an AI Conversational Chatbot using the GovStack Building Block Approach - so as to create (a) a chatbot for easier service discoverability; and (b) a chatbot framework that can be reused as a digital public good.</t>
+          <t xml:space="preserve">The dataset was created to enable translation from Kiswahili, which is the national language in Kenya, into three indigenous languages, namely, Kidaw'ida, Kalenjin, and Dholuo. All three languages are low resource, especially Kidaw'ida, which has only around 400,000 speakers and is at immediate risk of loss. By collecting the text and speech data, the project has taken a step towards preservation of these languages . The dataset consists of three parallel corpora: Kidaw'ida-Kiswahili; Kalenjin-Kiswahili; Dholuo-Kiswahili. On average, each corpus has thirty thousand sentence pairs. 
+In addition, the dataset has helped to preserve, revitalise and elevate the languages Kidaw'ida, Kalenjin, and Dholuo by making them work on Mozillas Common Voice Platform. The text and speech datasets are thereby supporting crowd-sourced voice recognition, promoting linguistic diversity and empoweromg local communities by enabling Natural Language Processing applications tailored to their needs. Namely, the resulting voice recognition datasets can be used to build AI voice applications such as advisory systems in local languages for farmers, citizens etc that "understand" speech input (instead of written input). As of August 2025, 120 hours of speech data have been recorded on Common Voice in Dholuo (with 14692 sentences available), 92 hours have been recorded for Kalendjin (With 29900 sentences available) and 56 hours have been recorded for Kidaw'ida (with 11773 sentences available). To download the crowd-sourced speech datasets in Kidaw'ida, Kalenjin, and Dholuo, visit https://commonvoice.mozilla.org/en/datasets </t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -766,10 +776,14 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Climate Action</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr"/>
+          <t>Reduced inequality through access to info in local languages/NLP (SDG 10), Achieve Gender Equality (SGD 5), achieve food security, sustainable agriculture (SDG 2)</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Text, Voice</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr">
         <is>
           <t>Audrey Mbogho (ambogho@usiu.ac.ke)</t>
@@ -780,18 +794,36 @@
           <t>Kenya</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>The dataset consists of three parallel corpora: Kidaw'ida-Kiswahili; Kalenjin-Kiswahili; Dholuo-Kiswahili. On averate, each corpus has thirty thousand sentence pairs. This dataset is available on Zenodo and on GitHub where it will continue to be grown and its quality improved. The project had a total of 105 speakers who came from different parts of each region where the three languages are spoken. Thus, different regional accents were included in the speech data, making the dataset more representative. Furthermore, both male and female speakers were contributing to the voice data.</t>
+        </is>
+      </c>
       <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">&gt; The datasets can help to build translation services from Kiswahili into three indigenous languages, namely, Kidaw'ida, Kalenjin, and Dholuo. 
+&gt; The datasets can help to preserve these three low resource languages, promote linguistic diversity and empower local communities by enabling Natural Language Processing applications tailored to their needs.
+&gt; the resulting voice recognition datasets can be used to build AI voice applications such as advisory systems in local languages for farmers, citizens etc that "understand" speech input (instead of written input).  </t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Apache License 2.0</t>
+        </is>
+      </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Powered by:  
+          <t>Powered by:   USIU - Africa in cooperation with Kabarak University and Maseno University, Kenya
 Catalyzed by: Lacuna-Fund / Meridian &amp; FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Balthas Seibold</t>
+        </is>
+      </c>
       <c r="R4" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -802,13 +834,22 @@
           <t>Dataset</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr"/>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Natural Language Processing (NLP)</t>
+        </is>
+      </c>
       <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://arxiv.org/pdf/2501.11003, https://github.com/waleghwa/low-resource-language-data, https://commonvoice.mozilla.org/en/datasets </t>
+        </is>
+      </c>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr">
         <is>
-          <t>JN: Can you add the missing info (e.g. link to dataset etc.)? It's from Lacuna (comment by DB) Link is there (JN).</t>
+          <t>Comment Balthas: original title is "Building parallel corpora for Kenya’s Indigenous Languages and Swahili"
+DONE on 25.8., Balthas</t>
         </is>
       </c>
     </row>
@@ -825,14 +866,14 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Labelled Open solar panel data for Madagascar</t>
+          <t>Helping to measure solar energy adoption across Madagascar via AI - Labelled Open solar panel data for Madagascar</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>This team annotated 2,125 Google Earth satellite images and 9,202 drone images, forming a combination of low and high-definition solar panel views in Madagascar. The Madagascar Initiatives for Digital Innovation (MAIDI) team performed field checks for up to 25% of satellite images and, in total, annotated 22,488 polygons.
- This dataset will help data scientists and users develop a solar panel detection algorithm to measure solar energy adoption across Madagascar. Notably, this project represented all regions of the country; instead of focusing only on big cities, it also covered average and small villages as well as coasts and mountains.</t>
+          <t>This dataset will help data scientists, government and users to measure solar energy adoption across Madagascar. It laid the groundwork needed to develop a solar panel detection algorithm working in Madagaskar. Notably, this project represented all regions of the country; instead of focusing only on big cities, it also covered average and small villages as well as coasts and mountains.
+The team annotated 2,125 Google Earth satellite images and 9,202 drone images, forming a combination of low and high-definition solar panel views in Madagascar. The Madagascar Initiatives for Digital Innovation (MAIDI) team performed field checks for up to 25% of satellite images and, in total, annotated 22,488 polygons.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -874,7 +915,11 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr"/>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
@@ -894,13 +939,13 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>A Nigerian Twitter Sentiment Corpus for Multilingual Sentiment Analysis</t>
+          <t>Detecting sentiments and combatting hate speech in Hausa, Igbo, Nigerian-Pidgin and Yorùbá - NaijaSenti: a Nigerian Corpus for Multilingual Sentiment Analysis</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>This dataset is the first large-scale human-annotated Twitter sentiment dataset for Hausa, Igbo, Nigerian-Pidgin, and Yorùbá, the four most widely spoken languages in Nigeria.</t>
+          <t>The NaijaSenti dataset is the first large-scale human-annotated Twitter sentiment dataset for Hausa, Igbo, Nigerian-Pidgin, and Yorùbá, the four most widely spoken languages in Nigeria. It consists of around 30,000 annotated tweets per language (except for Nigerian-Pidgin), including a significant fraction of code-mixed tweets. These datasets are useful not only for sentiment analysis but also for hate speech detection. The open-source package consists of datasets, trained models, sentiment lexicons, and code. With more than 200 million people and 522 native languages, Nigeria is the most populous and linguistically diverse country in Africa, as well as the third most multilingual country in the world. The majority of the population speaks either Hausa, Igbo, Yorùbá, or Nigerian-Pidgin.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -908,13 +953,21 @@
           <t>https://github.com/hausanlp/NaijaSenti</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://github.com/hausanlp/NaijaSenti</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>Climate Action, SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr">
         <is>
           <t>NaijaSenti (https://github.com/hausanlp/NaijaSenti?tab=readme-ov-file#contact-us)</t>
@@ -925,29 +978,65 @@
           <t>Nigeria</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>The project developed and made the following resources available:   1. Manually Annotated Twitter Sentiment Dataset 2. Manually Annotated Sentiment Lexicon 3. Semi-automatically Translated emotion lexicon 4. Semi-automatically Translated sentiment lexicon 5. Large Scale Unlabeled Twitter Sentiment Corpus 6. Stop-words for Hausa, Igbo, Pidgin and Yoruba     7. text  collection,  filtering, processing  and  labeling  methods  to  create  datasets  for  these  low-resource  languages.   8. evaluation og a  range of  pre-trained  models  and  transfer  strategies  on  the  dataset. 9. release  of datasets,  trained  models,  sentiment  lexicons,  and  code  to  incentivize research on sentiment analysis in under-represented languages. Authors: Shamsuddeen Hassan Muhammad, David Ifeoluwa Adelani, Sebastian Ruder, Ibrahim Said Ahmad, Idris Abdulmumin, Bello Shehu Bello, Monojit Choudhury, Chris Chinenye Emezue, Saheed Salahudeen Abdullahi, Anuoluwapo Aremu, Alipio Jeorge, and Pavel Brazdil</t>
+        </is>
+      </c>
       <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NaijaSenti can be used to advance sentiment analysis and other downstream NLP tasks in the languages involved and to work on hate speech detection. For such follow-up work on hate speech, see also: https://arxiv.org/abs/2501.08284 </t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>CC-BY 4.0</t>
+        </is>
+      </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Powered by:  
+          <t>Powered by:  Bayero University, Kano, Nigeria, Ahmadu Bello University, Zaria, Nigeria, Masakhane NLP, HausaNLP, Kaduna state University 
 Catalyzed by: Lacuna-Fund / Meridian &amp;  FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Balthas Seibold</t>
+        </is>
+      </c>
       <c r="R6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Dataset &gt; Model</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Natural language Processing” (NLP)</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>NaijaSenti/image/naijasenti_logo1.png at main · hausanlp/NaijaSenti · GitHub</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>https://arxiv.org/pdf/2201.08277</t>
+        </is>
+      </c>
       <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>DONE on 25.8., Balthas</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -962,14 +1051,13 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Datasets marking Personal Identifiable Information (PII) and Gender Bias</t>
+          <t>Preserving privacy and avoiding gender bias of AI systems in Luganda, Lumasaba, Hausa, and Kanuri - The Lacuna personally identifiable information Text Dataset</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>This dataset contains annotated sentences with personally identifiable information (PII) in Luganda, Lumasaba, Hausa, and Kanuri. These four languages span Central and Eastern Uganda, Nigeria, Ghana, and Northern Cameroon. The team collected 3,000 sentences for both Kanuri and Hausa, 5,000 for Lumasaba, and 4,000 for Luganda. Potential use cases for these datasets include named entity recognition (NER), text classification, privacy-preserving data analysis and research, language modeling, machine translation, and linguistic research.
- The team aimed to curate a dataset that is gender inclusive, and their work highlighted the need for standardized guidelines for annotating low-resourced languages. Having these guidelines would help to avoid common pitfalls and errors when labeling text data in these low-resource languages.</t>
+          <t>The Lacuna PII Multilingual Text Dataset  contains annotated sentences with personally identifiable information (PII) in Luganda, Lumasaba, Hausa, and Kanuri. These four languages span Central and Eastern Uganda, Nigeria, Ghana, and Northern Cameroon. The dataset can help to anonymize and pseudonymize personally identifiable information in AI tasks. This can help organizations comply with legal requirements while still being able to analyze and use and share their data effectively. It can also be used to improve machine translation systems for low-resource languages,  improve the performance of NLP applications in these languages, and support the extraction of specific information from text, such as automated form filling and information retrieval systems. It comprises 4000 Luganda sentences, 5000 Lumasaba sentences, 3000 Kanuri sentences, and 3000 Hausa sentences. The team aimed to curate a dataset that is gender inclusive. It was created by Makerere Artificial Intelligence Lab in collaboration with Marconi Lab and Clear Global.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -980,7 +1068,7 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Climate Action, SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>Climate Action, SDG 10 (Reduced inequality through access to info in local languages/NLP), Achieve Gender Equality (SDG 5)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -998,29 +1086,65 @@
           <t>Uganda,Kenya,Nigeria</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Text data:
+• Luganda: 4000 PII sentences with representation in entities of
+Person, Date, National identity, tribal identity, location, and organization.
+• Lumasaaba: 5000 PII sentences with representation in entities
+of Person, Date, National identity, tribal identity, location, and
+organization.
+• Hausa: 3000 PII sentences with representation in entities of Person, Date, National identity, tribal identity, location, and organization.
+• Kanuri: 3000 PII sentences with representation in entities of Person, Date, National identity, tribal identity, location, and organization
+For more, see data card here: https://dataverse.harvard.edu/file.xhtml?fileId=10577233&amp;version=2.0</t>
+        </is>
+      </c>
       <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This dataset of personally identifiable information (PII) can help any organization or initiative, that would like to comply with legal requirements while still being able to analyze and use and share data effectively in one of the languages in Luganda, Lumasaba, Hausa, and Kanuri. It can also be used to improve machine translation systems for these low-resource languages, improve the performance of NLP applications in these languages, and support the extraction of specific information from text, such as automated form filling and information retrieval systems. </t>
+        </is>
+      </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Powered by:  
+          <t>Powered by:  Makerere Artificial Intelligence Lab in collaboration with Marconi Lab and Clear Global
 Catalyzed by: Lacuna-Fund / Meridian &amp;  FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Balthas Seibold</t>
+        </is>
+      </c>
       <c r="R7" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Natural language Processing” (NLP)</t>
+        </is>
+      </c>
       <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>https://dataverse.harvard.edu/file.xhtml?fileId=10577234&amp;version=2.0</t>
+        </is>
+      </c>
       <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>First editing DONE on 25.8., Balthas</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1034,9 +1158,17 @@
           <t>Ecuadorian Dataset on Access, Demand, &amp; Availability of Electricity Supply</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Ecuador Electricity Access &amp; Supply Data</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Not published</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
@@ -1061,18 +1193,30 @@
 Financed by: BMZ</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Luisa Olaya</t>
+        </is>
+      </c>
       <c r="R8" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr"/>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>First editing DONE on 28.8., Luisa - There´s no much information available</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1083,7 +1227,7 @@
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Artificial Intelligence for Energy Access (AI4EA)</t>
+          <t>Powering Rural Futures in West Africa: AI-Driven Demand Data for Smarter Electrification</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -1132,18 +1276,39 @@
           <t>ui_63</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Residential Energy and Weather Dataset (REWD) of Pakistan</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Residential Energy and Weather Dataset (REWD) of Pakistan</t>
+          <t>Promoting energy conservation and market analysis in Pakistan through Residential Energy and Weather Data (REWD)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>This dataset helps to understand energy consumption patterns in relation to weather conditions in Pakistan. This can guide policymaking on energy and energy conservation, sustainabe energy initiatives and private sector use (market assessment and strategic planning as new entrants in the restructured energy market). 
+The project produced an energy dataset of residential consumption data from buildings across six climatic zones. The energy dataset is recorded on a 1-minute granularity for entire household usage as well as for individual appliances. With over a year of detailed energy consumption data and 18 months of weather data collected from a diverse array of households across six distinct climatic zones, it is one of the most comprehensive datasets of its kind. This meteorological dataset has been accumulated over a period of 18 months for the six urban centers. This weather data comprises of up to 10 essential variables such as temperature, atmospheric pressure, humidity and Precipitation, thus providing an all-around perspective of the environmental elements impacting energy consumption.</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Residential Energy and Weather Data (REWD) - Pakistan</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Climate action, clean energy SDG7</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Tabular</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr">
         <is>
           <t>Lahore University of Management Sciences (LUMS)</t>
@@ -1154,29 +1319,56 @@
           <t>Pakistan</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>This Dataset is available in the webpage of the Lahore University. The dataset consist oth three parallel corpora: 
+1. Electricity consumption datacollected over year through advanced smart meters. The dataset consists of 60 households belonging to six major urban centers in varying climatic zones across the country. It is recorded on a 1-minute granularity for entire household usage as well as for individual appliances.  
+2. Metadata encompassing building attributes and demographic information for each household. The households in the dataset represent a wide and mixed demographic, social structure, and financial background.
+3. Meteorological dataset created with infromation of 18 months for six urban centers. It comprises of up to 10 essential variables: temperature, atmospheric pressure, humidity, dew, precipitation, wind direction, wind speed, solar radiation, solar energy and UV index</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>The resources can support policymaking and inform energy sustainability initiatives. They can namely be  utilized by key stakeholders such as the Ministry of Climate Change, Ministry of Energy (Power Division),  Punjab Energy Efficiency &amp; Conservation Authority, and National Energy Efficiency &amp;  Conservation Authority (NEECA)  Moreover,  private sector companies can use the data for market assessment purposes and strategic planning as new entrants in the restructured energy market.  The resources can also support further academic research and innovation.</t>
+        </is>
+      </c>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Powered by:  [ADD!!!]
+          <t>Powered by: Lahore University (LUMS)
 Catalyzed by: Lacuna-Fund / Meridian (Climate-call) &amp;  FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Luisa Olaya</t>
+        </is>
+      </c>
       <c r="R10" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>First Editing done by Luisa 27.08.2025, Title and description revised by Balthas on 2.9. to strenghten the "What can I do with this dataset" dimension - catchy title.</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1190,12 +1382,32 @@
           <t>Datasets for transportation impact evaluation</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Urban roadspace classification data and model</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>The team developed a labeled training dataset, derived from 50cm or better satellite imagery, based on a novel, pre-defined road space classification taxonomy appropriate for training and deployment of large-scale deep-learning models</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>GitHub - yangshao2/UrbanInfraDL</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Reduce inequality, SDG2</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Geospatial</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr">
         <is>
           <t>Fundación Despacio,World Resources Institute,Fundación Despacio</t>
@@ -1206,29 +1418,63 @@
           <t>Colombia</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dataset and model available in Github. Dataset of  roadspace from 15 areas of Bogota each 1Km. 
+Bogotá’s orthophoto and GIS layers. 
+Data Dictionary </t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Model that was tested for the entire city of Bogotá to clasify urban roadspace..And it worked with 98% reliability. Unfortunately not more info available</t>
+        </is>
+      </c>
       <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>CC-BY 4.0 license</t>
+        </is>
+      </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Powered by:  [ADD!!!]
+          <t>Powered by: Fundación Despacio
 Catalyzed by: Lacuna-Fund / Meridian (Climate-call) &amp;  FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Luisa Olaya</t>
+        </is>
+      </c>
       <c r="R11" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Dataset &gt; Model</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Computer Vision </t>
+        </is>
+      </c>
       <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>Link to White paper</t>
+        </is>
+      </c>
       <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>First Editing done by Luisa 28.08.2026 / Availability on Github: it doesn´t have a good exmplanation, which makes it hard to know what is it about.</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1236,18 +1482,38 @@
           <t>ui_65</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Machine learning training data for continental Ecuador and Galapagos</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Machine learning training data for continental Ecuador and Galapagos</t>
+          <t>Monitoring the impact of palm oil monoculture, shrimp aquaculture &amp; mining in continental Ecuador and the Galapagos using AI</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>The dataset can help to build systems, that can monitor the impact of palm oil monoculture, shrimp aquaculture, mining and other land transformations in continental Ecuador and Galapagos. The project created a 20.000 points land use/cover classification training dataset from existing data, with labels that can be used to train multi-spectral Earth observation (EO) data machine learning (ML)  models covering continental Ecuador and the Galapagos islands.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>LULC training data for Ecuador - ML</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Climate action SDG 13, Life on Land (SDG 15): sustainably manage forests, halt and reverse land degradation and halt biodiversity loss.</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Geospatial</t>
+        </is>
+      </c>
       <c r="J12" t="inlineStr">
         <is>
           <t>Fundacion Ecociencia</t>
@@ -1258,29 +1524,64 @@
           <t>Ecuador</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr"/>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Two datasets available: 
+- BaseDatosValidacionFinal30052: This is the raw dataset containing 20,000 georeferenced points along with their respective land cover classifications.
+- LULC Training Data for Ecuador ML: This dataset builds upon the first by incorporating additional information on the conservation status of each point. This includes whether the location falls within protected areas, indigenous territories, areas under government forest incentive programs, and other conservation-related designations.</t>
+        </is>
+      </c>
       <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This dataset will allow for a better understanding of land transformation dynamics taking place, such as forest conversion to palm oil monoculture, mangrove transformation to shrimp aquaculture, water bodies and estuarine vegetation impacted by mining, natural grasslands encroached upon by expanding forest plantation, and more. It also has the potential to identify recovery cases. For example, the Galapagos data might provide the ability to estimate if invasive species control programs have had a positive impact in vegetation regeneration or if governmental forest incentives are promoting deforestation reduction in the Ecuadorian Amazon. The land’s conservation status has the potential to predict risk of future transformation. </t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>CC-BY 4.0 license</t>
+        </is>
+      </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Powered by:  [ADD!!!]
+          <t>Powered by:  Ecociencia
 Catalyzed by: Lacuna-Fund / Meridian (Climate-call) &amp;  FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Luisa Olaya</t>
+        </is>
+      </c>
       <c r="R12" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Computer Vision </t>
+        </is>
+      </c>
       <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quote: “Land cover/use temporal trends are essential to understand the status of the remaining natural cover and change trends. But understanding the drivers of land use/cover change with local precision has proved challenging when working with existing global-scale datasets. Lacuna Fund’s support will allow us to create a precise dataset that will elevate our ability to discriminate land use classes that are both temporally and spatially descriptive. This funding will also support an extra layer of data to support projects aimed at reducing the pressure on standing forests and help maintain the socio-natural systems that have successfully prevented conversion of forests for anthropogenic use.” 
+– Wagner Holguín, Coordinator of MapBiomas Ecuador, Fundación Ecociencia </t>
+        </is>
+      </c>
       <c r="W12" t="inlineStr"/>
-      <c r="X12" t="inlineStr"/>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>First Editing done by Luisa 28.08.2027, titel and description revised by Balthas on 2.9. to strenghten the "What can I do with this dataset" dimension - catchy title.</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1291,7 +1592,7 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Forest carbon sequestration in the Congo Basin</t>
+          <t xml:space="preserve">Forest carbon sequestration in the Congo Basin: combining In Situ Data and Artificial Intelligence to unlock climate finance </t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -1330,7 +1631,12 @@
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quote: "At a time when the Congo Basin has become the most important rainforest carbon sink, and one of the highest biodiversity hotspots in the world, understanding and tracking its dynamics is more urgent than ever if we want to achieve global 2030 climate and biodiversity goals. With support from Lacuna Fund, our project will help bring machine learning to scientists working on the ground to monitor this ecosystem. It will pilot innovative technologies to close knowledge gaps and help speed action towards better managing these rainforests, ensuring a better world for people, nature, and climate.”  
+— Teodyl Nkuintchua, Congo Basin Strategy and Engagement Leader and Country Manager for Republic of Congo, World Resources Institute Africa </t>
+        </is>
+      </c>
       <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
     </row>
@@ -1343,7 +1649,7 @@
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>GEO Indigenous Alliance</t>
+          <t>Indigenous Knowledge Meets AI: Monitoring Elephants and Rodents in Kenya and Ecuador with Biodiversity AI-Datasets</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -1362,7 +1668,11 @@
           <t>Ecuador,Kenya</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>This meteorological dataset has been accumulated over a period of 18 months for the six urban centers. This weather data comprises of up to 10 essential variables such as temperature, atmospheric pressure, humidity and Precipitation, thus providing an all-around perspective of the environmental elements impacting energy consumption.</t>
+        </is>
+      </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
@@ -1382,7 +1692,12 @@
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quote: “Through the integration of Indigenous knowledge and cutting-edge technology, the Ltome-Katip project not only addresses pressing environmental and technical machine learning challenges but empowers Indigenous communities to lead the way in conservation efforts. This initiative, in collaboration with the Rochester Institute and Space4Innovation, represents a true partnership between the Shuar tribe in the Ecuadorian Amazon and the Samburu tribe in northern Kenya, showcasing the power of collaboration and Indigenous knowledge in safeguarding our planet’s biodiversity.” 
+— Mario Vargas Shakaim (Shuar), Ltome-Katip Indigenous-Led Monitoring Project GEO Indigenous Alliance </t>
+        </is>
+      </c>
       <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr"/>
     </row>
@@ -1395,7 +1710,7 @@
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Ivorian mangroves and carbon stock</t>
+          <t>AI for Mangrove Carbon Credits: Turning Forest Data into Climate Action in Côte d’Ivoire</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -1434,7 +1749,12 @@
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quote: “As far as monitoring and calculating forest carbon stocks are concerned, there is still a major technological bottleneck blocking the large-scale development of forest carbon credits in Côte d’Ivoire, which needs to be overcome quickly. Remote sensing is a useful tool in the forest monitoring process; further studies should be carried out to enable it to meet the need for assessment on a smaller scale and to measure biomass directly. In this way, we can help decision-makers orient their conservation policies, but also support the process of rewarding small players, such as agricultural producers involved in agroforestry, private forestry, etc. Our aim, with the funds raised, is to provide practical field data to better train artificial intelligence algorithms for dynamic mapping of forest biomass and mangroves.”   
+ — Abraham Bio, Actum Dev General Manager </t>
+        </is>
+      </c>
       <c r="W15" t="inlineStr"/>
       <c r="X15" t="inlineStr"/>
     </row>
@@ -1447,15 +1767,31 @@
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Reference Data Collection for Improving Land Use Change Mapping in Ghana</t>
+          <t>Mapping Cocoa Landscapes in Ghana: Reference Data for Tracking Land Use Change</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>This dataset was produced by the Centre for Remote Sensing and Geographic Information Services (CERSGIS) as part of the project Reference Data Collection for Improving Land Use Change Mapping in Ghana. The primary objective was to develop high-quality reference data to enhance the accuracy of remote sensing-based land use and land cover (LULC) change mapping using machine learning methods in Ghana’s cocoa production landscapes.</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://zenodo.org/records/15778396</t>
+        </is>
+      </c>
       <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Life on Land (SDG 15): sustainably manage forests, halt and reverse land degradation and halt biodiversity loss.</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Geospatial</t>
+        </is>
+      </c>
       <c r="J16" t="inlineStr">
         <is>
           <t>Center for Remote Sensing and Geographic Information Services</t>
@@ -1466,27 +1802,88 @@
           <t>Ghana</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Content:
+• 21,031 geocoded cocoa farm polygons (including agroforestry and shadeless cocoa)
+• 14,192 homogeneous (shadeless) cocoa polygons digitized from farm plots
+• 20,035 additional points/polygons for other land uses (informal gold mining, degraded forest, oil palm, rubber)
+• 485 anonymised household clusters (from 4,444 individual surveys) providing socioeconomic context
+Collection methods:
+• OpenForis Ground (field-based polygon collection)
+• Collect Earth Online (land use mapping)
+• KoboToolbox (household survey data)
+Purpose: Reference dataset for remote sensing, land cover classification, and land use change mapping in cocoa production landscapes.
+Limitations:
+• Polygons represent portions of farms, not legal or property boundaries.
+• Farm sizes do not reflect entire holdings.
+• Not suitable for certification or compliance purposes.</t>
+        </is>
+      </c>
       <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>What can be done immediately:
+• Train and validate machine learning models for cocoa farm detection, deforestation monitoring, and land use classification.
+• Use as a benchmark dataset to evaluate remote sensing products in heterogeneous tropical landscapes.
+• Support policy analysis on sustainable cocoa, land degradation, and restoration planning in Ghana.
+How to extend or improve:
+• Add new field reference data from other cocoa-producing regions (e.g., Côte d’Ivoire, Nigeria) to increase transferability.
+• Integrate household-level socioeconomic data to study drivers of land use change and cocoa–forest dynamics.
+• Combine with climate and soil datasets to model sustainability scenarios.
+Limitations / ethical use:
+• Must not be used for farm-level regulation or compliance; polygons are reference only.
+• Potential imbalances between cocoa vs. non-cocoa land use classes should be addressed in model training.
+• Users are encouraged to conduct an ethical AI assessment before deploying derived models.
+Cost considerations:
+• Dataset itself is open access (no cost).
+• Small-scale applications (e.g., testing models in Google Earth Engine or QGIS) incur negligible costs.
+• Larger-scale ML training and national-scale mapping may require cloud compute budgets
+• Train and validate machine learning models for cocoa farm detection, deforestation monitoring, and land use classification.
+• Use as a benchmark dataset to evaluate remote sensing products in heterogeneous tropical landscapes.
+How to extend or improve: 
+• Add new field reference data from other cocoa-producing regions (e.g., Côte d’Ivoire, Nigeria) to increase transferability.</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>CC-BY 4.0</t>
+        </is>
+      </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Powered by:  [ADD!!!]
+          <t>Powered by:  WRI, CERSGIS, NASA SERVIR, Earth System Science Center
 Catalyzed by: Lacuna-Fund / Meridian (Climate-call) &amp;  FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Jonas Nothnagel</t>
+        </is>
+      </c>
       <c r="R16" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr"/>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>Computer Vision</t>
+        </is>
+      </c>
       <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quote: “We are extremely grateful to Lacuna Fund and are delighted that our reference data collection effort will contribute immensely to an evolving data ecosystem to set up scalable machine learning applications for monitoring land-use change in cocoa-forest mosaic landscapes. Led by the Centre for Remote Sensing and Geographic Services (CERSGIS) and supported by researchers from the Centre for Climate Change and Sustainability Studies University of Ghana, International Crops Research Institute for the Semi-Arid Tropics (ICRISAT), Boston University, and the University of Alabama in Huntsville through SERVIR West Africa and the SERVIR Global network, this work will leverage the local knowledge of youth and community members for science-based participatory data collection. This data will provide critical input for enabling the transformation of commodity-driven supply chain traceability and commercial opportunities for ecosystem sustainability.  
+— Foster Mensah Center for Remote Sensing and Geographic Information Services University of Ghana </t>
+        </is>
+      </c>
       <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr"/>
     </row>
@@ -1499,18 +1896,34 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Remote sensing and weather dataset for improved reforestation monitoring</t>
+          <t>Supporting reforestation in Kenya through AI-powered monitoring of trees</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>This project developed a efficient AI-powered method and dataset for monitoring of trees in forests in Kenya. Accurate tree crown detection and other parameters will support reforestation efforts in several ways: The datasets enable the development of tools that can rapidly assess the success of reforestation efforts by enabling counting of trees, estimation of trees’ biophysical parameters from drone images, and prediction of tree growth in relation to tree species and weather variables. The data consists of a high-resolution dataset of drone imagery, ground truth tree parameter measurements, and aggregate weather data from a large, reforested area in Kenya.</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>[not yet published]</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Life on Land (SDG 15): sustainably manage forests, halt and reverse land degradation and halt biodiversity loss.</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Geospatial, Images</t>
+        </is>
+      </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Dedan Kimathi University of Technology,Data Science Africa</t>
+          <t>Prof. Ciira Maina, Centre for Data Science and Artificial Intelligence, Dedan Kimathi University of Technology</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1520,29 +1933,52 @@
       </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Effective forest management and conservation require monitoring tree attributes such as height, crown diameter, and tree count to assess growth in reforested areas. These data enable the development of tools that can speed up the process to assess the success of reforestation efforts and other various ecological and forestry applications, including biomass estimation, forest health assessment, and carbon sequestration studies. Such tools could include the automated counting of trees, estimation of trees’ biophysical parameters from drone images such as tree crown diameter, and prediction of tree growth in relation to tree species and weather variables. In all these areas, AI can offer a cost-effective and scalable alternative to traditional methods of monitoring and counting.
+Concretely the following areas of restoration can be improved:
+1) Planning - create baseline assessment: By automatically detecting existing tree crowns, tools based on this dataset can create a baseline assessment of the current forest cover. This information is valuable for planning and prioritizing reforestation areas.
+2) Monitor Progress: Repeated application of the tree crown detection model can track the success of reforestation initiatives. The model can quantify the increase in tree cover over time, allowing for informed adjustments to reforestation strategies.</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>https://creativecommons.org/licenses/by/4.0/</t>
+        </is>
+      </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Powered by:  [ADD!!!]
+          <t>Powered by:  Dedan Kimathi University of Technology, Kenya
 Catalyzed by: Lacuna-Fund / Meridian (Climate-call) &amp;  FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
       </c>
-      <c r="Q17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Balthas Seibold</t>
+        </is>
+      </c>
       <c r="R17" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="S17" t="inlineStr"/>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
-      <c r="V17" t="inlineStr"/>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>https://www.dw.com/en/artificial-intelligence-boosts-kenyas-forestry-conservation/video-69618432, https://dekut-dsail.github.io/projects/treedetection.html, https://agu.confex.com/agu/agu24/meetingapp.cgi/Paper/1728502, https://ieeexplore.ieee.org/document/11060524</t>
+        </is>
+      </c>
       <c r="W17" t="inlineStr"/>
       <c r="X17" t="inlineStr">
         <is>
-          <t>Is this from Lacuna? (DB).    yes (JN)</t>
+          <t>Original title: Remote sensing and weather dataset for improved reforestation monitoring</t>
         </is>
       </c>
     </row>
@@ -1555,14 +1991,26 @@
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>DATASETS FOR PREDICTION OF LAND USE/COVER CHANGES IN UGANDA</t>
+          <t>Combatting deforestation &amp; supporting natural resource management in Uganda through satellite imagery AI-datasets and National Forestry Inventory AI-datasets</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Deforestation is a significant contributor to changes in land use/cover in Uganda. This challenge is intensified by agriculture’s extreme vulnerability to climate change. This project has generated datasets that can be utilized to predict land cover types or changes for informed decision-making in natural resource management. The data is accessible, quality satellite imagery datasets and National Forestry Inventory datasets.  Specifically, Sentinel 2 and Hansen tree cover image datasets have been augmented with the inclusion of inventory datasets. A biomass mean stock per hectare dataset for each vegetation type has also been acquired. Annotation procedures of the different datasets allow for machine learning tasks. </t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>[not yet published]</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Life on Land (SDG 15): sustainably manage forests, halt and reverse land degradation and halt biodiversity loss.</t>
+        </is>
+      </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
@@ -1576,27 +2024,49 @@
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The land use/cover change datasets improve the understanding of the relationship between land cover/land use change and climate change. The can also be used to inform practice and policy on how best to manage various potential scenarios and combat deforestation.        </t>
+        </is>
+      </c>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Powered by:  [ADD!!!]
+          <t>Powered by: Makerere University in cooperation with the Uganda National Forestry Authority (NFA)
 Catalyzed by: Lacuna-Fund / Meridian (Climate-call) &amp;  FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Balthas Seibold</t>
+        </is>
+      </c>
       <c r="R18" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="S18" t="inlineStr"/>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>Dataset &gt; Model</t>
+        </is>
+      </c>
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
-      <c r="V18" t="inlineStr"/>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quote: “With funding from Lacuna Fund, satellite image and forest inventory datasets will help to develop machine learning models for prediction of land cover types or changes for informed decision-making in natural resource management. Under joint research from Makerere College of Agriculture and Environment Studies and Makerere AI Health Lab, and in partnership with the National Forestry Authority, Uganda, our land use/cover change datasets will improve our understanding of the relationship between land cover/land use change and climate change. It will also be useful in informing practice and policy on how best to manage various potential scenarios. 
+— Dr. Sarah Akello, College of Agriculture and Environmental Sciences, Makerere University 
+</t>
+        </is>
+      </c>
       <c r="W18" t="inlineStr"/>
-      <c r="X18" t="inlineStr"/>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>original title: DATASETS FOR PREDICTION OF LAND USE/COVER CHANGES IN UGANDA</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1611,11 +2081,27 @@
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Extensive bioinformatics resource that leverages tree species’ medicinal, food provision, and other trait data, together with southern African trees’ climate relationships and growth characteristics for climate adaptation and mitigation planning.  The data can serve to promote the use of indigenous trees for reforestation, regenerative agriculture, ecological restoration, human health and livelihood support, and urban afforestation programs to adapt to and mitigate the impacts of climate change.</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>[not yet published]</t>
+        </is>
+      </c>
       <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Life on Land (SDG 15): sustainably manage forests</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Images, Tabular, </t>
+        </is>
+      </c>
       <c r="J19" t="inlineStr">
         <is>
           <t>University of Stellenbosch</t>
@@ -1623,32 +2109,57 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Angola,DRC,Germany,Kenya,Mozambique,Nigeria,South Africa,Tanzania,United Kingdom,Zambia</t>
+          <t>Angola, DRC, Kenya, Mozambique, Nigeria, South Africa,Tanzania, Zambia</t>
         </is>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>The primary application of this work will include identifying indigenous species that can enhance ecological resilience by mapping adaptation and mitigation opportunities and assessing climate risks to African trees. Existing cutting-edge functional niche modeling will allow for the identification of areas for optimal use of African trees based on the results of tree growth performance. This will promote the use of indigenous trees for reforestation, regenerative agriculture, ecological restoration, human health and livelihood support, and urban afforestation programs to adapt to and mitigate the impacts of climate change.</t>
+        </is>
+      </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Powered by:  [ADD!!!]
+          <t>Powered by:  [Stellenbosch University]
 Catalyzed by: Lacuna-Fund / Meridian (Climate-call) &amp;  FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Luisa Olaya</t>
+        </is>
+      </c>
       <c r="R19" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="S19" t="inlineStr"/>
-      <c r="T19" t="inlineStr"/>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>Computer Vision/Picture data</t>
+        </is>
+      </c>
       <c r="U19" t="inlineStr"/>
-      <c r="V19" t="inlineStr"/>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>Quote: "We are excited that Lacuna Fund has provided Stellenbosch, and our team, with the opportunity to utilize these datasets to enable researchers to model the impacts of indigenous trees for adaptation and mitigation to climate change in southern Africa. This information is of the utmost importance in ensuring the continent can build resilience against the rapid unfolding of climate change which is affecting livelihoods and demanding that we find solutions.” 
+— Professor Guy Midgley, Acting Director at School for Climate Studies, Stellenbosch University</t>
+        </is>
+      </c>
       <c r="W19" t="inlineStr"/>
-      <c r="X19" t="inlineStr"/>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>First Editing done by Luisa 28.08.2027</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1659,18 +2170,34 @@
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Datasets to understand mangroves health in relationship to climate change</t>
+          <t>Mangroves Protection in West Africa through AI-powered monitoring of mangrove health - Benin Mangroves Open Data (BeMOD)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mangroves are valuable coastal ecosystems, providing diverse services to humans and playing a critical role in the global strategy to mitigate impacts of climate change. Regular monitoring of their conditions is essential to provide evidence that supports timely decisions for their management. The “Benin Mangroves Open Data (BeMOD)” project generated annotated images, observations on water quality, observations on soil characteristics, climate observations, forest inventories data (tree diversity, canopy height and cover, tree diameter, total height, biomass, etc.) from plots, and data on socio-cultural contexts (e.g., uses, activities) of mangroves in multiple sites in Benin. </t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>[not yet published]</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>climate action (SDG 13), clean water (SDG 6), Life below water (SDG 14), Life on land / biodiversity (SDG 15)</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Images, Tabular, </t>
+        </is>
+      </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>"Laboratory of Biomathematics and Forest Estimations, University of Abomey-Calavi"</t>
+          <t>Romain Lucas        Glèlè Kakaï, Laboratory of Biomathematics and Forest Estimations, University of Abomey-Calavi (glele.romain@gmail.com or romain.glelekakai@fsa.uac.bj)</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1680,27 +2207,48 @@
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This datasets can be used to build systems for faster, more regular monitoring of mangrove conditions. This is essential to provide evidence that supports timely decisions for mangrove management and mitigate the outcomes of climate change.
+</t>
+        </is>
+      </c>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Powered by:  [ADD!!!]
+          <t>Powered by: University of Abomey-Calavi, Republic of Benin 
 Catalyzed by: Lacuna-Fund / Meridian (Climate-call) &amp;  FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
       </c>
-      <c r="Q20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Balthas Seibold</t>
+        </is>
+      </c>
       <c r="R20" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="S20" t="inlineStr"/>
-      <c r="T20" t="inlineStr"/>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>Computer Vision/Picture data</t>
+        </is>
+      </c>
       <c r="U20" t="inlineStr"/>
       <c r="V20" t="inlineStr"/>
       <c r="W20" t="inlineStr"/>
-      <c r="X20" t="inlineStr"/>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>Original title: Datasets to understand mangroves health in relationship to climate change</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1708,21 +2256,44 @@
           <t>ui_74</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Advancing oil palm mapping with social forestry and machine learning</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Advancing oil palm mapping with social forestry and machine learning</t>
+          <t>Mitigating the impacts of oil palm cultivation on forests and climate change in Indonesia through AI and social forestry</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>This dataset contributes to improved understanding and mitigation of the impacts of oil palm cultivation on forests and climate change. It can also serve to support sustainable forest management practices and empower local communities in forest resource management. 
+The project created open and accessible training and evaluation datasets for machine learning applications focused on forest cover and change in Indonesia. It contains collections of polygons of uniform land cover, with labels indicating land cover type and, possibly, information on land cover change over time. To label land cover patches, the team has reviewed high-resolution satellite imagery facilitated by Collect Earth Online (CEO) and augmented it with field visits to difficult-to-classify areas. It has prioritized areas with significant landcover diversity with a preference for areas with significant smallholder production of  oil palm, coconut, and other commodities - given the well-known difficulties of distinguishing oil palm 
+from coconut palm with lower resolution imagery.
+Possible users of these outputs are local communities engaged in community forestry in Indonesia, as well as researchers, policymakers, and civil society organizations. The dataset also contributes to social forestry, which recognizes that people who depend on local forests are best placed to look after them, and that allowing communities to manage and use forest resources can have positive social, environmental and economic impacts. Social forestry is a broad term and has different names in different places. Some examples are community forestry, village forestry, participatory forestry, community-based forest management and people-centred forestry.</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>[not yet published]</t>
+        </is>
+      </c>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Climate action (SDG 13), Life on Land (SDG 15): sustainably manage forests, halt and reverse land degradation and halt biodiversity loss.</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Geospacial,  land cover information, metadata, satellite imagery</t>
+        </is>
+      </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>RECOFTC</t>
+          <t>RECOFTC, Peter Cutter (peter.cutter@recoftc.org)</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1732,25 +2303,51 @@
       </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>This dataset can help you to get an improved understanding of the impacts of oil palm cultivation on forests and climate change. It can also serve to support sustainable forest management practices and empower local communities in forest resource management.</t>
+        </is>
+      </c>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Powered by:  [ADD!!!]
+          <t>Powered by:  RECOFTC
 Catalyzed by: Lacuna-Fund / Meridian (Climate-call) &amp;  FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>Balthas Seibold</t>
+        </is>
+      </c>
       <c r="R21" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="S21" t="inlineStr"/>
-      <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr"/>
-      <c r="V21" t="inlineStr"/>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>Earth Observation/Satellite&amp; drone data</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>https://www.recoftc.org/sites/default/files/styles/image_scale_w1024/public/2025-03/dji_0037.jpg.webp?itok=l0ilgQi8</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://www.recoftc.org/projects/advancing-oil-palm-mapping-social-forestry-and-machine-learning 
+Quote: “Communities in the areas targeted by this project are challenged when it comes to mapping the rapidly changing forest landscapes on which they depend. The datasets this project generates will provide valuable insight into these dynamic patterns of change.”  
+— Gamma Galudra, Director, Indonesia Country Office, RECOFTC </t>
+        </is>
+      </c>
       <c r="W21" t="inlineStr"/>
       <c r="X21" t="inlineStr"/>
     </row>
@@ -1802,7 +2399,13 @@
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
-      <c r="V22" t="inlineStr"/>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quote: “Lacuna Fund will be instrumental in supporting the development of an MRV system that will enable us to participatorily map the health of forests in the biodiverse Eastern Himalayan region with indigenous communities, facilitating targeted interventions for climate resilience through forest management – impacting the millions of people that depend on forests for their lives and livelihoods in the Eastern Himalayas.”  
+— Michael Dawson, Rural Futures – Anthropological Visioner, Balipara Foundation 
+</t>
+        </is>
+      </c>
       <c r="W22" t="inlineStr"/>
       <c r="X22" t="inlineStr"/>
     </row>
@@ -1822,7 +2425,11 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
+        </is>
+      </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
@@ -1854,7 +2461,12 @@
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr"/>
-      <c r="V23" t="inlineStr"/>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quote: “The Lacuna-funded Agro4Resilience Project offers Kenyan farmers and decision makers a pathway for informed decision-making that supports tree cover increase. It will also improve agricultural productivity and mitigate climate change effects through ecosystem services.” 
+— David Makori, International Centre of Insect Physiology and Ecology (ICIPE)  </t>
+        </is>
+      </c>
       <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr"/>
     </row>
@@ -1883,7 +2495,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Columbia</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="L24" t="inlineStr"/>
@@ -1906,7 +2518,12 @@
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
       <c r="U24" t="inlineStr"/>
-      <c r="V24" t="inlineStr"/>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quote: “The dataset compiled during the project will facilitate accurate AGB and AGC estimation in Colombian Caribbean mangroves, enabling better understanding of carbon storage and supporting conservation and management efforts. It will also provide a valuable resource for future research and monitoring activities related to these important coastal ecosystems. Furthermore, the methodology developed in this project might even be applied beyond the Colombian Caribbean to other mangrove ecosystems with similar structures.”  
+— María Cuevas-González, Geomatics Research Unit, Centre Tecnològic de Telecomunicacions de Catalunya (CTTC)  </t>
+        </is>
+      </c>
       <c r="W24" t="inlineStr"/>
       <c r="X24" t="inlineStr"/>
     </row>
@@ -1958,7 +2575,12 @@
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
-      <c r="V25" t="inlineStr"/>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>Quote: “The threat of climate change on forest health affects leaf, flower, and fruit resource availability, but we cannot be prepared unless we have adequate data with predictive power. We have an incredible opportunity to create a harmonized machine-learning-ready dataset for ecological forecasting with the support of Lacuna Fund. Such a forecast could provide the basis for an early warning system that will help communities and resource managers better plan and prepare for climate change impact on forest resources.”
+— Bismark Ofosu-Bamfo, Department of Biological Sciences, University of Energy and Natural Resources</t>
+        </is>
+      </c>
       <c r="W25" t="inlineStr"/>
       <c r="X25" t="inlineStr"/>
     </row>
@@ -2110,7 +2732,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Climate Action, Agriculture</t>
+          <t>Climate Action, End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2208,7 +2830,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Agriculture</t>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2279,18 +2901,19 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Leverage Sentinel-2 Satellite Data to predict biomass in cocoa plantations in Cote d'Ivoire
+          <t xml:space="preserve">Detectinging forest degradation by predicting biomass in cocoa plantations in Cote d'Ivoire
 </t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Leveraging ML to predict above-ground biomass in cocoa plantations in Cote d'Ivoire</t>
+          <t xml:space="preserve">Detectinging forest degradation by predicting biomass in cocoa plantations in Cote d'Ivoire
+</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>This dataset and the models developed from it aim to predict biomass levels in shaded regions of Côte d'Ivoire using a combination of GEDI, Sentinel-2 satellite imagery, and ground truth biomass measurements. The resulting models enable efficient and cost-effective remote monitoring of biomass changes, crucial for assessing reforestation success and detecting forest degradation due to cocoa farming, reducing the need for extensive on-the-ground surveys.</t>
+          <t xml:space="preserve">The AI model based on this dataset enables efficient and cost-effective remote monitoring of biomass changes. This is crucial for assessing reforestation success and detecting forest degradation due to cocoa farming. Also it reduces the need for extensive and expensive on-the-ground surveys. The dataset and the models developed from it aim to predict biomass levels in shaded regions of Côte d'Ivoire using a combination of GEDI, Sentinel-2 satellite imagery, and ground truth biomass measurements. </t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2301,7 +2924,7 @@
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Climate Action</t>
+          <t>climate action (SDG 13), Life on Land (SDG 15): sustainably manage forests, halt and reverse land degradation and halt biodiversity loss.</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2452,7 +3075,7 @@
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Explore the effectiveness of Agrivoltaic farming systems to optimize productivity of farmlands</t>
+          <t>Optimizing productivity of farmlands by AI-powered enhancement of the effectiveness of Agrivoltaic farming systems</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2473,7 +3096,7 @@
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Agriculture, Climate Action, Energy</t>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2), Climate Action, Energy</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2586,7 +3209,11 @@
           <t>Innovate Africa Challenge AI for Climate Action,</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>[note this is a bundle of applications - to be divided and checked] Climate Smart Agriculture in Africa: eight AI applications supported through the "Innovate Africa Challenge", e.g. real-time weather forecasts, solar-powered AI robots for crop pest detections, AI forcasting natural disasters, AI-powered farming advise, high-yield farming in fish and vegetables</t>
+        </is>
+      </c>
       <c r="D33" t="inlineStr">
         <is>
           <t>[note this is a bundle of applications - to be divided and checked] Climate Smart Agriculture in Africa: eight AI applications supported through the "Innovate Africa Challenge", e.g. real-time weather forecasts, solar-powered AI robots for crop pest detections, AI forcasting natural disasters, AI-powered farming advise, high-yield farming in fish and vegetables</t>
@@ -2642,7 +3269,11 @@
           <t>Scaling Language AI: 4 Billion Conversations with CLEAR Global</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr"/>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Providing a toolbox to build chatbots in African languages</t>
+        </is>
+      </c>
       <c r="D34" t="inlineStr">
         <is>
           <t>Providing a toolbox to build chatbots in African languages</t>
@@ -2708,7 +3339,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Maybe catchy project title?</t>
+          <t>Supporting Pan-African research Networks on natural language processing (Masakhane)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -2780,7 +3411,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TBC</t>
+          <t>Our language, our data: Co-creating equitable governance models with African language communities - language dataset creatd: Dhuluo</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2879,7 +3510,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), Achieve Gender Equality (SDG 5), End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2962,18 +3593,18 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Open-source text-to-speech datasets in 9 Indian languages (Hindi | Bengali | Marathi | Telugu | Bhojpuri | Kannada | Magadhi | Chhattisgarhi | Maithili)</t>
+          <t>Making AI speak 9 Indian languages: Hindi, Bengali, Marathi, Telugu, Bhojpuri, Kannada, Magadhi, Chhattisgarhi, Maithili - Open-source text-to-speech datasets</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Build inclusive voice technologies in 9 Indian Languages through open language datasets</t>
+          <t>Making AI speak 9 Indian languages: Hindi, Bengali, Marathi, Telugu, Bhojpuri, Kannada, Magadhi, Chhattisgarhi, Maithili - Open-source text-to-speech models</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
           <t>This dataset is part of the initiative SYSPIN (SYnthesizing SPeech in INdian languages), that develops large open-source Text-to-Speech (TTS) corpora, i.e., speech training datasets and AI models in 9 Indian languages, namely – Bengali, Bhojpuri, Chhattisgarhi, Hindi, Kannada, Magahi, Maithili, Marathi, and Telugu. This data is useful for those wishing to build voice-enabled, user-friendly applications in Indian languages. Through voice-based solutions, these AI models can be used to empower communities that do not have access to digital services in their own native language. They can be used by private companies, researchers, NGOs or government departments to develop digital applications. 
- The datasets and TTS models are available to the AI community and anyone wishing to build voice-enabled applications in Indian languages.</t>
+ The datasets and TTS models are available to the AI community and anyone wishing to build voice-enabled applications in Indian languages. Given the distribution of speakers. some of the languages are especially useful for programmes wishing to engage with rural communities and promote sustainable agriculture in rural settings.</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2988,7 +3619,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -3032,7 +3663,8 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>The TTS models can be used to develop innovative solutions and voice-based services for Indians in their native language. This would be especially beneficial for those who cannot read/write or have speech and visual disabilities but can access digital services through audio/voice-based mediums. The data and models are a crucial stepping stone for developing such assistive technologies. Including low-resource languages, some of which do not even have enough print/digital literature, would benefit vulnerable communities for whom language barriers make access to technological solutions even more difficult. The 720 hours of open-source TTS data also present immense opportunities for academic and industrial research.</t>
+          <t xml:space="preserve">The TTS models can be used to develop innovative solutions and voice-based services for Indians in their native language. This would be especially beneficial for those who cannot read/write or have speech and visual disabilities but can access digital services through audio/voice-based mediums. The data and models are a crucial stepping stone for developing such assistive technologies. Including low-resource languages, some of which do not even have enough print/digital literature, would benefit vulnerable communities for whom language barriers make access to technological solutions even more difficult. Given the distribution of speakers. some of the languages are especially useful for programmes wishing to engage with rural communities and promote sustainable agriculture in rural settings. The 720 hours of open-source TTS data also present immense opportunities for academic and industrial research.
+You can directly access and use the models on Bashini here via web and API: https://anuvaad.bhashini.gov.in/ </t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
@@ -3115,7 +3747,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Agriculture</t>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -3442,7 +4074,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Agriculture, Climate Action</t>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2), Climate Action</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -3533,7 +4165,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Support Sustainable Agriculture in Telangana through AI-powered Crop Identification and Crop Health Prediction</t>
+          <t>https://github.com/pranavmyname/zindi_crop_health; https://zindi.africa/competitions/telangana-crop-health-challenge</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -3553,7 +4185,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Agriculture, Climate Action</t>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2), Climate Action</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -3643,7 +4275,11 @@
           <t>Developing a concept with MFIN on voice-based chatbot</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr"/>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>MicroFinance Industry Network India use of voice technology (Gramvaani)</t>
+        </is>
+      </c>
       <c r="D44" t="inlineStr">
         <is>
           <t>MicroFinance Industry Network India use of voice technology (Gramvaani)</t>
@@ -3845,7 +4481,11 @@
       </c>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
+        </is>
+      </c>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr">
@@ -3896,7 +4536,11 @@
           <t>Two Al-based dialogue systems (e.g. voice-based chatbot) in Indian Languages - consultancy for design implementation etc</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr"/>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Voice-based advisory for farmers (female kitchen gardeners) with NiceSSM / Use Case Gramvaani</t>
+        </is>
+      </c>
       <c r="D47" t="inlineStr">
         <is>
           <t>Voice-based advisory for farmers (female kitchen gardeners) with NiceSSM / Use Case Gramvaani</t>
@@ -3960,7 +4604,11 @@
           <t>Making the Indian voice datasets more sustainable: Hackathon with Bhashini on voice data for climate &amp; sustainable agriculture</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr"/>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Hack4TTS: Crafting Voice for India’s Low-Resource Languages - Building TTS Systems for Low-Resource Indian Languages with Accent and Style Transfer</t>
+        </is>
+      </c>
       <c r="D48" t="inlineStr">
         <is>
           <t>Hack4TTS: Crafting Voice for India’s Low-Resource Languages - Building TTS Systems for Low-Resource Indian Languages with Accent and Style Transfer</t>
@@ -4032,7 +4680,11 @@
           <t>Use case development Indonesia</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr"/>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Climate Disinformation in Local Indonesian Languages</t>
+        </is>
+      </c>
       <c r="D49" t="inlineStr">
         <is>
           <t>Climate Disinformation in Local Indonesian Languages</t>
@@ -4140,7 +4792,11 @@
           <t>HCSA: High Carbon Stock Mapping in Southeast Asia</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr"/>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Forest Forward: Using AI to protect forests and combat the climate crisis in Indonesia by maping carbon using "High Carbon Stock Approach"</t>
+        </is>
+      </c>
       <c r="D50" t="inlineStr">
         <is>
           <t>Forest Forward: Using AI to protect forests and combat the climate crisis in Indonesia by maping carbon using "High Carbon Stock Approach"</t>
@@ -4163,7 +4819,7 @@
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Climate Action</t>
+          <t>Climate action SDG 13, Life on Land (SDG 15): sustainably manage forests, halt and reverse land degradation and halt biodiversity loss.</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -4269,7 +4925,7 @@
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -4404,7 +5060,11 @@
           <t>Early Warning System LDRI</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr"/>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Early Warning System: Advisory services on climate-smart farming for small-holder farmers</t>
+        </is>
+      </c>
       <c r="D53" t="inlineStr">
         <is>
           <t>Early Warning System: Advisory services on climate-smart farming for small-holder farmers</t>
@@ -4419,7 +5079,7 @@
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -4514,7 +5174,11 @@
           <t>Office of Data Protection Commission (ODPC) Chatbot Kenya</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr"/>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Citizen chatbot of the Kenyan Office of the Data Protection Commissioner</t>
+        </is>
+      </c>
       <c r="D54" t="inlineStr">
         <is>
           <t>Citizen chatbot of the Kenyan Office of the Data Protection Commissioner</t>
@@ -4600,17 +5264,17 @@
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Open voice datasets for Kiswahili, Kinyarwanda and Luganda</t>
+          <t>Making AI understand 3 East African languages:  Kiswahili, Kinyarwanda and Luganda - Open-source text-to-speech datasets</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Crowdsourcing open voice datasets for Kiswahili, Kinyarwanda and Luganda</t>
+          <t>Making AI understand 3 East African languages:  Kiswahili, Kinyarwanda and Luganda - Open-source text-to-speech datasets</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t xml:space="preserve">By collecting more than 1000 hours of AI voice data (by 04/2025), this effort created the largest open-source voice dataset of diverse Swahili speakers for speech recognition (speech-to-text). You can use this resource to build AI systems understanding spoken Swahili e.g. in cellphones . This facilitates access to information in mother tongue, including by illiterate persons. </t>
+          <t>By collecting more than 1000 hours of AI voice data (by 04/2025), this effort created the largest open-source voice dataset of diverse Swahili speakers for speech recognition (speech-to-text). You can use this resource to build AI systems understanding spoken Swahili e.g. in cellphones . This facilitates access to information in mother tongue, including by illiterate persons and persons in rural settings.</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4621,7 +5285,7 @@
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -4683,7 +5347,11 @@
         </is>
       </c>
       <c r="W55" t="inlineStr"/>
-      <c r="X55" t="inlineStr"/>
+      <c r="X55" t="inlineStr">
+        <is>
+          <t>Original title: Open voice datasets for Kiswahili, Kinyarwanda and Luganda</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -4696,7 +5364,11 @@
           <t>AIEP MVP Development</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr"/>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Providing farmers in Kenya and Bihar, India with high-quality, personalized information through AI and developing blueprints for AI-powered Agriculture Information Exchange Platforms</t>
+        </is>
+      </c>
       <c r="D56" t="inlineStr">
         <is>
           <t>Providing farmers in Kenya and Bihar, India with high-quality, personalized information through AI and developing blueprints for AI-powered Agriculture Information Exchange Platforms</t>
@@ -4722,7 +5394,7 @@
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -4732,7 +5404,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Digital Green, Viamo and Partners, Tech for Her</t>
+          <t>Digital Green, Viamo and Partners, Tech for Her, DynAg, Digifarm, Opportunity International</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4783,7 +5455,11 @@
           <t>Support Mozilla Swahili grantee</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr"/>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Paza Sauti - chatbot and IVR service in Swahili to raise awareness about the use of collateral (security) to access credit for women in Kenya</t>
+        </is>
+      </c>
       <c r="D57" t="inlineStr">
         <is>
           <t>Paza Sauti - chatbot and IVR service in Swahili to raise awareness about the use of collateral (security) to access credit for women in Kenya</t>
@@ -4798,7 +5474,7 @@
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), Achieve Gender Equality (SDG 5), End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -4863,7 +5539,11 @@
           <t>Building Kenya Language Corpus incl. governance model</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr"/>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Building Kenya Language Corpus incl. governance model</t>
+        </is>
+      </c>
       <c r="D58" t="inlineStr">
         <is>
           <t>Building Kenya Language Corpus incl. governance model</t>
@@ -4935,15 +5615,20 @@
           <t>AI Conversational Chatbot (with GovStack)</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr"/>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Hello, government - better citizen services in Kenya through "AI Chatbots" as a replicable open-source building block</t>
+        </is>
+      </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Hello, government - better citizen services through "AI Chatbots" as a digital public good</t>
+          <t>Hello, government - better citizen services in Kenya through "AI Chatbots" as a replicable open-source building block</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>There is a significant opportunity to make digitized government services in Kenya more easily discoverable and, by extension, enhance their accessibility and use by citizens through chatbot technology. Based on NLP technology, chatbots can help citizens access information on Kenya’s eGovernment services through text and voice inputs in Kiswahili and English. This project foresees the development of an AI Conversational Chatbot using the GovStack Building Block Approach - so as to create (a) a chatbot for easier service discoverability; and (b) a chatbot framework that can be reused as a digital public good.</t>
+          <t xml:space="preserve">There is a significant opportunity to make digitized government services in Kenya more easily discoverable and, by extension, enhance their accessibility and use by citizens through chatbot technology. Based on NLP technology, chatbots can help citizens access information on Kenya’s eGovernment services through text and voice inputs in Kiswahili and English. This project foresees the development of an AI Conversational Chatbot using the GovStack Building Block Approach - so as to create (a) a chatbot for easier service discoverability; and (b) a chatbot framework that can be reused as a digital public good. 
+</t>
         </is>
       </c>
       <c r="F59" t="inlineStr"/>
@@ -5021,11 +5706,7 @@
           <t>Landslide and flood disaster hotspot monitoring using computer vision in Rwanda</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>to be filled in once data and algorithms are available</t>
-        </is>
-      </c>
+      <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr">
@@ -5091,7 +5772,11 @@
           <t>Expansion of voice data collection and development of use cases [Mozilla]</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr"/>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Services to citizens in Swahili: Paza Sauti - chatbot and interactive voice response service in Swahili for better access to credit for women in Kenya and 5 other AI-powered services in Swahili based on Mozillas Common-Voice dataset</t>
+        </is>
+      </c>
       <c r="D61" t="inlineStr">
         <is>
           <t>Services to citizens in Swahili: Paza Sauti - chatbot and interactive voice response service in Swahili for better access to credit for women in Kenya and 5 other AI-powered services in Swahili based on Mozillas Common-Voice dataset</t>
@@ -5155,7 +5840,11 @@
           <t>Develop Mbaza AI Chatbot for Covid 19 [with Mozilla]</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr"/>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Mbaza Chatbot Rwanda for health related inquiries by citizens</t>
+        </is>
+      </c>
       <c r="D62" t="inlineStr">
         <is>
           <t>Mbaza Chatbot Rwanda for health related inquiries by citizens</t>
@@ -5223,7 +5912,11 @@
           <t>Agriculture chatbot / early warning system for farmers / AI entrepreneurship competition</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr"/>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Better Advise to farmers in Rwanda through Agricultural chatbot (Mbaza Chatbot scaling)</t>
+        </is>
+      </c>
       <c r="D63" t="inlineStr">
         <is>
           <t>Better Advise to farmers in Rwanda through Agricultural chatbot (Mbaza Chatbot scaling)</t>
@@ -5234,7 +5927,7 @@
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I63" t="inlineStr"/>
@@ -5283,7 +5976,11 @@
           <t>Bot of Bots Activity - in collaboration with Govstack for Kenya</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr"/>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Hello, government - better citizen services through "AI Chatbots" as a digital public good</t>
+        </is>
+      </c>
       <c r="D64" t="inlineStr">
         <is>
           <t>Hello, government - better citizen services through "AI Chatbots" as a digital public good</t>
@@ -5352,7 +6049,7 @@
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve">This effort created the largest open-source voice dataset of diverse Kinyarwanda speakers for speech recognition (speech-to-text). It collected more than 2300  hours of AI voice data in Kinyarwanda (by 04/2025). You can use this resource to build AI systems understanding spoken Kinyarwanda e.g. in cellphones . This facilitates access to information in mother tongue, including by illiterate persons. </t>
+          <t xml:space="preserve">This effort created the largest open-source voice dataset of diverse Kinyarwanda speakers for speech recognition (speech-to-text). It collected more than 2300  hours of AI voice data in Kinyarwanda (by 04/2025). You can use this resource to build AI systems understanding spoken Kinyarwanda e.g. in cellphones . This facilitates access to information in mother tongue, including by illiterate persons and in rural settings. </t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5363,7 +6060,7 @@
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
@@ -5425,7 +6122,11 @@
           <t>Kinyarwanda Screen Reader for visually impaired people</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr"/>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Supporting visually impaired people in Rwanda through a Kinyarwanda Screen Reader</t>
+        </is>
+      </c>
       <c r="D66" t="inlineStr">
         <is>
           <t>Supporting visually impaired people in Rwanda through a Kinyarwanda Screen Reader</t>
@@ -5488,7 +6189,7 @@
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Climate Action, Agriculture, Food Security</t>
+          <t>Climate Action, End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I67" t="inlineStr"/>
@@ -5610,7 +6311,7 @@
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Agriculture, Climate Action, Disaster Risk Management</t>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2), Climate Action, Disaster Risk Management</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
@@ -5719,7 +6420,7 @@
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Agriculture, Disaster Risk Management, SDG 2</t>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2), Disaster Risk Management, SDG 2</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -5820,7 +6521,7 @@
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr">
         <is>
-          <t xml:space="preserve">Agriculture, Disaster Risk Management, SDG 2 </t>
+          <t xml:space="preserve">End hunger, achieve food security, sustainable agriculture (SDG 2), Disaster Risk Management, SDG 2 </t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
@@ -5921,7 +6622,7 @@
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Agriculture, Disaster Risk Management, SDG 2</t>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2), Disaster Risk Management, SDG 2</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
@@ -6022,7 +6723,7 @@
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Agriculture, Disaster Risk Management, SDG 2, SDG 12</t>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2), Disaster Risk Management, SDG 2, SDG 12</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
@@ -6123,7 +6824,7 @@
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Agriculture, Disaster Risk Management, SDG 2</t>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2), Disaster Risk Management, SDG 2</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
@@ -6224,7 +6925,7 @@
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Agriculture, Disaster Risk Management, SDG 2 </t>
+          <t xml:space="preserve">End hunger, achieve food security, sustainable agriculture (SDG 2), Disaster Risk Management, SDG 2 </t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
@@ -6325,7 +7026,7 @@
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Agriculture, Disaster Risk Management, Climate Action, SDG 2</t>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2), Disaster Risk Management, Climate Action, SDG 2</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -6426,7 +7127,7 @@
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Agriculture, Climate Action, SDG 2 </t>
+          <t xml:space="preserve">End hunger, achieve food security, sustainable agriculture (SDG 2), Climate Action, SDG 2 </t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
@@ -6528,7 +7229,7 @@
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Agriculture, SDG 2</t>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2), SDG 2</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
@@ -6629,7 +7330,7 @@
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Agriculture, SDG 2</t>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2), SDG 2</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
@@ -6713,20 +7414,13 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Speaking Data, Speaking Home 
-Mzansi Speaks
-Our voices, our code
-Voices of Mzansi (project title)</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>Making voice data available in all official languages of South Africa as a digital public good - Voices of Mzansi</t>
-        </is>
-      </c>
+          <t>Voices of Mzansi - Making all official languages of South Africa AI-ready: translating the Common-Voice interface &amp; enabling Open-source text-to-speech dataset collection</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Univ of Stellenbosch Grant (Febe de Wet) - Voices of Mzansi project aimed to get South Africa's languages launched on the Mozilla Common Voice platform1. To achieve this aim the Common Voice website had to be translated from English into the other official languages and at least 5 000 sentences had to be collected for each language. The collected sentences have to be available in the open domain under CC-0 licensing. Once a languages is launched, the sentences are used as prompts for speech data collection through the Common Voice platform.</t>
+          <t xml:space="preserve">Univ of Stellenbosch Grant (Febe de Wet) - Voices of Mzansi project aimed to get South Africa's languages launched on the Mozilla Common Voice platform1. To achieve this aim the Common Voice website had to be translated from English into the other official languages and at least 5 000 sentences had to be collected for each language. The collected sentences have to be available in the open domain under CC-0 licensing. Once a languages is launched, the sentences are used as prompts for speech data collection through the Common Voice platform. This unlocks open-source text-to-speech dataset collection and thereby ultimately facilitates access to information in mother tongue, including by illiterate persons and in rural settings. </t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6737,7 +7431,7 @@
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
@@ -6789,7 +7483,11 @@
         </is>
       </c>
       <c r="W80" t="inlineStr"/>
-      <c r="X80" t="inlineStr"/>
+      <c r="X80" t="inlineStr">
+        <is>
+          <t>Original title: Making voice data available in all official languages of South Africa as a digital public good - Voices of Mzansi: Speaking Data, Speaking home</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -6829,7 +7527,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Climate Action, Agriculture</t>
+          <t>Climate Action, End hunger, achieve food security, sustainable agriculture (SDG 2)</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
@@ -6913,7 +7611,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Precision Farming Simplified: Croppie’s AI-Powered Agronomic Advisor</t>
+          <t>Croppie- helping smallholder coffee producers to plan sales, get loans, and trace coffee - AI powered coffee yield prediction</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -6938,7 +7636,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Agriculture, Climate Action</t>
+          <t>End hunger, achieve food security, sustainable agriculture (SDG 2), Climate Action</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
@@ -7007,7 +7705,11 @@
       <c r="U82" t="inlineStr"/>
       <c r="V82" t="inlineStr"/>
       <c r="W82" t="inlineStr"/>
-      <c r="X82" t="inlineStr"/>
+      <c r="X82" t="inlineStr">
+        <is>
+          <t>Alternative title: Precision Farming Simplified: Croppie’s AI-Powered Agronomic Advisor</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -7121,7 +7823,11 @@
           <t>ML-based site identification for MiniGrids in Uganda</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr"/>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Electrification Dashboard for Ugandan government - help to find the best energy sources for villages in Uganda</t>
+        </is>
+      </c>
       <c r="D84" t="inlineStr">
         <is>
           <t>Electrification Dashboard for Ugandan government - help to find the best energy sources for villages in Uganda</t>
@@ -7181,7 +7887,12 @@
           <t>Development of Unbiased AI Models for Solar Irradiance Uganda</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr"/>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Developing AI Models for Estimating Solar Irradiance for
+Improved Solar Energy Planning in Sub-Saharan Africa</t>
+        </is>
+      </c>
       <c r="D85" t="inlineStr">
         <is>
           <t>Developing AI Models for Estimating Solar Irradiance for
@@ -7259,7 +7970,11 @@
           <t>NLP Use Case Strengthening relevance of Auditing reports in Uganda</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr"/>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>NLP Use Case Strengthening relevance of Auditing reports in Uganda</t>
+        </is>
+      </c>
       <c r="D86" t="inlineStr">
         <is>
           <t>NLP Use Case Strengthening relevance of Auditing reports in Uganda</t>
@@ -7417,66 +8132,28 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>ui_80</t>
+          <t>ui_83</t>
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>AI Advisory for Agriculture chatbots</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AI bots that are at least partly open from the AIEP cohorts </t>
-        </is>
-      </c>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>Agriculture, SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
-        </is>
-      </c>
+      <c r="H88" t="inlineStr"/>
       <c r="I88" t="inlineStr"/>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>Digital Green, Viamo, DeHaat, Digifarm, dynAg</t>
-        </is>
-      </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>India, Kenya</t>
-        </is>
-      </c>
+      <c r="J88" t="inlineStr"/>
+      <c r="K88" t="inlineStr"/>
       <c r="L88" t="inlineStr"/>
       <c r="M88" t="inlineStr"/>
       <c r="N88" t="inlineStr"/>
       <c r="O88" t="inlineStr"/>
-      <c r="P88" t="inlineStr">
-        <is>
-          <t>Powered by: Digital Green, Viamo, DeHaat, Digifarm, dynAg
-Catalyzed by: FAIR Forward - AI for All
-Financed by: Gates Foundation</t>
-        </is>
-      </c>
-      <c r="Q88" t="inlineStr">
-        <is>
-          <t>Christian M</t>
-        </is>
-      </c>
+      <c r="P88" t="inlineStr"/>
+      <c r="Q88" t="inlineStr"/>
       <c r="R88" t="inlineStr"/>
-      <c r="S88" t="inlineStr">
-        <is>
-          <t>Dataset  &gt; Model &gt; Pilot &gt; Use-Case</t>
-        </is>
-      </c>
-      <c r="T88" t="inlineStr">
-        <is>
-          <t>NLP</t>
-        </is>
-      </c>
+      <c r="S88" t="inlineStr"/>
+      <c r="T88" t="inlineStr"/>
       <c r="U88" t="inlineStr"/>
       <c r="V88" t="inlineStr"/>
       <c r="W88" t="inlineStr"/>
@@ -7485,70 +8162,28 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>ui_81</t>
+          <t>ui_84</t>
         </is>
       </c>
       <c r="B89" t="inlineStr"/>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Ag sector specific language datasets </t>
-        </is>
-      </c>
+      <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr"/>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>Language datasets in local Indian language collected by AIEP cohort (dynAg)</t>
-        </is>
-      </c>
+      <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr"/>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Agriculture, SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
-        </is>
-      </c>
-      <c r="I89" t="inlineStr">
-        <is>
-          <t>Voice</t>
-        </is>
-      </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>dynAg</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
+      <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
+      <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr"/>
       <c r="M89" t="inlineStr"/>
       <c r="N89" t="inlineStr"/>
       <c r="O89" t="inlineStr"/>
-      <c r="P89" t="inlineStr">
-        <is>
-          <t>Powered by: dynAg
-Catalyzed by: FAIR Forward - AI for All
-Financed by: Gates Foundation</t>
-        </is>
-      </c>
-      <c r="Q89" t="inlineStr">
-        <is>
-          <t>Christian M</t>
-        </is>
-      </c>
+      <c r="P89" t="inlineStr"/>
+      <c r="Q89" t="inlineStr"/>
       <c r="R89" t="inlineStr"/>
-      <c r="S89" t="inlineStr">
-        <is>
-          <t>Dataset &gt; Model &gt; Pilot</t>
-        </is>
-      </c>
-      <c r="T89" t="inlineStr">
-        <is>
-          <t>NLP</t>
-        </is>
-      </c>
+      <c r="S89" t="inlineStr"/>
+      <c r="T89" t="inlineStr"/>
       <c r="U89" t="inlineStr"/>
       <c r="V89" t="inlineStr"/>
       <c r="W89" t="inlineStr"/>
@@ -7557,70 +8192,28 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>ui_82</t>
+          <t>ui_85</t>
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>Vector DB for smallholder agriculture RAG</t>
-        </is>
-      </c>
+      <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>It's a vector DB that has been developed by Tech4Her cohort to map user requests with semantically similar data</t>
-        </is>
-      </c>
+      <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr"/>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>Agriculture, SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
-        </is>
-      </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>DeHaat</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
+      <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr"/>
+      <c r="K90" t="inlineStr"/>
       <c r="L90" t="inlineStr"/>
       <c r="M90" t="inlineStr"/>
       <c r="N90" t="inlineStr"/>
       <c r="O90" t="inlineStr"/>
-      <c r="P90" t="inlineStr">
-        <is>
-          <t>Powered by: DeHaat
-Catalyzed by: FAIR Forward - AI for All
-Financed by: Gates Foundation</t>
-        </is>
-      </c>
-      <c r="Q90" t="inlineStr">
-        <is>
-          <t>Christian M</t>
-        </is>
-      </c>
+      <c r="P90" t="inlineStr"/>
+      <c r="Q90" t="inlineStr"/>
       <c r="R90" t="inlineStr"/>
-      <c r="S90" t="inlineStr">
-        <is>
-          <t>Dataset &gt; Model &gt; Pilot</t>
-        </is>
-      </c>
-      <c r="T90" t="inlineStr">
-        <is>
-          <t>NLP</t>
-        </is>
-      </c>
+      <c r="S90" t="inlineStr"/>
+      <c r="T90" t="inlineStr"/>
       <c r="U90" t="inlineStr"/>
       <c r="V90" t="inlineStr"/>
       <c r="W90" t="inlineStr"/>
@@ -7629,7 +8222,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>ui_83</t>
+          <t>ui_86</t>
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
@@ -7659,7 +8252,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>ui_84</t>
+          <t>ui_87</t>
         </is>
       </c>
       <c r="B92" t="inlineStr"/>
@@ -7689,7 +8282,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>ui_85</t>
+          <t>ui_88</t>
         </is>
       </c>
       <c r="B93" t="inlineStr"/>
@@ -7719,7 +8312,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>ui_86</t>
+          <t>ui_89</t>
         </is>
       </c>
       <c r="B94" t="inlineStr"/>
@@ -7749,7 +8342,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>ui_87</t>
+          <t>ui_90</t>
         </is>
       </c>
       <c r="B95" t="inlineStr"/>
@@ -7779,7 +8372,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>ui_88</t>
+          <t>ui_91</t>
         </is>
       </c>
       <c r="B96" t="inlineStr"/>
@@ -7806,96 +8399,6 @@
       <c r="W96" t="inlineStr"/>
       <c r="X96" t="inlineStr"/>
     </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>ui_89</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr"/>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr"/>
-      <c r="E97" t="inlineStr"/>
-      <c r="F97" t="inlineStr"/>
-      <c r="G97" t="inlineStr"/>
-      <c r="H97" t="inlineStr"/>
-      <c r="I97" t="inlineStr"/>
-      <c r="J97" t="inlineStr"/>
-      <c r="K97" t="inlineStr"/>
-      <c r="L97" t="inlineStr"/>
-      <c r="M97" t="inlineStr"/>
-      <c r="N97" t="inlineStr"/>
-      <c r="O97" t="inlineStr"/>
-      <c r="P97" t="inlineStr"/>
-      <c r="Q97" t="inlineStr"/>
-      <c r="R97" t="inlineStr"/>
-      <c r="S97" t="inlineStr"/>
-      <c r="T97" t="inlineStr"/>
-      <c r="U97" t="inlineStr"/>
-      <c r="V97" t="inlineStr"/>
-      <c r="W97" t="inlineStr"/>
-      <c r="X97" t="inlineStr"/>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>ui_90</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr"/>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="inlineStr"/>
-      <c r="F98" t="inlineStr"/>
-      <c r="G98" t="inlineStr"/>
-      <c r="H98" t="inlineStr"/>
-      <c r="I98" t="inlineStr"/>
-      <c r="J98" t="inlineStr"/>
-      <c r="K98" t="inlineStr"/>
-      <c r="L98" t="inlineStr"/>
-      <c r="M98" t="inlineStr"/>
-      <c r="N98" t="inlineStr"/>
-      <c r="O98" t="inlineStr"/>
-      <c r="P98" t="inlineStr"/>
-      <c r="Q98" t="inlineStr"/>
-      <c r="R98" t="inlineStr"/>
-      <c r="S98" t="inlineStr"/>
-      <c r="T98" t="inlineStr"/>
-      <c r="U98" t="inlineStr"/>
-      <c r="V98" t="inlineStr"/>
-      <c r="W98" t="inlineStr"/>
-      <c r="X98" t="inlineStr"/>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>ui_91</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr"/>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr"/>
-      <c r="E99" t="inlineStr"/>
-      <c r="F99" t="inlineStr"/>
-      <c r="G99" t="inlineStr"/>
-      <c r="H99" t="inlineStr"/>
-      <c r="I99" t="inlineStr"/>
-      <c r="J99" t="inlineStr"/>
-      <c r="K99" t="inlineStr"/>
-      <c r="L99" t="inlineStr"/>
-      <c r="M99" t="inlineStr"/>
-      <c r="N99" t="inlineStr"/>
-      <c r="O99" t="inlineStr"/>
-      <c r="P99" t="inlineStr"/>
-      <c r="Q99" t="inlineStr"/>
-      <c r="R99" t="inlineStr"/>
-      <c r="S99" t="inlineStr"/>
-      <c r="T99" t="inlineStr"/>
-      <c r="U99" t="inlineStr"/>
-      <c r="V99" t="inlineStr"/>
-      <c r="W99" t="inlineStr"/>
-      <c r="X99" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
removed not working links
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -641,11 +641,7 @@
           <t>Extensive bioinformatics resource that leverages tree species’ medicinal, food provision, and other trait data, together with southern African trees’ climate relationships and growth characteristics for climate adaptation and mitigation planning.  The data can serve to promote the use of indigenous trees for reforestation, regenerative agriculture, ecological restoration, human health and livelihood support, and urban afforestation programs to adapt to and mitigate the impacts of climate change.</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>[not yet published]</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
@@ -734,11 +730,7 @@
           <t xml:space="preserve">Mangroves are valuable coastal ecosystems, providing diverse services to humans and playing a critical role in the global strategy to mitigate impacts of climate change. Regular monitoring of their conditions is essential to provide evidence that supports timely decisions for their management. The “Benin Mangroves Open Data (BeMOD)” project generated annotated images, observations on water quality, observations on soil characteristics, climate observations, forest inventories data (tree diversity, canopy height and cover, tree diameter, total height, biomass, etc.) from plots, and data on socio-cultural contexts (e.g., uses, activities) of mangroves in multiple sites in Benin. </t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>[not yet published]</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
removed more missing links
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -930,7 +930,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>GitHub - yangshao2/UrbanInfraDL</t>
+          <t>https://github.com/yangshao2/UrbanInfraDL</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>LULC training data for Ecuador - ML</t>
+          <t>https://www.kaggle.com/datasets/mapbiomasecuador/lulc-training-data-for-ecuador-ml/data</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -3832,11 +3832,7 @@
 Possible users of these outputs are local communities engaged in community forestry in Indonesia, as well as researchers, policymakers, and civil society organizations. The dataset also contributes to social forestry, which recognizes that people who depend on local forests are best placed to look after them, and that allowing communities to manage and use forest resources can have positive social, environmental and economic impacts. Social forestry is a broad term and has different names in different places. Some examples are community forestry, village forestry, participatory forestry, community-based forest management and people-centred forestry.</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>[not yet published]</t>
-        </is>
-      </c>
+      <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
@@ -4414,11 +4410,7 @@
           <t>This project developed a efficient AI-powered method and dataset for monitoring of trees in forests in Kenya. Accurate tree crown detection and other parameters will support reforestation efforts in several ways: The datasets enable the development of tools that can rapidly assess the success of reforestation efforts by enabling counting of trees, estimation of trees’ biophysical parameters from drone images, and prediction of tree growth in relation to tree species and weather variables. The data consists of a high-resolution dataset of drone imagery, ground truth tree parameter measurements, and aggregate weather data from a large, reforested area in Kenya.</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>[not yet published]</t>
-        </is>
-      </c>
+      <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
@@ -5402,7 +5394,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Residential Energy and Weather Data (REWD) - Pakistan</t>
+          <t>https://lei.lums.edu.pk/datasets/residential-energy-and-weather-data-pakistan.html</t>
         </is>
       </c>
       <c r="G57" t="inlineStr"/>
@@ -7432,11 +7424,7 @@
           <t xml:space="preserve">Deforestation is a significant contributor to changes in land use/cover in Uganda. This challenge is intensified by agriculture’s extreme vulnerability to climate change. This project has generated datasets that can be utilized to predict land cover types or changes for informed decision-making in natural resource management. The data is accessible, quality satellite imagery datasets and National Forestry Inventory datasets.  Specifically, Sentinel 2 and Hansen tree cover image datasets have been augmented with the inclusion of inventory datasets. A biomass mean stock per hectare dataset for each vegetation type has also been acquired. Annotation procedures of the different datasets allow for machine learning tasks. </t>
         </is>
       </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>[not yet published]</t>
-        </is>
-      </c>
+      <c r="F79" t="inlineStr"/>
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
checked new url validator
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -4152,11 +4152,7 @@
 NusaDialogue covers 3 underrepresented languages under the Malayo-Polynesian languages group, i.e., Minangkabau (min), Balinese (ban), and Buginese (bug), each consisting of 10,000 dialogue and summary pairs. The dialogues in NusaDialogue encompass numerous topics including culture, occupation, politics, science, history, news, sports, religion, etc</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>prosa-text/nusa-dialogue · Datasets at Hugging Face</t>
-        </is>
-      </c>
+      <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
data clean up & removed unused features: react frontend and analytics
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -637,7 +637,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>SAT-CARe</t>
+          <t>African Trees for Climate Resilience</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -653,7 +653,7 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Life on Land (SDG 15): sustainably manage forests</t>
+          <t>SDG 15</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -663,7 +663,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Professor Guy F Midgley gfmidgley@sun.ac.za University of Stellenbosch</t>
+          <t>Prof. Guy F. Midgley University of Stellenbosch (gfmidgley@sun.ac.za)</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -689,7 +689,7 @@
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Powered by:  [Stellenbosch University]
+          <t>Powered by:  Stellenbosch University
 Catalyzed by: Lacuna-Fund / Meridian (Climate-call) &amp;  FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
@@ -956,7 +956,7 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 10, SDG 2</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -966,7 +966,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Fundación Despacio,World Resources Institute,Fundación Despacio</t>
+          <t>Fundación Despacio (mafe@despacio.org), World Resources Institute</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -989,7 +989,7 @@
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
-          <t>CC-BY 4.0 license</t>
+          <t>CC-BY 4.0</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1063,7 +1063,7 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>SDG 15 (Life of Land)</t>
+          <t>SDG 15</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>María Cuevas (mcuevas@cttc.es / Centre Tecnològic de Telecomunicacions de Catalunya, CTTC, Spain),  Cristian Montes (cristian.montes@invemar.org.co / Instituto de Investigaciones Marinas y Costeras José Benito Vives de Andreis, INVEMAR, Colombia)</t>
+          <t>CTTC María Cuevas (mcuevas@cttc.es),  INVEMAR Cristian Montes (cristian.montes@invemar.org.co)</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1253,7 +1253,7 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>SDG 13 (Climate Action), Life on Land (SDG 15): sustainably manage forests, halt and reverse land degradation and halt biodiversity loss.</t>
+          <t>SDG 13, SDG 15</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Powered by:  
+          <t>Powered by: Data354
 Catalyzed by: FAIR Forward - AI for All (https://www.bmz-digital.global/en/overview-of-initiatives/fair-forward/)
 Financed by: BMZ (https://www.bmz-digital.global/en/digital-transformation-and-development-cooperation/)</t>
         </is>
@@ -1337,9 +1337,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t xml:space="preserve">SDG 7 (Affordable and clean energy)
-SDG 11 (Sustainable cities and communities)
-</t>
+          <t>SDG 7, SDG 11</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1349,7 +1347,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>ESPOL University</t>
+          <t>ESPOL University (jecordov@espol.edu.ec)</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1443,7 +1441,7 @@
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>SDG 13 (Climate Action), Life on Land (SDG 15): sustainably manage forests, halt and reverse land degradation and halt biodiversity loss.</t>
+          <t>SDG 13, SDG 15</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1453,7 +1451,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Fundacion Ecociencia</t>
+          <t>Fundacion Ecociencia (carmenjosse@ecociencia.org)</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1548,19 +1546,15 @@
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SGD 1, 2, 3, 4, 5, 8,10, 13, 15 </t>
-        </is>
-      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Drone Imagery, Text, Voice, Geospatial/Remote Sensing, Images, Meterological, Tabular, Other</t>
+          <t>Voice</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Space4Innovation, Diana Mastracci diana@space4innovation.com</t>
+          <t>Space4Innovation, Diana Mastracci (diana@space4innovation.com)</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1576,7 +1570,6 @@
 This dataset contains Indigenous-labelled bioacoustic recordings from two ecosystems—semi-arid savannah and tropical rainforest—collected through AudioMoth bioacustic sensors. Data include species-specific sounds (e.g., elephants, rodents), environmental background, and associated metadata following the CARE Principles for Indigenous Data Governance.
 Use cases: biodiversity monitoring, species classification, human–wildlife conflict alerts, and AI model training for conservation.
 Limitations: class imbalance (key species overrepresented), environmental noise, and spatial clustering; users should apply noise filtering and ethical review before reuse. These audio data are collected 24/7 when deployed in time periods ranging from hours to several weeks. The data are acquired from multiple microphones spread across the study site. Each microphone has a unique serial number and the geographic locations are provided using GPS. The data are time stamped, however there are data gaps in time and space due to logistics, equipment failure, or power loss. The original data are stored as 16-bit WAV files and are available. To make the data more widely available, they have been uploaded to the Arbimon.org platform. The Arbimon cloud platform is built for bioacoustics analysis using various ML . 
-License: CC BY-NC-SA 4.0 — reuse and adaptation allowed for non-commercial purposes, with attribution and benefit sharing to Indigenous custodians.
 </t>
         </is>
       </c>
@@ -1677,7 +1670,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Dennis Asamoah Owusu (DOWUSU@ASHESI.EDU.GH)</t>
+          <t>Dennis Asamoah Owusu (dowusu@ashesi.edu.gh)</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1764,7 +1757,7 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Life on Land (SDG 15): sustainably manage forests, halt and reverse land degradation and halt biodiversity loss.</t>
+          <t>SDG 15</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1774,7 +1767,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Center for Remote Sensing and Geographic Information Services</t>
+          <t>Center for Remote Sensing and Geographic Information Services CERSGIS (fkmawusi@gmail.com)</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -2003,7 +1996,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -2035,7 +2028,7 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Powered by:  
+          <t>Powered by:  RAIL - KNUST (https://rail.knust.edu.gh/)
 Catalyzed by: FAIR Forward - AI for All (https://www.bmz-digital.global/en/overview-of-initiatives/fair-forward/)
 Financed by: BMZ (https://www.bmz-digital.global/en/digital-transformation-and-development-cooperation/)</t>
         </is>
@@ -2091,7 +2084,7 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -2179,7 +2172,7 @@
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture), Climate Action, Energy</t>
+          <t>SDG 2</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -2267,7 +2260,7 @@
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>SDG 15 (Life of Land)</t>
+          <t>SDG 15</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2381,7 +2374,7 @@
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>SDG 13 (Climate Action), SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2, SDG 13</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2781,7 +2774,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>SDG 13 (Climate Action), Life on Land (SDG 15): sustainably manage forests, halt and reverse land degradation and halt biodiversity loss.</t>
+          <t>SDG 15, SDG 13</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2791,8 +2784,8 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Vertify.earth, Michael Anthony michael@vertify.earth ,
-Alsisar Impact, Saurabh Singhavi saurabh@alsisarimpact.com</t>
+          <t>Vertify.earth - Michael Anthony (michael@vertify.earth), 
+Alsisar Impact - Saurabh Singhavi (saurabh@alsisarimpact.com)</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2899,7 +2892,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), Achieve Gender Equality (SDG 5), SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2, SDG 10, SDG 5</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -3008,7 +3001,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2, SDG 10</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -3136,7 +3129,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -3246,7 +3239,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -3352,7 +3345,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -3463,7 +3456,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture), Climate Action</t>
+          <t>SDG 2</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -3574,7 +3567,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture), Climate Action</t>
+          <t>SDG 2</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -4197,7 +4190,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -4245,7 +4238,7 @@
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Powered by:  
+          <t>Powered by: Bappenas, Prosa AI
 Catalyzed by: FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
@@ -4309,7 +4302,7 @@
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>SDG 13 (Climate Action), Life on Land (SDG 15): sustainably manage forests, halt and reverse land degradation and halt biodiversity loss.</t>
+          <t>SDG 13, SDG 15</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -4354,7 +4347,7 @@
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Powered by:  
+          <t>Powered by:  Bappenas
 Catalyzed by: FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
@@ -4411,7 +4404,7 @@
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2, SDG 10</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -4419,7 +4412,11 @@
           <t>Text</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr"/>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Prosa AI (https://prosa.ai/)</t>
+        </is>
+      </c>
       <c r="K43" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -4764,7 +4761,7 @@
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -4774,7 +4771,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>International Center of Insect Physiology and Ecology (ICIPE)</t>
+          <t>International Center of Insect Physiology and Ecology ICIPE (dg@icipe.org)</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -4796,7 +4793,7 @@
       <c r="O47" t="inlineStr"/>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Powered by:  [ADD!!!]
+          <t>Powered by:  International Center of Insect Physiology and Ecology (ICIPE)
 Catalyzed by: Lacuna-Fund / Meridian (Climate-call) &amp;  FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
@@ -5311,7 +5308,7 @@
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP),  SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2, SDG 10</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -5339,7 +5336,7 @@
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Powered by: 
+          <t>Powered by: Digital Green, Viamo and Partners, Tech for Her, DynAg, Digifarm, Opportunity International
 Catalyzed by: FAIR Forward - AI for All
 Financed by: Gates Foundation</t>
         </is>
@@ -5395,7 +5392,7 @@
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2, SDG 10</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
@@ -5514,7 +5511,7 @@
       <c r="O55" t="inlineStr"/>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Powered by:  
+          <t>Powered by:  Association Maidi
 Catalyzed by: Lacuna-Fund / Meridian &amp; FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
@@ -5570,7 +5567,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP)</t>
+          <t>SDG 10</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -5679,7 +5676,7 @@
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr">
         <is>
-          <t>SDG 13 (Climate Action), SDG 7</t>
+          <t>SDG 13, SDG 7</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -5689,7 +5686,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Lahore University of Management Sciences (LUMS)</t>
+          <t>Lahore University of Management Sciences LUMS (naveedarshad@gmail.com)</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -6055,7 +6052,7 @@
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2, SDG 10</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -6063,7 +6060,11 @@
           <t>Voice</t>
         </is>
       </c>
-      <c r="J62" t="inlineStr"/>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>Digital Umuganda (https://digitalumuganda.com/#contact)</t>
+        </is>
+      </c>
       <c r="K62" t="inlineStr">
         <is>
           <t>Rwanda</t>
@@ -6145,7 +6146,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Climate Action, SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
@@ -6155,8 +6156,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Benson Kenduiyvo
-b.kenduiywo@cgiar.org</t>
+          <t>Benson Kenduiyvo (b.kenduiywo@cgiar.org)</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -6300,7 +6300,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t xml:space="preserve">FAIR Forward Rwanda / Digital Umuganda </t>
+          <t>Digital Umuganda (https://digitalumuganda.com/#contact), FAIR Forward Rwanda</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -6330,7 +6330,9 @@
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Atingi, Digital Umuganda, Clear Global</t>
+          <t>Powered by: Atingi, Digital Umuganda, Clear Global
+Catalyzed by: FAIR Forward - AI for All
+Financed by: BMZ</t>
         </is>
       </c>
       <c r="Q65" t="inlineStr">
@@ -6394,7 +6396,7 @@
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture), SDG 13 (Climate Action), SDG 11</t>
+          <t>SDG 2, SDG 13, SDG 11</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -6507,7 +6509,7 @@
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture), SDG 11</t>
+          <t>SDG 2, SDG 11</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
@@ -6608,7 +6610,7 @@
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
@@ -6709,7 +6711,7 @@
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture), SDG 11</t>
+          <t>SDG 2, SDG 11</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
@@ -6810,7 +6812,7 @@
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture), SDG 11</t>
+          <t>SDG 2, SDG 11</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -6911,7 +6913,7 @@
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture), SDG 11, SDG 12</t>
+          <t>SDG 2, SDG 11, SDG 12</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
@@ -7012,7 +7014,7 @@
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture), SDG 11, SDG 13 (Climate Action)</t>
+          <t>SDG 2, SDG 11, SDG 13</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
@@ -7113,7 +7115,7 @@
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture), SDG 11, SDG 13 (Climate Action)</t>
+          <t>SDG 2, SDG 11, SDG 13</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
@@ -7214,7 +7216,7 @@
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture), SDG 11, SDG 13 (Climate Action)</t>
+          <t>SDG 2, SDG 11, SDG 13</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
@@ -7315,7 +7317,7 @@
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture), SDG 13 (Climate Action)</t>
+          <t>SDG 2, SDG 13</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
@@ -7417,7 +7419,7 @@
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -7518,7 +7520,7 @@
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr">
         <is>
-          <t>SDG 10 (Reduced inequality through access to info in local languages/NLP), SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2, SDG 10</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
@@ -7614,7 +7616,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>SDG 13 (Climate Action), SDG 2 (End hunger, achieve food security, sustainable agriculture)</t>
+          <t>SDG 2, SDG 13</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
@@ -7805,7 +7807,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>SDG 2 (End hunger, achieve food security, sustainable agriculture), SDG 13 (Climate Action)</t>
+          <t>SDG 2, SDG 13</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
@@ -7854,7 +7856,7 @@
       <c r="O80" t="inlineStr"/>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Powered by:  
+          <t>Powered by:  Croppie
 Catalyzed by: FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
@@ -7928,8 +7930,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Sunbird.ai
-Ernest Mwebaze &lt;emwebaze@sunbird.ai&gt;</t>
+          <t>Sunbird.ai (emwebaze@sunbird.ai)</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -7959,7 +7960,7 @@
       <c r="O81" t="inlineStr"/>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Powered by:  
+          <t>Powered by:  Sunbird.ai
 Catalyzed by: FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
@@ -8230,7 +8231,7 @@
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
         <is>
-          <t>SDG 13 (Climate Action), SDG 10 (Reduced inequality through access to info in local languages/NLP), Achieve Gender Equality (SDG 5)</t>
+          <t>SDG 13, SDG 5, SDG 10</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">

</xml_diff>

<commit_message>
refactored to react and vite
</commit_message>
<xml_diff>
--- a/docs/data_catalog.xlsx
+++ b/docs/data_catalog.xlsx
@@ -4663,28 +4663,36 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Blue economy for climate mitigation and climate - leveraging AI, community-based approaches and local IoT-measurements</t>
+          <t>Blue economy for climate mitigation and climate - leveraging AI, community-based approaches and local IoT-measurements in Indonesia</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Blue economy for climate mitigation and climate - leveraging AI, community-based approaches and local IoT-measurements</t>
+          <t>Blue economy for climate mitigation and climate - leveraging AI, community-based approaches and local IoT-measurements in Indonesia</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Follow up of HCSA with focus on blue carbon and training of marginalized communities, as well as policy dialogue on climate</t>
+          <t xml:space="preserve">This dataset helps researcher observe daily weather changes, analyze local climate patterns, and support research, planning, or environmental modeling through machine learning and data science in Balai Silvofishery Maros Regency, South Sulawes. Weather Data is a collection of environmental condition records gathered from a monitoring point located in Balai Silvofishery Maros Regency. The dataset includes key weather parameters such as temperature, humidity, rainfall, light intensity, wind speed, and other atmospheric indicators. </t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>ruth.schmidt@giz.de Hi Ruth, will this still deliver dataset/use-case? Or remove?</t>
+          <t>GitHub - insaninfonesia/WeatherData: Weather Data Set from Colabs Project</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Meterological</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Common Room Networks Foundation https://commonroom.info/   </t>
+        </is>
+      </c>
       <c r="K41" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -4696,7 +4704,7 @@
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Powered by:  
+          <t>Powered by: Common Room Networks Foundation https://commonroom.info/   
 Catalyzed by: FAIR Forward - AI for All
 Financed by: BMZ</t>
         </is>
@@ -4710,7 +4718,7 @@
       </c>
       <c r="T41" t="inlineStr">
         <is>
-          <t>Computer Vision</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="U41" t="inlineStr"/>
@@ -9437,15 +9445,43 @@
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr"/>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>CarbonLens (High Carbon Stock Approach)</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>CarbonLens</t>
+        </is>
+      </c>
       <c r="E88" t="inlineStr"/>
-      <c r="F88" t="inlineStr"/>
-      <c r="G88" t="inlineStr"/>
-      <c r="H88" t="inlineStr"/>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>tbd</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>tbd</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>SDG 13</t>
+        </is>
+      </c>
       <c r="I88" t="inlineStr"/>
-      <c r="J88" t="inlineStr"/>
-      <c r="K88" t="inlineStr"/>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>data354 (gabriel.fonlladosa@data354.co)</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Senegal </t>
+        </is>
+      </c>
       <c r="L88" t="inlineStr"/>
       <c r="M88" t="inlineStr"/>
       <c r="N88" t="inlineStr"/>

</xml_diff>